<commit_message>
worked on fastapi backend - the backend is running
</commit_message>
<xml_diff>
--- a/data/blumen_data.xlsx
+++ b/data/blumen_data.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danja\python_projects\blumn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danja\python_projects\blumn\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC5FF59-128F-47B2-A2B9-7C023E73AE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9E7E92-EEC7-4A87-BF96-2DC5F4ED3588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="23">
   <si>
     <t>Calathea</t>
   </si>
@@ -80,6 +91,21 @@
   <si>
     <t>date</t>
   </si>
+  <si>
+    <t>hat angefangen blätter zu gelben und blätter haben angefangen sich zu krümmen</t>
+  </si>
+  <si>
+    <t>es hat sich links ein neuer ast angefangen zu bilden</t>
+  </si>
+  <si>
+    <t>compo 1pw</t>
+  </si>
+  <si>
+    <t>0,5 compo 1pw</t>
+  </si>
+  <si>
+    <t>days without fertilizer</t>
+  </si>
 </sst>
 </file>
 
@@ -110,7 +136,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,6 +146,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,18 +180,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -428,78 +481,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS108"/>
+  <dimension ref="A1:AT163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="3" width="40.140625" customWidth="1"/>
-    <col min="4" max="10" width="42" customWidth="1"/>
-    <col min="11" max="11" width="27" customWidth="1"/>
-    <col min="12" max="12" width="42" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" customWidth="1"/>
-    <col min="15" max="15" width="22.28515625" customWidth="1"/>
-    <col min="16" max="16" width="27.5703125" customWidth="1"/>
-    <col min="17" max="18" width="37.5703125" customWidth="1"/>
-    <col min="19" max="19" width="38.85546875" customWidth="1"/>
-    <col min="20" max="20" width="37" customWidth="1"/>
-    <col min="21" max="21" width="31.5703125" customWidth="1"/>
-    <col min="22" max="22" width="27.85546875" customWidth="1"/>
-    <col min="23" max="23" width="26.42578125" customWidth="1"/>
-    <col min="24" max="24" width="29" customWidth="1"/>
-    <col min="25" max="27" width="37.28515625" customWidth="1"/>
-    <col min="28" max="28" width="36.42578125" customWidth="1"/>
-    <col min="29" max="29" width="28.5703125" customWidth="1"/>
-    <col min="30" max="31" width="30.140625" customWidth="1"/>
-    <col min="32" max="32" width="30.28515625" customWidth="1"/>
-    <col min="33" max="33" width="31" customWidth="1"/>
-    <col min="34" max="34" width="39.140625" customWidth="1"/>
-    <col min="35" max="35" width="41.7109375" customWidth="1"/>
-    <col min="36" max="36" width="39.5703125" customWidth="1"/>
-    <col min="37" max="37" width="29.42578125" customWidth="1"/>
-    <col min="38" max="38" width="30.28515625" customWidth="1"/>
-    <col min="39" max="39" width="25.85546875" customWidth="1"/>
-    <col min="40" max="40" width="30" customWidth="1"/>
-    <col min="41" max="41" width="37.7109375" customWidth="1"/>
-    <col min="42" max="42" width="36" customWidth="1"/>
-    <col min="43" max="43" width="37.7109375" customWidth="1"/>
-    <col min="44" max="44" width="37.28515625" customWidth="1"/>
-    <col min="45" max="45" width="38.5703125" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" customWidth="1"/>
+    <col min="5" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="74.28515625" customWidth="1"/>
+    <col min="10" max="11" width="42" customWidth="1"/>
+    <col min="12" max="12" width="27" customWidth="1"/>
+    <col min="13" max="13" width="42" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="26.7109375" customWidth="1"/>
+    <col min="16" max="16" width="22.28515625" customWidth="1"/>
+    <col min="17" max="17" width="27.5703125" customWidth="1"/>
+    <col min="18" max="19" width="37.5703125" customWidth="1"/>
+    <col min="20" max="20" width="38.85546875" customWidth="1"/>
+    <col min="21" max="21" width="37" customWidth="1"/>
+    <col min="22" max="22" width="31.5703125" customWidth="1"/>
+    <col min="23" max="23" width="27.85546875" customWidth="1"/>
+    <col min="24" max="24" width="26.42578125" customWidth="1"/>
+    <col min="25" max="25" width="29" customWidth="1"/>
+    <col min="26" max="28" width="37.28515625" customWidth="1"/>
+    <col min="29" max="29" width="36.42578125" customWidth="1"/>
+    <col min="30" max="30" width="28.5703125" customWidth="1"/>
+    <col min="31" max="32" width="30.140625" customWidth="1"/>
+    <col min="33" max="33" width="30.28515625" customWidth="1"/>
+    <col min="34" max="34" width="31" customWidth="1"/>
+    <col min="35" max="35" width="39.140625" customWidth="1"/>
+    <col min="36" max="36" width="41.7109375" customWidth="1"/>
+    <col min="37" max="37" width="39.5703125" customWidth="1"/>
+    <col min="38" max="38" width="29.42578125" customWidth="1"/>
+    <col min="39" max="39" width="30.28515625" customWidth="1"/>
+    <col min="40" max="40" width="25.85546875" customWidth="1"/>
+    <col min="41" max="41" width="30" customWidth="1"/>
+    <col min="42" max="42" width="37.7109375" customWidth="1"/>
+    <col min="43" max="43" width="36" customWidth="1"/>
+    <col min="44" max="44" width="37.7109375" customWidth="1"/>
+    <col min="45" max="45" width="37.28515625" customWidth="1"/>
+    <col min="46" max="46" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:46" s="6" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45774</v>
       </c>
@@ -516,21 +578,22 @@
       <c r="J2"/>
       <c r="K2"/>
       <c r="L2"/>
-      <c r="Q2"/>
-      <c r="S2"/>
+      <c r="M2"/>
+      <c r="R2"/>
       <c r="T2"/>
       <c r="U2"/>
-      <c r="Y2"/>
-      <c r="AC2"/>
-      <c r="AH2"/>
+      <c r="V2"/>
+      <c r="Z2"/>
+      <c r="AD2"/>
       <c r="AI2"/>
       <c r="AJ2"/>
       <c r="AK2"/>
-      <c r="AO2"/>
-      <c r="AR2"/>
+      <c r="AL2"/>
+      <c r="AP2"/>
       <c r="AS2"/>
-    </row>
-    <row r="3" spans="1:45" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AT2"/>
+    </row>
+    <row r="3" spans="1:46" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45774</v>
       </c>
@@ -547,16 +610,19 @@
       <c r="J3"/>
       <c r="K3"/>
       <c r="L3"/>
-      <c r="AA3" s="3"/>
-    </row>
-    <row r="4" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M3"/>
+      <c r="AB3" s="3"/>
+    </row>
+    <row r="4" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45774</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4"/>
+      <c r="C4">
+        <v>1</v>
+      </c>
       <c r="D4"/>
       <c r="E4"/>
       <c r="F4"/>
@@ -566,17 +632,22 @@
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
-      <c r="AA4" s="3"/>
-    </row>
-    <row r="5" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="M4"/>
+      <c r="AB4" s="3"/>
+    </row>
+    <row r="5" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>45774</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5"/>
-      <c r="D5"/>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>100</v>
+      </c>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5"/>
@@ -585,17 +656,22 @@
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5"/>
-      <c r="AA5" s="3"/>
-    </row>
-    <row r="6" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="M5"/>
+      <c r="AB5" s="3"/>
+    </row>
+    <row r="6" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>45774</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6"/>
-      <c r="D6"/>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>100</v>
+      </c>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
@@ -604,17 +680,22 @@
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
-      <c r="AA6" s="3"/>
-    </row>
-    <row r="7" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="M6"/>
+      <c r="AB6" s="3"/>
+    </row>
+    <row r="7" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>45774</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7"/>
-      <c r="D7"/>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>100</v>
+      </c>
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7"/>
@@ -623,9 +704,10 @@
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
-      <c r="AA7" s="3"/>
-    </row>
-    <row r="8" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M7"/>
+      <c r="AB7" s="3"/>
+    </row>
+    <row r="8" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45774</v>
       </c>
@@ -642,17 +724,22 @@
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
-      <c r="AA8" s="3"/>
-    </row>
-    <row r="9" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="M8"/>
+      <c r="AB8" s="3"/>
+    </row>
+    <row r="9" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>45774</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9"/>
-      <c r="D9"/>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>100</v>
+      </c>
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
@@ -661,24 +748,26 @@
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9"/>
-      <c r="AA9" s="3"/>
-    </row>
-    <row r="10" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="AA10" s="3"/>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="M9"/>
+      <c r="AB9" s="3"/>
+    </row>
+    <row r="10" spans="1:46" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="AB10" s="11"/>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45775</v>
       </c>
@@ -686,51 +775,65 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>45775</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6">
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45775</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45775</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45775</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45775</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45775</v>
       </c>
@@ -738,80 +841,105 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45775</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>45776</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6">
+      <c r="B20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="13">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
         <v>150</v>
       </c>
       <c r="E20" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>45776</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6">
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
         <v>50</v>
       </c>
       <c r="E21" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45776</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45776</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45776</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45776</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45776</v>
       </c>
@@ -819,637 +947,1612 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45776</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>45777</v>
       </c>
       <c r="B29" t="s">
         <v>2</v>
       </c>
-      <c r="C29"/>
-    </row>
-    <row r="30" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>45777</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
       </c>
-      <c r="C30"/>
-    </row>
-    <row r="31" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
         <v>45777</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6">
+      <c r="B31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4">
         <v>200</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="G31" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>45777</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
       </c>
-      <c r="C32"/>
-    </row>
-    <row r="33" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="C32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>45777</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
       </c>
-      <c r="C33"/>
-      <c r="F33" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>45777</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
       </c>
-      <c r="C34"/>
-    </row>
-    <row r="35" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="C34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>45777</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
         <v>45777</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
-      <c r="C36"/>
-    </row>
-    <row r="37" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>45778</v>
       </c>
       <c r="B38" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>45778</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>45778</v>
       </c>
       <c r="B40" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>45778</v>
       </c>
       <c r="B41" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>45778</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>45778</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="7">
+      <c r="C43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
         <v>45778</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6">
+      <c r="C44" s="4">
+        <v>0</v>
+      </c>
+      <c r="D44" s="4">
         <v>100</v>
       </c>
-      <c r="F44" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>45778</v>
       </c>
       <c r="B45" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>45779</v>
       </c>
       <c r="B47" t="s">
         <v>2</v>
       </c>
-      <c r="F47" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45779</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
-      <c r="F48" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>45779</v>
       </c>
       <c r="B49" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>45779</v>
       </c>
       <c r="B50" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>45779</v>
       </c>
       <c r="B51" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>45779</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
       </c>
-      <c r="F52" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>5</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>45779</v>
       </c>
       <c r="B53" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>45779</v>
       </c>
       <c r="B54" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>45780</v>
       </c>
       <c r="B56" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="F56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>45780</v>
       </c>
       <c r="B57" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>5</v>
+      </c>
+      <c r="F57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>45780</v>
       </c>
       <c r="B58" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>45780</v>
       </c>
       <c r="B59" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>45780</v>
       </c>
       <c r="B60" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>45780</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>45780</v>
       </c>
       <c r="B62" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>45780</v>
       </c>
       <c r="B63" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="8"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>45781</v>
       </c>
       <c r="B65" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="F65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
         <v>45781</v>
       </c>
-      <c r="B66" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
+      <c r="B66" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="13">
+        <v>0</v>
+      </c>
+      <c r="D66" s="4">
+        <v>350</v>
+      </c>
+      <c r="E66" t="s">
+        <v>20</v>
+      </c>
+      <c r="F66" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
         <v>45781</v>
       </c>
-      <c r="B67" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="13">
+        <v>0</v>
+      </c>
+      <c r="D67" s="4">
+        <v>400</v>
+      </c>
+      <c r="E67" t="s">
+        <v>20</v>
+      </c>
+      <c r="F67" s="4">
+        <v>0</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>45781</v>
       </c>
       <c r="B68" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
+      <c r="C68" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="5">
         <v>45781</v>
       </c>
-      <c r="B69" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="13">
+        <v>0</v>
+      </c>
+      <c r="D69" s="4">
+        <v>150</v>
+      </c>
+      <c r="E69" t="s">
+        <v>20</v>
+      </c>
+      <c r="F69" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>45781</v>
       </c>
       <c r="B70" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>45781</v>
       </c>
       <c r="B71" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>45781</v>
       </c>
       <c r="B72" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="2"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="8"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>45782</v>
       </c>
       <c r="B74" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <v>6</v>
+      </c>
+      <c r="F74">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>45782</v>
       </c>
       <c r="B75" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>45782</v>
       </c>
       <c r="B76" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>1</v>
+      </c>
+      <c r="I76" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>45782</v>
       </c>
       <c r="B77" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>45782</v>
       </c>
       <c r="B78" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="5">
         <v>45782</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79" s="4">
+        <v>0</v>
+      </c>
+      <c r="D79" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>45782</v>
       </c>
       <c r="B80" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
+      <c r="C80">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="5">
         <v>45782</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81" s="4">
+        <v>0</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>45783</v>
       </c>
       <c r="B83" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83" s="7">
+        <f>C74+1</f>
+        <v>7</v>
+      </c>
+      <c r="F83">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>45783</v>
       </c>
       <c r="B84" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <f>C75+1</f>
+        <v>2</v>
+      </c>
+      <c r="F84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>45783</v>
       </c>
       <c r="B85" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <f t="shared" ref="C85:C88" si="0">C76+1</f>
+        <v>2</v>
+      </c>
+      <c r="F85">
+        <v>2</v>
+      </c>
+      <c r="I85" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>45783</v>
       </c>
       <c r="B86" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86" s="13">
+        <v>0</v>
+      </c>
+      <c r="E86" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>45783</v>
       </c>
       <c r="B87" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I87" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>45783</v>
       </c>
       <c r="B88" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>45783</v>
       </c>
       <c r="B89" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C89" s="13">
+        <v>0</v>
+      </c>
+      <c r="E89" t="s">
+        <v>20</v>
+      </c>
+      <c r="F89" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>45783</v>
       </c>
       <c r="B90" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C90" s="13">
+        <v>0</v>
+      </c>
+      <c r="E90" t="s">
+        <v>20</v>
+      </c>
+      <c r="F90" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>45784</v>
       </c>
       <c r="B92" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C92" s="7">
+        <f>C83+1</f>
+        <v>8</v>
+      </c>
+      <c r="F92">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>45784</v>
       </c>
       <c r="B93" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <f t="shared" ref="C93:C99" si="1">C84+1</f>
+        <v>3</v>
+      </c>
+      <c r="F93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>45784</v>
       </c>
       <c r="B94" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>45784</v>
       </c>
       <c r="B95" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>45784</v>
       </c>
       <c r="B96" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C96">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F96">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>45784</v>
       </c>
       <c r="B97" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C97">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>45784</v>
       </c>
       <c r="B98" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>45784</v>
       </c>
       <c r="B99" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C99">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>45785</v>
       </c>
       <c r="B101" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C101" s="13">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>200</v>
+      </c>
+      <c r="E101" t="s">
+        <v>20</v>
+      </c>
+      <c r="F101" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>45785</v>
       </c>
       <c r="B102" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <f t="shared" ref="C102:C108" si="2">C93+1</f>
+        <v>4</v>
+      </c>
+      <c r="F102">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>45785</v>
       </c>
       <c r="B103" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C103" s="13">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>500</v>
+      </c>
+      <c r="E103" t="s">
+        <v>21</v>
+      </c>
+      <c r="F103" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>45785</v>
       </c>
       <c r="B104" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C104">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>45785</v>
       </c>
       <c r="B105" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C105" s="13">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>200</v>
+      </c>
+      <c r="E105" t="s">
+        <v>20</v>
+      </c>
+      <c r="F105" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>45785</v>
       </c>
       <c r="B106" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C106">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>45785</v>
       </c>
       <c r="B107" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C107">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>45785</v>
       </c>
       <c r="B108" t="s">
         <v>9</v>
       </c>
-    </row>
+      <c r="C108">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>45786</v>
+      </c>
+      <c r="B110" t="s">
+        <v>2</v>
+      </c>
+      <c r="C110">
+        <f>C101+1</f>
+        <v>1</v>
+      </c>
+      <c r="F110">
+        <f>F101+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>45786</v>
+      </c>
+      <c r="B111" t="s">
+        <v>3</v>
+      </c>
+      <c r="C111">
+        <f t="shared" ref="C111:C117" si="3">C102+1</f>
+        <v>5</v>
+      </c>
+      <c r="F111">
+        <f t="shared" ref="F111:F117" si="4">F102+1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>45786</v>
+      </c>
+      <c r="B112" t="s">
+        <v>4</v>
+      </c>
+      <c r="C112">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <v>45786</v>
+      </c>
+      <c r="B113" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <v>45786</v>
+      </c>
+      <c r="B114" t="s">
+        <v>6</v>
+      </c>
+      <c r="C114">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <v>45786</v>
+      </c>
+      <c r="B115" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <v>45786</v>
+      </c>
+      <c r="B116" t="s">
+        <v>8</v>
+      </c>
+      <c r="C116">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>45786</v>
+      </c>
+      <c r="B117" t="s">
+        <v>9</v>
+      </c>
+      <c r="C117">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>45787</v>
+      </c>
+      <c r="B119" t="s">
+        <v>2</v>
+      </c>
+      <c r="C119">
+        <f>C110+1</f>
+        <v>2</v>
+      </c>
+      <c r="F119">
+        <f>F110+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>45787</v>
+      </c>
+      <c r="B120" t="s">
+        <v>3</v>
+      </c>
+      <c r="C120">
+        <f t="shared" ref="C120:C126" si="5">C111+1</f>
+        <v>6</v>
+      </c>
+      <c r="F120">
+        <f t="shared" ref="F120:F126" si="6">F111+1</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <v>45787</v>
+      </c>
+      <c r="B121" t="s">
+        <v>4</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>45787</v>
+      </c>
+      <c r="B122" t="s">
+        <v>5</v>
+      </c>
+      <c r="C122">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>45787</v>
+      </c>
+      <c r="B123" t="s">
+        <v>6</v>
+      </c>
+      <c r="C123">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>45787</v>
+      </c>
+      <c r="B124" t="s">
+        <v>7</v>
+      </c>
+      <c r="C124">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>45787</v>
+      </c>
+      <c r="B125" t="s">
+        <v>8</v>
+      </c>
+      <c r="C125">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>45787</v>
+      </c>
+      <c r="B126" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
+        <v>45788</v>
+      </c>
+      <c r="B128" t="s">
+        <v>2</v>
+      </c>
+      <c r="C128">
+        <f>C119+1</f>
+        <v>3</v>
+      </c>
+      <c r="F128">
+        <f>F119+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
+        <v>45788</v>
+      </c>
+      <c r="B129" t="s">
+        <v>3</v>
+      </c>
+      <c r="C129">
+        <f t="shared" ref="C129:C135" si="7">C120+1</f>
+        <v>7</v>
+      </c>
+      <c r="F129">
+        <f t="shared" ref="F129:F135" si="8">F120+1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
+        <v>45788</v>
+      </c>
+      <c r="B130" t="s">
+        <v>4</v>
+      </c>
+      <c r="C130">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
+        <v>45788</v>
+      </c>
+      <c r="B131" t="s">
+        <v>5</v>
+      </c>
+      <c r="C131">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="F131">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
+        <v>45788</v>
+      </c>
+      <c r="B132" t="s">
+        <v>6</v>
+      </c>
+      <c r="C132">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="F132">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
+        <v>45788</v>
+      </c>
+      <c r="B133" t="s">
+        <v>7</v>
+      </c>
+      <c r="C133">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="F133">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <v>45788</v>
+      </c>
+      <c r="B134" t="s">
+        <v>8</v>
+      </c>
+      <c r="C134" s="4">
+        <v>0</v>
+      </c>
+      <c r="D134">
+        <v>200</v>
+      </c>
+      <c r="F134">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
+        <v>45788</v>
+      </c>
+      <c r="B135" t="s">
+        <v>9</v>
+      </c>
+      <c r="C135" s="4">
+        <v>0</v>
+      </c>
+      <c r="D135">
+        <v>200</v>
+      </c>
+      <c r="F135">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
+        <v>45789</v>
+      </c>
+      <c r="B137" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
+        <v>45789</v>
+      </c>
+      <c r="B138" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
+        <v>45789</v>
+      </c>
+      <c r="B139" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
+        <v>45789</v>
+      </c>
+      <c r="B140" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
+        <v>45789</v>
+      </c>
+      <c r="B141" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
+        <v>45789</v>
+      </c>
+      <c r="B142" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
+        <v>45789</v>
+      </c>
+      <c r="B143" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
+        <v>45789</v>
+      </c>
+      <c r="B144" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
+        <v>45790</v>
+      </c>
+      <c r="B146" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
+        <v>45790</v>
+      </c>
+      <c r="B147" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
+        <v>45790</v>
+      </c>
+      <c r="B148" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
+        <v>45790</v>
+      </c>
+      <c r="B149" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
+        <v>45790</v>
+      </c>
+      <c r="B150" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <v>45790</v>
+      </c>
+      <c r="B151" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <v>45790</v>
+      </c>
+      <c r="B152" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
+        <v>45790</v>
+      </c>
+      <c r="B153" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="2"/>
+      <c r="B155" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="2"/>
+      <c r="B156" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="2"/>
+      <c r="B157" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="2"/>
+      <c r="B158" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="2"/>
+      <c r="B159" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="2"/>
+      <c r="B160" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="2"/>
+      <c r="B161" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="2"/>
+      <c r="B162" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
the algo for adding new entries seems to work but it should be tested what happens when the dates are far behind
</commit_message>
<xml_diff>
--- a/data/blumen_data.xlsx
+++ b/data/blumen_data.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="38280" yWindow="1815" windowWidth="16440" windowHeight="28320" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -450,11 +450,11 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB233"/>
+  <dimension ref="A1:AB226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H157" sqref="H157"/>
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E158" sqref="E158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2893,781 +2893,686 @@
         <v>8</v>
       </c>
     </row>
-    <row r="163" customFormat="1" s="9">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>14.05.2025</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>Calathea Medalion</t>
-        </is>
-      </c>
-    </row>
+    <row r="163"/>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>14.05.2025</t>
+          <t>15.05.2025</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Calathea Orbifolia</t>
+          <t>Calathea Medalion</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>14.05.2025</t>
+          <t>15.05.2025</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Epiprenum Aureum</t>
+          <t>Calathea Orbifolia</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>14.05.2025</t>
+          <t>15.05.2025</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t xml:space="preserve">Philodendron Scandens Micans </t>
+          <t>Epiprenum Aureum</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>14.05.2025</t>
+          <t>15.05.2025</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Scindapsus Treubii Moonlight</t>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>14.05.2025</t>
+          <t>15.05.2025</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Philodendron Hedaracium Brasil</t>
+          <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>14.05.2025</t>
+          <t>15.05.2025</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Coffea Arabica</t>
+          <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>14.05.2025</t>
+          <t>15.05.2025</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
+          <t>Coffea Arabica</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>15.05.2025</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
           <t>Monstera Adenossii</t>
         </is>
       </c>
     </row>
-    <row r="171"/>
-    <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>15.05.2025</t>
-        </is>
-      </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>Calathea Medalion</t>
-        </is>
-      </c>
-    </row>
+    <row r="172"/>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>15.05.2025</t>
+          <t>16.05.2025</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Calathea Orbifolia</t>
+          <t>Calathea Medalion</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>15.05.2025</t>
+          <t>16.05.2025</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Epiprenum Aureum</t>
+          <t>Calathea Orbifolia</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>15.05.2025</t>
+          <t>16.05.2025</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t xml:space="preserve">Philodendron Scandens Micans </t>
+          <t>Epiprenum Aureum</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>15.05.2025</t>
+          <t>16.05.2025</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Scindapsus Treubii Moonlight</t>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>15.05.2025</t>
+          <t>16.05.2025</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Philodendron Hedaracium Brasil</t>
+          <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>15.05.2025</t>
+          <t>16.05.2025</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Coffea Arabica</t>
+          <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>15.05.2025</t>
+          <t>16.05.2025</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
+          <t>Coffea Arabica</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>16.05.2025</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
           <t>Monstera Adenossii</t>
         </is>
       </c>
     </row>
-    <row r="180"/>
-    <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>16.05.2025</t>
-        </is>
-      </c>
-      <c r="B181" t="inlineStr">
-        <is>
-          <t>Calathea Medalion</t>
-        </is>
-      </c>
-    </row>
+    <row r="181"/>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>16.05.2025</t>
+          <t>17.05.2025</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Calathea Orbifolia</t>
+          <t>Calathea Medalion</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>16.05.2025</t>
+          <t>17.05.2025</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Epiprenum Aureum</t>
+          <t>Calathea Orbifolia</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>16.05.2025</t>
+          <t>17.05.2025</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t xml:space="preserve">Philodendron Scandens Micans </t>
+          <t>Epiprenum Aureum</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>16.05.2025</t>
+          <t>17.05.2025</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Scindapsus Treubii Moonlight</t>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>16.05.2025</t>
+          <t>17.05.2025</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Philodendron Hedaracium Brasil</t>
+          <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>16.05.2025</t>
+          <t>17.05.2025</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Coffea Arabica</t>
+          <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>16.05.2025</t>
+          <t>17.05.2025</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
+          <t>Coffea Arabica</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>17.05.2025</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
           <t>Monstera Adenossii</t>
         </is>
       </c>
     </row>
-    <row r="189"/>
-    <row r="190">
-      <c r="A190" t="inlineStr">
-        <is>
-          <t>17.05.2025</t>
-        </is>
-      </c>
-      <c r="B190" t="inlineStr">
-        <is>
-          <t>Calathea Medalion</t>
-        </is>
-      </c>
-    </row>
+    <row r="190"/>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>17.05.2025</t>
+          <t>18.05.2025</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Calathea Orbifolia</t>
+          <t>Calathea Medalion</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>17.05.2025</t>
+          <t>18.05.2025</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Epiprenum Aureum</t>
+          <t>Calathea Orbifolia</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>17.05.2025</t>
+          <t>18.05.2025</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t xml:space="preserve">Philodendron Scandens Micans </t>
+          <t>Epiprenum Aureum</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>17.05.2025</t>
+          <t>18.05.2025</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Scindapsus Treubii Moonlight</t>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>17.05.2025</t>
+          <t>18.05.2025</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Philodendron Hedaracium Brasil</t>
+          <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>17.05.2025</t>
+          <t>18.05.2025</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Coffea Arabica</t>
+          <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>17.05.2025</t>
+          <t>18.05.2025</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
+          <t>Coffea Arabica</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>18.05.2025</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
           <t>Monstera Adenossii</t>
         </is>
       </c>
     </row>
-    <row r="198"/>
-    <row r="199">
-      <c r="A199" t="inlineStr">
-        <is>
-          <t>18.05.2025</t>
-        </is>
-      </c>
-      <c r="B199" t="inlineStr">
-        <is>
-          <t>Calathea Medalion</t>
-        </is>
-      </c>
-    </row>
+    <row r="199"/>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>18.05.2025</t>
+          <t>19.05.2025</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Calathea Orbifolia</t>
+          <t>Calathea Medalion</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>18.05.2025</t>
+          <t>19.05.2025</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Epiprenum Aureum</t>
+          <t>Calathea Orbifolia</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>18.05.2025</t>
+          <t>19.05.2025</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t xml:space="preserve">Philodendron Scandens Micans </t>
+          <t>Epiprenum Aureum</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>18.05.2025</t>
+          <t>19.05.2025</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Scindapsus Treubii Moonlight</t>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>18.05.2025</t>
+          <t>19.05.2025</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Philodendron Hedaracium Brasil</t>
+          <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>18.05.2025</t>
+          <t>19.05.2025</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Coffea Arabica</t>
+          <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>18.05.2025</t>
+          <t>19.05.2025</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
+          <t>Coffea Arabica</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>19.05.2025</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
           <t>Monstera Adenossii</t>
         </is>
       </c>
     </row>
-    <row r="207"/>
-    <row r="208">
-      <c r="A208" t="inlineStr">
-        <is>
-          <t>19.05.2025</t>
-        </is>
-      </c>
-      <c r="B208" t="inlineStr">
-        <is>
-          <t>Calathea Medalion</t>
-        </is>
-      </c>
-    </row>
+    <row r="208"/>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>19.05.2025</t>
+          <t>20.05.2025</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Calathea Orbifolia</t>
+          <t>Calathea Medalion</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>19.05.2025</t>
+          <t>20.05.2025</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Epiprenum Aureum</t>
+          <t>Calathea Orbifolia</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>19.05.2025</t>
+          <t>20.05.2025</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t xml:space="preserve">Philodendron Scandens Micans </t>
+          <t>Epiprenum Aureum</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>19.05.2025</t>
+          <t>20.05.2025</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Scindapsus Treubii Moonlight</t>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>19.05.2025</t>
+          <t>20.05.2025</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Philodendron Hedaracium Brasil</t>
+          <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>19.05.2025</t>
+          <t>20.05.2025</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Coffea Arabica</t>
+          <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>19.05.2025</t>
+          <t>20.05.2025</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
+          <t>Coffea Arabica</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>20.05.2025</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
           <t>Monstera Adenossii</t>
         </is>
       </c>
     </row>
-    <row r="216"/>
-    <row r="217">
-      <c r="A217" t="inlineStr">
-        <is>
-          <t>20.05.2025</t>
-        </is>
-      </c>
-      <c r="B217" t="inlineStr">
-        <is>
-          <t>Calathea Medalion</t>
-        </is>
-      </c>
-    </row>
+    <row r="217"/>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>20.05.2025</t>
+          <t>21.05.2025</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Calathea Orbifolia</t>
+          <t>Calathea Medalion</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>20.05.2025</t>
+          <t>21.05.2025</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Epiprenum Aureum</t>
+          <t>Calathea Orbifolia</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>20.05.2025</t>
+          <t>21.05.2025</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t xml:space="preserve">Philodendron Scandens Micans </t>
+          <t>Epiprenum Aureum</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>20.05.2025</t>
+          <t>21.05.2025</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Scindapsus Treubii Moonlight</t>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>20.05.2025</t>
+          <t>21.05.2025</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Philodendron Hedaracium Brasil</t>
+          <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>20.05.2025</t>
+          <t>21.05.2025</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Coffea Arabica</t>
+          <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>20.05.2025</t>
+          <t>21.05.2025</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
+          <t>Coffea Arabica</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>21.05.2025</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
           <t>Monstera Adenossii</t>
         </is>
       </c>
     </row>
-    <row r="225"/>
-    <row r="226">
-      <c r="A226" t="inlineStr">
-        <is>
-          <t>21.05.2025</t>
-        </is>
-      </c>
-      <c r="B226" t="inlineStr">
-        <is>
-          <t>Calathea Medalion</t>
-        </is>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="inlineStr">
-        <is>
-          <t>21.05.2025</t>
-        </is>
-      </c>
-      <c r="B227" t="inlineStr">
-        <is>
-          <t>Calathea Orbifolia</t>
-        </is>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="inlineStr">
-        <is>
-          <t>21.05.2025</t>
-        </is>
-      </c>
-      <c r="B228" t="inlineStr">
-        <is>
-          <t>Epiprenum Aureum</t>
-        </is>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="inlineStr">
-        <is>
-          <t>21.05.2025</t>
-        </is>
-      </c>
-      <c r="B229" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Philodendron Scandens Micans </t>
-        </is>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="inlineStr">
-        <is>
-          <t>21.05.2025</t>
-        </is>
-      </c>
-      <c r="B230" t="inlineStr">
-        <is>
-          <t>Scindapsus Treubii Moonlight</t>
-        </is>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" t="inlineStr">
-        <is>
-          <t>21.05.2025</t>
-        </is>
-      </c>
-      <c r="B231" t="inlineStr">
-        <is>
-          <t>Philodendron Hedaracium Brasil</t>
-        </is>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" t="inlineStr">
-        <is>
-          <t>21.05.2025</t>
-        </is>
-      </c>
-      <c r="B232" t="inlineStr">
-        <is>
-          <t>Coffea Arabica</t>
-        </is>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" t="inlineStr">
-        <is>
-          <t>21.05.2025</t>
-        </is>
-      </c>
-      <c r="B233" t="inlineStr">
-        <is>
-          <t>Monstera Adenossii</t>
-        </is>
-      </c>
-    </row>
+    <row r="226"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added a nice overwie and plot of periodic watering
</commit_message>
<xml_diff>
--- a/data/blumen_data.xlsx
+++ b/data/blumen_data.xlsx
@@ -3,20 +3,20 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="38280" yWindow="1815" windowWidth="16440" windowHeight="28320" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -38,12 +38,6 @@
       <b val="1"/>
       <color theme="1"/>
       <sz val="14"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <sz val="8"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -98,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -120,8 +114,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -471,51 +464,51 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G192" sqref="G192"/>
+      <selection pane="bottomLeft" activeCell="B186" sqref="B186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col width="14.42578125" customWidth="1" style="15" min="1" max="1"/>
-    <col width="40.140625" customWidth="1" style="15" min="2" max="2"/>
-    <col width="16.28515625" customWidth="1" style="15" min="3" max="3"/>
-    <col width="7.85546875" customWidth="1" style="15" min="4" max="4"/>
-    <col width="15.140625" customWidth="1" style="15" min="5" max="6"/>
-    <col width="8.5703125" customWidth="1" style="15" min="7" max="7"/>
-    <col width="11.42578125" customWidth="1" style="15" min="8" max="8"/>
-    <col width="74.28515625" customWidth="1" style="15" min="9" max="9"/>
-    <col width="42" customWidth="1" style="15" min="10" max="11"/>
-    <col width="27" customWidth="1" style="15" min="12" max="12"/>
-    <col width="42" customWidth="1" style="15" min="13" max="13"/>
-    <col width="15.7109375" customWidth="1" style="15" min="14" max="14"/>
-    <col width="26.7109375" customWidth="1" style="15" min="15" max="15"/>
-    <col width="22.28515625" customWidth="1" style="15" min="16" max="16"/>
-    <col width="27.5703125" customWidth="1" style="15" min="17" max="17"/>
-    <col width="37.5703125" customWidth="1" style="15" min="18" max="19"/>
-    <col width="38.85546875" customWidth="1" style="15" min="20" max="20"/>
-    <col width="37" customWidth="1" style="15" min="21" max="21"/>
-    <col width="31.5703125" customWidth="1" style="15" min="22" max="22"/>
-    <col width="27.85546875" customWidth="1" style="15" min="23" max="23"/>
-    <col width="26.42578125" customWidth="1" style="15" min="24" max="24"/>
-    <col width="29" customWidth="1" style="15" min="25" max="25"/>
-    <col width="37.28515625" customWidth="1" style="15" min="26" max="28"/>
-    <col width="36.42578125" customWidth="1" style="15" min="29" max="29"/>
-    <col width="28.5703125" customWidth="1" style="15" min="30" max="30"/>
-    <col width="30.140625" customWidth="1" style="15" min="31" max="32"/>
-    <col width="30.28515625" customWidth="1" style="15" min="33" max="33"/>
-    <col width="31" customWidth="1" style="15" min="34" max="34"/>
-    <col width="39.140625" customWidth="1" style="15" min="35" max="35"/>
-    <col width="41.7109375" customWidth="1" style="15" min="36" max="36"/>
-    <col width="39.5703125" customWidth="1" style="15" min="37" max="37"/>
-    <col width="29.42578125" customWidth="1" style="15" min="38" max="38"/>
-    <col width="30.28515625" customWidth="1" style="15" min="39" max="39"/>
-    <col width="25.85546875" customWidth="1" style="15" min="40" max="40"/>
-    <col width="30" customWidth="1" style="15" min="41" max="41"/>
-    <col width="37.7109375" customWidth="1" style="15" min="42" max="42"/>
-    <col width="36" customWidth="1" style="15" min="43" max="43"/>
-    <col width="37.7109375" customWidth="1" style="15" min="44" max="44"/>
-    <col width="37.28515625" customWidth="1" style="15" min="45" max="45"/>
-    <col width="38.5703125" customWidth="1" style="15" min="46" max="46"/>
+    <col width="14.42578125" customWidth="1" min="1" max="1"/>
+    <col width="40.140625" customWidth="1" min="2" max="2"/>
+    <col width="16.28515625" customWidth="1" min="3" max="3"/>
+    <col width="7.85546875" customWidth="1" min="4" max="4"/>
+    <col width="15.140625" customWidth="1" min="5" max="6"/>
+    <col width="8.5703125" customWidth="1" min="7" max="7"/>
+    <col width="11.42578125" customWidth="1" min="8" max="8"/>
+    <col width="74.28515625" customWidth="1" min="9" max="9"/>
+    <col width="42" customWidth="1" min="10" max="11"/>
+    <col width="27" customWidth="1" min="12" max="12"/>
+    <col width="42" customWidth="1" min="13" max="13"/>
+    <col width="15.7109375" customWidth="1" min="14" max="14"/>
+    <col width="26.7109375" customWidth="1" min="15" max="15"/>
+    <col width="22.28515625" customWidth="1" min="16" max="16"/>
+    <col width="27.5703125" customWidth="1" min="17" max="17"/>
+    <col width="37.5703125" customWidth="1" min="18" max="19"/>
+    <col width="38.85546875" customWidth="1" min="20" max="20"/>
+    <col width="37" customWidth="1" min="21" max="21"/>
+    <col width="31.5703125" customWidth="1" min="22" max="22"/>
+    <col width="27.85546875" customWidth="1" min="23" max="23"/>
+    <col width="26.42578125" customWidth="1" min="24" max="24"/>
+    <col width="29" customWidth="1" min="25" max="25"/>
+    <col width="37.28515625" customWidth="1" min="26" max="28"/>
+    <col width="36.42578125" customWidth="1" min="29" max="29"/>
+    <col width="28.5703125" customWidth="1" min="30" max="30"/>
+    <col width="30.140625" customWidth="1" min="31" max="32"/>
+    <col width="30.28515625" customWidth="1" min="33" max="33"/>
+    <col width="31" customWidth="1" min="34" max="34"/>
+    <col width="39.140625" customWidth="1" min="35" max="35"/>
+    <col width="41.7109375" customWidth="1" min="36" max="36"/>
+    <col width="39.5703125" customWidth="1" min="37" max="37"/>
+    <col width="29.42578125" customWidth="1" min="38" max="38"/>
+    <col width="30.28515625" customWidth="1" min="39" max="39"/>
+    <col width="25.85546875" customWidth="1" min="40" max="40"/>
+    <col width="30" customWidth="1" min="41" max="41"/>
+    <col width="37.7109375" customWidth="1" min="42" max="42"/>
+    <col width="36" customWidth="1" min="43" max="43"/>
+    <col width="37.7109375" customWidth="1" min="44" max="44"/>
+    <col width="37.28515625" customWidth="1" min="45" max="45"/>
+    <col width="38.5703125" customWidth="1" min="46" max="46"/>
   </cols>
   <sheetData>
     <row r="1" ht="53.25" customFormat="1" customHeight="1" s="6">
@@ -574,7 +567,7 @@
           <t>Calathea Medalion</t>
         </is>
       </c>
-      <c r="J2" s="16" t="inlineStr">
+      <c r="J2" s="15" t="inlineStr">
         <is>
           <t>Calathea veitchiana</t>
         </is>
@@ -2996,7 +2989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" s="15">
+    <row r="169">
       <c r="A169" t="inlineStr">
         <is>
           <t>15.05.2025</t>
@@ -3029,7 +3022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" s="15">
+    <row r="171">
       <c r="A171" t="inlineStr">
         <is>
           <t>15.05.2025</t>

</xml_diff>

<commit_message>
added an api for calcualting the periodicity of watering
</commit_message>
<xml_diff>
--- a/data/blumen_data.xlsx
+++ b/data/blumen_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="38280" yWindow="1815" windowWidth="16440" windowHeight="28320" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId1"/>
@@ -463,8 +463,8 @@
   <dimension ref="A1:AB292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B186" sqref="B186"/>
+      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I178" sqref="I178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1756,6 +1756,9 @@
       <c r="C86" s="13" t="n">
         <v>0</v>
       </c>
+      <c r="D86" t="n">
+        <v>250</v>
+      </c>
       <c r="E86" t="inlineStr">
         <is>
           <t>compo 1pw</t>
@@ -1811,6 +1814,9 @@
       <c r="C89" s="13" t="n">
         <v>0</v>
       </c>
+      <c r="D89" t="n">
+        <v>200</v>
+      </c>
       <c r="E89" t="inlineStr">
         <is>
           <t>compo 1pw</t>
@@ -1831,6 +1837,9 @@
       </c>
       <c r="C90" s="13" t="n">
         <v>0</v>
+      </c>
+      <c r="D90" t="n">
+        <v>200</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2829,6 +2838,9 @@
       <c r="C157" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="D157" t="n">
+        <v>500</v>
+      </c>
       <c r="F157" t="n">
         <v>0</v>
       </c>
@@ -2861,6 +2873,9 @@
       <c r="C159" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="D159" t="n">
+        <v>150</v>
+      </c>
       <c r="F159" t="n">
         <v>0</v>
       </c>
@@ -3130,6 +3145,9 @@
       <c r="C178" s="13" t="n">
         <v>0</v>
       </c>
+      <c r="D178" t="n">
+        <v>150</v>
+      </c>
       <c r="E178" t="inlineStr">
         <is>
           <t>compo 1pw</t>
@@ -3165,6 +3183,9 @@
       <c r="C180" s="13" t="n">
         <v>0</v>
       </c>
+      <c r="D180" t="n">
+        <v>200</v>
+      </c>
       <c r="E180" t="inlineStr">
         <is>
           <t>compo 1pw</t>
@@ -3196,6 +3217,9 @@
       </c>
       <c r="C182" s="13" t="n">
         <v>0</v>
+      </c>
+      <c r="D182" t="n">
+        <v>500</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
first version of the plot created
</commit_message>
<xml_diff>
--- a/data/blumen_data.xlsx
+++ b/data/blumen_data.xlsx
@@ -463,8 +463,8 @@
   <dimension ref="A1:AB292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I178" sqref="I178"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -838,16 +838,8 @@
       <c r="C21" t="n">
         <v>1</v>
       </c>
-      <c r="D21" t="n">
-        <v>50</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Calathea</t>
-        </is>
-      </c>
       <c r="F21" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">

</xml_diff>

<commit_message>
made advanced functionality in frontend plot - indicators for watering and other indicators
</commit_message>
<xml_diff>
--- a/data/blumen_data.xlsx
+++ b/data/blumen_data.xlsx
@@ -48,7 +48,7 @@
       <sz val="24"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -76,6 +76,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.3499862666707358"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -117,8 +123,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -465,52 +471,52 @@
   <dimension ref="A1:AB307"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F77" sqref="F77"/>
+      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I184" sqref="I184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col width="14.42578125" customWidth="1" style="17" min="1" max="1"/>
-    <col width="40.140625" customWidth="1" style="17" min="2" max="2"/>
-    <col width="16.28515625" customWidth="1" style="17" min="3" max="3"/>
-    <col width="7.85546875" customWidth="1" style="17" min="4" max="4"/>
-    <col width="15.140625" customWidth="1" style="17" min="5" max="6"/>
-    <col width="8.5703125" customWidth="1" style="17" min="7" max="7"/>
-    <col width="11.42578125" customWidth="1" style="17" min="8" max="8"/>
-    <col width="74.28515625" customWidth="1" style="17" min="9" max="9"/>
-    <col width="42" customWidth="1" style="17" min="10" max="11"/>
-    <col width="27" customWidth="1" style="17" min="12" max="12"/>
-    <col width="42" customWidth="1" style="17" min="13" max="13"/>
-    <col width="15.7109375" customWidth="1" style="17" min="14" max="14"/>
-    <col width="26.7109375" customWidth="1" style="17" min="15" max="15"/>
-    <col width="22.28515625" customWidth="1" style="17" min="16" max="16"/>
-    <col width="27.5703125" customWidth="1" style="17" min="17" max="17"/>
-    <col width="37.5703125" customWidth="1" style="17" min="18" max="19"/>
-    <col width="38.85546875" customWidth="1" style="17" min="20" max="20"/>
-    <col width="37" customWidth="1" style="17" min="21" max="21"/>
-    <col width="31.5703125" customWidth="1" style="17" min="22" max="22"/>
-    <col width="27.85546875" customWidth="1" style="17" min="23" max="23"/>
-    <col width="26.42578125" customWidth="1" style="17" min="24" max="24"/>
-    <col width="29" customWidth="1" style="17" min="25" max="25"/>
-    <col width="37.28515625" customWidth="1" style="17" min="26" max="28"/>
-    <col width="36.42578125" customWidth="1" style="17" min="29" max="29"/>
-    <col width="28.5703125" customWidth="1" style="17" min="30" max="30"/>
-    <col width="30.140625" customWidth="1" style="17" min="31" max="32"/>
-    <col width="30.28515625" customWidth="1" style="17" min="33" max="33"/>
-    <col width="31" customWidth="1" style="17" min="34" max="34"/>
-    <col width="39.140625" customWidth="1" style="17" min="35" max="35"/>
-    <col width="41.7109375" customWidth="1" style="17" min="36" max="36"/>
-    <col width="39.5703125" customWidth="1" style="17" min="37" max="37"/>
-    <col width="29.42578125" customWidth="1" style="17" min="38" max="38"/>
-    <col width="30.28515625" customWidth="1" style="17" min="39" max="39"/>
-    <col width="25.85546875" customWidth="1" style="17" min="40" max="40"/>
-    <col width="30" customWidth="1" style="17" min="41" max="41"/>
-    <col width="37.7109375" customWidth="1" style="17" min="42" max="42"/>
-    <col width="36" customWidth="1" style="17" min="43" max="43"/>
-    <col width="37.7109375" customWidth="1" style="17" min="44" max="44"/>
-    <col width="37.28515625" customWidth="1" style="17" min="45" max="45"/>
-    <col width="38.5703125" customWidth="1" style="17" min="46" max="46"/>
+    <col width="14.42578125" customWidth="1" style="16" min="1" max="1"/>
+    <col width="40.140625" customWidth="1" style="16" min="2" max="2"/>
+    <col width="16.28515625" customWidth="1" style="16" min="3" max="3"/>
+    <col width="7.85546875" customWidth="1" style="16" min="4" max="4"/>
+    <col width="15.140625" customWidth="1" style="16" min="5" max="6"/>
+    <col width="8.5703125" customWidth="1" style="16" min="7" max="7"/>
+    <col width="11.42578125" customWidth="1" style="16" min="8" max="8"/>
+    <col width="74.28515625" customWidth="1" style="16" min="9" max="9"/>
+    <col width="42" customWidth="1" style="16" min="10" max="11"/>
+    <col width="27" customWidth="1" style="16" min="12" max="12"/>
+    <col width="42" customWidth="1" style="16" min="13" max="13"/>
+    <col width="15.7109375" customWidth="1" style="16" min="14" max="14"/>
+    <col width="26.7109375" customWidth="1" style="16" min="15" max="15"/>
+    <col width="22.28515625" customWidth="1" style="16" min="16" max="16"/>
+    <col width="27.5703125" customWidth="1" style="16" min="17" max="17"/>
+    <col width="37.5703125" customWidth="1" style="16" min="18" max="19"/>
+    <col width="38.85546875" customWidth="1" style="16" min="20" max="20"/>
+    <col width="37" customWidth="1" style="16" min="21" max="21"/>
+    <col width="31.5703125" customWidth="1" style="16" min="22" max="22"/>
+    <col width="27.85546875" customWidth="1" style="16" min="23" max="23"/>
+    <col width="26.42578125" customWidth="1" style="16" min="24" max="24"/>
+    <col width="29" customWidth="1" style="16" min="25" max="25"/>
+    <col width="37.28515625" customWidth="1" style="16" min="26" max="28"/>
+    <col width="36.42578125" customWidth="1" style="16" min="29" max="29"/>
+    <col width="28.5703125" customWidth="1" style="16" min="30" max="30"/>
+    <col width="30.140625" customWidth="1" style="16" min="31" max="32"/>
+    <col width="30.28515625" customWidth="1" style="16" min="33" max="33"/>
+    <col width="31" customWidth="1" style="16" min="34" max="34"/>
+    <col width="39.140625" customWidth="1" style="16" min="35" max="35"/>
+    <col width="41.7109375" customWidth="1" style="16" min="36" max="36"/>
+    <col width="39.5703125" customWidth="1" style="16" min="37" max="37"/>
+    <col width="29.42578125" customWidth="1" style="16" min="38" max="38"/>
+    <col width="30.28515625" customWidth="1" style="16" min="39" max="39"/>
+    <col width="25.85546875" customWidth="1" style="16" min="40" max="40"/>
+    <col width="30" customWidth="1" style="16" min="41" max="41"/>
+    <col width="37.7109375" customWidth="1" style="16" min="42" max="42"/>
+    <col width="36" customWidth="1" style="16" min="43" max="43"/>
+    <col width="37.7109375" customWidth="1" style="16" min="44" max="44"/>
+    <col width="37.28515625" customWidth="1" style="16" min="45" max="45"/>
+    <col width="38.5703125" customWidth="1" style="16" min="46" max="46"/>
   </cols>
   <sheetData>
     <row r="1" ht="53.25" customFormat="1" customHeight="1" s="6">
@@ -561,7 +567,7 @@
       </c>
     </row>
     <row r="2" ht="61.5" customFormat="1" customHeight="1" s="1">
-      <c r="A2" s="16" t="n">
+      <c r="A2" s="2" t="n">
         <v>45774</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -581,7 +587,7 @@
       </c>
     </row>
     <row r="3" ht="15.75" customFormat="1" customHeight="1" s="1">
-      <c r="A3" s="16" t="n">
+      <c r="A3" s="2" t="n">
         <v>45774</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -592,7 +598,7 @@
       <c r="AB3" s="3" t="n"/>
     </row>
     <row r="4" customFormat="1" s="1">
-      <c r="A4" s="16" t="n">
+      <c r="A4" s="2" t="n">
         <v>45774</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -657,7 +663,7 @@
       <c r="AB7" s="3" t="n"/>
     </row>
     <row r="8" customFormat="1" s="1">
-      <c r="A8" s="16" t="n">
+      <c r="A8" s="2" t="n">
         <v>45774</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -701,7 +707,7 @@
       <c r="AB10" s="11" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="16" t="n">
+      <c r="A11" s="2" t="n">
         <v>45775</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -727,7 +733,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="16" t="n">
+      <c r="A13" s="2" t="n">
         <v>45775</v>
       </c>
       <c r="B13" t="inlineStr">
@@ -740,7 +746,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="16" t="n">
+      <c r="A14" s="2" t="n">
         <v>45775</v>
       </c>
       <c r="B14" t="inlineStr">
@@ -753,7 +759,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="16" t="n">
+      <c r="A15" s="2" t="n">
         <v>45775</v>
       </c>
       <c r="B15" t="inlineStr">
@@ -766,7 +772,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="16" t="n">
+      <c r="A16" s="2" t="n">
         <v>45775</v>
       </c>
       <c r="B16" t="inlineStr">
@@ -779,7 +785,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="16" t="n">
+      <c r="A17" s="2" t="n">
         <v>45775</v>
       </c>
       <c r="B17" t="inlineStr">
@@ -789,7 +795,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="16" t="n">
+      <c r="A18" s="2" t="n">
         <v>45775</v>
       </c>
       <c r="B18" t="inlineStr">
@@ -829,7 +835,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="16" t="n">
+      <c r="A21" s="2" t="n">
         <v>45776</v>
       </c>
       <c r="B21" t="inlineStr">
@@ -845,7 +851,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="16" t="n">
+      <c r="A22" s="2" t="n">
         <v>45776</v>
       </c>
       <c r="B22" t="inlineStr">
@@ -858,7 +864,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="16" t="n">
+      <c r="A23" s="2" t="n">
         <v>45776</v>
       </c>
       <c r="B23" t="inlineStr">
@@ -871,7 +877,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="16" t="n">
+      <c r="A24" s="2" t="n">
         <v>45776</v>
       </c>
       <c r="B24" t="inlineStr">
@@ -884,7 +890,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="16" t="n">
+      <c r="A25" s="2" t="n">
         <v>45776</v>
       </c>
       <c r="B25" t="inlineStr">
@@ -897,7 +903,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="16" t="n">
+      <c r="A26" s="2" t="n">
         <v>45776</v>
       </c>
       <c r="B26" t="inlineStr">
@@ -907,7 +913,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="16" t="n">
+      <c r="A27" s="2" t="n">
         <v>45776</v>
       </c>
       <c r="B27" t="inlineStr">
@@ -923,7 +929,7 @@
       <c r="A28" s="8" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="16" t="n">
+      <c r="A29" s="2" t="n">
         <v>45777</v>
       </c>
       <c r="B29" t="inlineStr">
@@ -939,7 +945,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="16" t="n">
+      <c r="A30" s="2" t="n">
         <v>45777</v>
       </c>
       <c r="B30" t="inlineStr">
@@ -976,7 +982,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="16" t="n">
+      <c r="A32" s="2" t="n">
         <v>45777</v>
       </c>
       <c r="B32" t="inlineStr">
@@ -989,7 +995,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="16" t="n">
+      <c r="A33" s="2" t="n">
         <v>45777</v>
       </c>
       <c r="B33" t="inlineStr">
@@ -1007,7 +1013,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="16" t="n">
+      <c r="A34" s="2" t="n">
         <v>45777</v>
       </c>
       <c r="B34" t="inlineStr">
@@ -1020,7 +1026,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="16" t="n">
+      <c r="A35" s="2" t="n">
         <v>45777</v>
       </c>
       <c r="B35" t="inlineStr">
@@ -1030,7 +1036,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="16" t="n">
+      <c r="A36" s="2" t="n">
         <v>45777</v>
       </c>
       <c r="B36" t="inlineStr">
@@ -1046,7 +1052,7 @@
       <c r="A37" s="8" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="16" t="n">
+      <c r="A38" s="2" t="n">
         <v>45778</v>
       </c>
       <c r="B38" t="inlineStr">
@@ -1062,7 +1068,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="16" t="n">
+      <c r="A39" s="2" t="n">
         <v>45778</v>
       </c>
       <c r="B39" t="inlineStr">
@@ -1078,7 +1084,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="16" t="n">
+      <c r="A40" s="2" t="n">
         <v>45778</v>
       </c>
       <c r="B40" t="inlineStr">
@@ -1091,7 +1097,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="16" t="n">
+      <c r="A41" s="2" t="n">
         <v>45778</v>
       </c>
       <c r="B41" t="inlineStr">
@@ -1104,7 +1110,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="16" t="n">
+      <c r="A42" s="2" t="n">
         <v>45778</v>
       </c>
       <c r="B42" t="inlineStr">
@@ -1117,7 +1123,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="16" t="n">
+      <c r="A43" s="2" t="n">
         <v>45778</v>
       </c>
       <c r="B43" t="inlineStr">
@@ -1151,7 +1157,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="16" t="n">
+      <c r="A45" s="2" t="n">
         <v>45778</v>
       </c>
       <c r="B45" t="inlineStr">
@@ -1167,7 +1173,7 @@
       <c r="A46" s="8" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="16" t="n">
+      <c r="A47" s="2" t="n">
         <v>45779</v>
       </c>
       <c r="B47" t="inlineStr">
@@ -1188,7 +1194,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="16" t="n">
+      <c r="A48" s="2" t="n">
         <v>45779</v>
       </c>
       <c r="B48" t="inlineStr">
@@ -1209,7 +1215,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="16" t="n">
+      <c r="A49" s="2" t="n">
         <v>45779</v>
       </c>
       <c r="B49" t="inlineStr">
@@ -1222,7 +1228,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="16" t="n">
+      <c r="A50" s="2" t="n">
         <v>45779</v>
       </c>
       <c r="B50" t="inlineStr">
@@ -1235,7 +1241,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="16" t="n">
+      <c r="A51" s="2" t="n">
         <v>45779</v>
       </c>
       <c r="B51" t="inlineStr">
@@ -1248,7 +1254,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="16" t="n">
+      <c r="A52" s="2" t="n">
         <v>45779</v>
       </c>
       <c r="B52" t="inlineStr">
@@ -1266,7 +1272,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="16" t="n">
+      <c r="A53" s="2" t="n">
         <v>45779</v>
       </c>
       <c r="B53" t="inlineStr">
@@ -1279,7 +1285,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="16" t="n">
+      <c r="A54" s="2" t="n">
         <v>45779</v>
       </c>
       <c r="B54" t="inlineStr">
@@ -1293,7 +1299,7 @@
     </row>
     <row r="55" customFormat="1" s="9"/>
     <row r="56">
-      <c r="A56" s="16" t="n">
+      <c r="A56" s="2" t="n">
         <v>45780</v>
       </c>
       <c r="B56" t="inlineStr">
@@ -1309,7 +1315,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="16" t="n">
+      <c r="A57" s="2" t="n">
         <v>45780</v>
       </c>
       <c r="B57" t="inlineStr">
@@ -1325,7 +1331,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="16" t="n">
+      <c r="A58" s="2" t="n">
         <v>45780</v>
       </c>
       <c r="B58" t="inlineStr">
@@ -1338,7 +1344,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="16" t="n">
+      <c r="A59" s="2" t="n">
         <v>45780</v>
       </c>
       <c r="B59" t="inlineStr">
@@ -1351,7 +1357,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="16" t="n">
+      <c r="A60" s="2" t="n">
         <v>45780</v>
       </c>
       <c r="B60" t="inlineStr">
@@ -1364,7 +1370,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="16" t="n">
+      <c r="A61" s="2" t="n">
         <v>45780</v>
       </c>
       <c r="B61" t="inlineStr">
@@ -1377,7 +1383,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="16" t="n">
+      <c r="A62" s="2" t="n">
         <v>45780</v>
       </c>
       <c r="B62" t="inlineStr">
@@ -1390,7 +1396,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="16" t="n">
+      <c r="A63" s="2" t="n">
         <v>45780</v>
       </c>
       <c r="B63" t="inlineStr">
@@ -1406,7 +1412,7 @@
       <c r="A64" s="8" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" s="16" t="n">
+      <c r="A65" s="2" t="n">
         <v>45781</v>
       </c>
       <c r="B65" t="inlineStr">
@@ -1475,7 +1481,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="16" t="n">
+      <c r="A68" s="2" t="n">
         <v>45781</v>
       </c>
       <c r="B68" t="inlineStr">
@@ -1512,7 +1518,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="16" t="n">
+      <c r="A70" s="2" t="n">
         <v>45781</v>
       </c>
       <c r="B70" t="inlineStr">
@@ -1525,7 +1531,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="16" t="n">
+      <c r="A71" s="2" t="n">
         <v>45781</v>
       </c>
       <c r="B71" t="inlineStr">
@@ -1538,7 +1544,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="16" t="n">
+      <c r="A72" s="2" t="n">
         <v>45781</v>
       </c>
       <c r="B72" t="inlineStr">
@@ -1554,7 +1560,7 @@
       <c r="A73" s="8" t="n"/>
     </row>
     <row r="74">
-      <c r="A74" s="16" t="n">
+      <c r="A74" s="2" t="n">
         <v>45782</v>
       </c>
       <c r="B74" t="inlineStr">
@@ -1570,7 +1576,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="16" t="n">
+      <c r="A75" s="2" t="n">
         <v>45782</v>
       </c>
       <c r="B75" t="inlineStr">
@@ -1586,7 +1592,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="16" t="n">
+      <c r="A76" s="2" t="n">
         <v>45782</v>
       </c>
       <c r="B76" t="inlineStr">
@@ -1607,7 +1613,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="16" t="n">
+      <c r="A77" s="2" t="n">
         <v>45782</v>
       </c>
       <c r="B77" t="inlineStr">
@@ -1620,7 +1626,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="16" t="n">
+      <c r="A78" s="2" t="n">
         <v>45782</v>
       </c>
       <c r="B78" t="inlineStr">
@@ -1654,7 +1660,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="16" t="n">
+      <c r="A80" s="2" t="n">
         <v>45782</v>
       </c>
       <c r="B80" t="inlineStr">
@@ -1667,7 +1673,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="16" t="n">
+      <c r="A81" s="2" t="n">
         <v>45782</v>
       </c>
       <c r="B81" t="inlineStr">
@@ -1681,7 +1687,7 @@
     </row>
     <row r="82" customFormat="1" s="9"/>
     <row r="83">
-      <c r="A83" s="16" t="n">
+      <c r="A83" s="2" t="n">
         <v>45783</v>
       </c>
       <c r="B83" t="inlineStr">
@@ -1697,7 +1703,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="16" t="n">
+      <c r="A84" s="2" t="n">
         <v>45783</v>
       </c>
       <c r="B84" t="inlineStr">
@@ -1713,7 +1719,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="16" t="n">
+      <c r="A85" s="2" t="n">
         <v>45783</v>
       </c>
       <c r="B85" t="inlineStr">
@@ -1758,7 +1764,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="16" t="n">
+      <c r="A87" s="2" t="n">
         <v>45783</v>
       </c>
       <c r="B87" t="inlineStr">
@@ -1776,7 +1782,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="16" t="n">
+      <c r="A88" s="2" t="n">
         <v>45783</v>
       </c>
       <c r="B88" t="inlineStr">
@@ -1841,7 +1847,7 @@
     </row>
     <row r="91" customFormat="1" s="9"/>
     <row r="92">
-      <c r="A92" s="16" t="n">
+      <c r="A92" s="2" t="n">
         <v>45784</v>
       </c>
       <c r="B92" t="inlineStr">
@@ -1857,7 +1863,7 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="16" t="n">
+      <c r="A93" s="2" t="n">
         <v>45784</v>
       </c>
       <c r="B93" t="inlineStr">
@@ -1873,7 +1879,7 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="16" t="n">
+      <c r="A94" s="2" t="n">
         <v>45784</v>
       </c>
       <c r="B94" t="inlineStr">
@@ -1889,7 +1895,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="16" t="n">
+      <c r="A95" s="2" t="n">
         <v>45784</v>
       </c>
       <c r="B95" t="inlineStr">
@@ -1905,7 +1911,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="16" t="n">
+      <c r="A96" s="2" t="n">
         <v>45784</v>
       </c>
       <c r="B96" t="inlineStr">
@@ -1921,7 +1927,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="16" t="n">
+      <c r="A97" s="2" t="n">
         <v>45784</v>
       </c>
       <c r="B97" t="inlineStr">
@@ -1934,7 +1940,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="16" t="n">
+      <c r="A98" s="2" t="n">
         <v>45784</v>
       </c>
       <c r="B98" t="inlineStr">
@@ -1950,7 +1956,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="16" t="n">
+      <c r="A99" s="2" t="n">
         <v>45784</v>
       </c>
       <c r="B99" t="inlineStr">
@@ -1991,7 +1997,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="16" t="n">
+      <c r="A102" s="2" t="n">
         <v>45785</v>
       </c>
       <c r="B102" t="inlineStr">
@@ -2031,7 +2037,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="16" t="n">
+      <c r="A104" s="2" t="n">
         <v>45785</v>
       </c>
       <c r="B104" t="inlineStr">
@@ -2071,7 +2077,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="16" t="n">
+      <c r="A106" s="2" t="n">
         <v>45785</v>
       </c>
       <c r="B106" t="inlineStr">
@@ -2084,7 +2090,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="16" t="n">
+      <c r="A107" s="2" t="n">
         <v>45785</v>
       </c>
       <c r="B107" t="inlineStr">
@@ -2100,7 +2106,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="16" t="n">
+      <c r="A108" s="2" t="n">
         <v>45785</v>
       </c>
       <c r="B108" t="inlineStr">
@@ -2117,7 +2123,7 @@
     </row>
     <row r="109" customFormat="1" s="9"/>
     <row r="110">
-      <c r="A110" s="16" t="n">
+      <c r="A110" s="2" t="n">
         <v>45786</v>
       </c>
       <c r="B110" t="inlineStr">
@@ -2133,7 +2139,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="16" t="n">
+      <c r="A111" s="2" t="n">
         <v>45786</v>
       </c>
       <c r="B111" t="inlineStr">
@@ -2149,7 +2155,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="16" t="n">
+      <c r="A112" s="2" t="n">
         <v>45786</v>
       </c>
       <c r="B112" t="inlineStr">
@@ -2165,7 +2171,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="16" t="n">
+      <c r="A113" s="2" t="n">
         <v>45786</v>
       </c>
       <c r="B113" t="inlineStr">
@@ -2181,7 +2187,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="16" t="n">
+      <c r="A114" s="2" t="n">
         <v>45786</v>
       </c>
       <c r="B114" t="inlineStr">
@@ -2197,7 +2203,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="16" t="n">
+      <c r="A115" s="2" t="n">
         <v>45786</v>
       </c>
       <c r="B115" t="inlineStr">
@@ -2213,7 +2219,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="16" t="n">
+      <c r="A116" s="2" t="n">
         <v>45786</v>
       </c>
       <c r="B116" t="inlineStr">
@@ -2229,7 +2235,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="16" t="n">
+      <c r="A117" s="2" t="n">
         <v>45786</v>
       </c>
       <c r="B117" t="inlineStr">
@@ -2246,7 +2252,7 @@
     </row>
     <row r="118" customFormat="1" s="9"/>
     <row r="119">
-      <c r="A119" s="16" t="n">
+      <c r="A119" s="2" t="n">
         <v>45787</v>
       </c>
       <c r="B119" t="inlineStr">
@@ -2262,7 +2268,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="16" t="n">
+      <c r="A120" s="2" t="n">
         <v>45787</v>
       </c>
       <c r="B120" t="inlineStr">
@@ -2278,7 +2284,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="16" t="n">
+      <c r="A121" s="2" t="n">
         <v>45787</v>
       </c>
       <c r="B121" t="inlineStr">
@@ -2294,7 +2300,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="16" t="n">
+      <c r="A122" s="2" t="n">
         <v>45787</v>
       </c>
       <c r="B122" t="inlineStr">
@@ -2310,7 +2316,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="16" t="n">
+      <c r="A123" s="2" t="n">
         <v>45787</v>
       </c>
       <c r="B123" t="inlineStr">
@@ -2326,7 +2332,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="16" t="n">
+      <c r="A124" s="2" t="n">
         <v>45787</v>
       </c>
       <c r="B124" t="inlineStr">
@@ -2342,7 +2348,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="16" t="n">
+      <c r="A125" s="2" t="n">
         <v>45787</v>
       </c>
       <c r="B125" t="inlineStr">
@@ -2358,7 +2364,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="16" t="n">
+      <c r="A126" s="2" t="n">
         <v>45787</v>
       </c>
       <c r="B126" t="inlineStr">
@@ -2375,7 +2381,7 @@
     </row>
     <row r="127" customFormat="1" s="9"/>
     <row r="128">
-      <c r="A128" s="16" t="n">
+      <c r="A128" s="2" t="n">
         <v>45788</v>
       </c>
       <c r="B128" t="inlineStr">
@@ -2391,7 +2397,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="16" t="n">
+      <c r="A129" s="2" t="n">
         <v>45788</v>
       </c>
       <c r="B129" t="inlineStr">
@@ -2407,7 +2413,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="16" t="n">
+      <c r="A130" s="2" t="n">
         <v>45788</v>
       </c>
       <c r="B130" t="inlineStr">
@@ -2423,7 +2429,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="16" t="n">
+      <c r="A131" s="2" t="n">
         <v>45788</v>
       </c>
       <c r="B131" t="inlineStr">
@@ -2439,7 +2445,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="16" t="n">
+      <c r="A132" s="2" t="n">
         <v>45788</v>
       </c>
       <c r="B132" t="inlineStr">
@@ -2455,7 +2461,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="16" t="n">
+      <c r="A133" s="2" t="n">
         <v>45788</v>
       </c>
       <c r="B133" t="inlineStr">
@@ -2510,7 +2516,7 @@
     </row>
     <row r="136" customFormat="1" s="9"/>
     <row r="137">
-      <c r="A137" s="16" t="n">
+      <c r="A137" s="2" t="n">
         <v>45789</v>
       </c>
       <c r="B137" t="inlineStr">
@@ -2550,7 +2556,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="16" t="n">
+      <c r="A139" s="2" t="n">
         <v>45789</v>
       </c>
       <c r="B139" t="inlineStr">
@@ -2590,7 +2596,7 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="16" t="n">
+      <c r="A141" s="2" t="n">
         <v>45789</v>
       </c>
       <c r="B141" t="inlineStr">
@@ -2606,7 +2612,7 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="16" t="n">
+      <c r="A142" s="2" t="n">
         <v>45789</v>
       </c>
       <c r="B142" t="inlineStr">
@@ -2622,7 +2628,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="16" t="n">
+      <c r="A143" s="2" t="n">
         <v>45789</v>
       </c>
       <c r="B143" t="inlineStr">
@@ -2638,7 +2644,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="16" t="n">
+      <c r="A144" s="2" t="n">
         <v>45789</v>
       </c>
       <c r="B144" t="inlineStr">
@@ -2655,7 +2661,7 @@
     </row>
     <row r="145" customFormat="1" s="9"/>
     <row r="146">
-      <c r="A146" s="16" t="n">
+      <c r="A146" s="2" t="n">
         <v>45790</v>
       </c>
       <c r="B146" t="inlineStr">
@@ -2671,7 +2677,7 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="16" t="n">
+      <c r="A147" s="2" t="n">
         <v>45790</v>
       </c>
       <c r="B147" t="inlineStr">
@@ -2687,7 +2693,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="16" t="n">
+      <c r="A148" s="2" t="n">
         <v>45790</v>
       </c>
       <c r="B148" t="inlineStr">
@@ -2703,7 +2709,7 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="16" t="n">
+      <c r="A149" s="2" t="n">
         <v>45790</v>
       </c>
       <c r="B149" t="inlineStr">
@@ -2719,7 +2725,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="16" t="n">
+      <c r="A150" s="2" t="n">
         <v>45790</v>
       </c>
       <c r="B150" t="inlineStr">
@@ -2735,7 +2741,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="16" t="n">
+      <c r="A151" s="2" t="n">
         <v>45790</v>
       </c>
       <c r="B151" t="inlineStr">
@@ -2751,7 +2757,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="16" t="n">
+      <c r="A152" s="2" t="n">
         <v>45790</v>
       </c>
       <c r="B152" t="inlineStr">
@@ -2767,7 +2773,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="16" t="n">
+      <c r="A153" s="2" t="n">
         <v>45790</v>
       </c>
       <c r="B153" t="inlineStr">
@@ -2784,7 +2790,7 @@
     </row>
     <row r="154" customFormat="1" s="9"/>
     <row r="155">
-      <c r="A155" s="16" t="n">
+      <c r="A155" s="2" t="n">
         <v>45791</v>
       </c>
       <c r="B155" t="inlineStr">
@@ -2800,7 +2806,7 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="16" t="n">
+      <c r="A156" s="2" t="n">
         <v>45791</v>
       </c>
       <c r="B156" t="inlineStr">
@@ -2835,7 +2841,7 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="16" t="n">
+      <c r="A158" s="2" t="n">
         <v>45791</v>
       </c>
       <c r="B158" t="inlineStr">
@@ -2870,7 +2876,7 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="16" t="n">
+      <c r="A160" s="2" t="n">
         <v>45791</v>
       </c>
       <c r="B160" t="inlineStr">
@@ -2886,7 +2892,7 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="16" t="n">
+      <c r="A161" s="2" t="n">
         <v>45791</v>
       </c>
       <c r="B161" t="inlineStr">
@@ -2902,7 +2908,7 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="16" t="n">
+      <c r="A162" s="2" t="n">
         <v>45791</v>
       </c>
       <c r="B162" t="inlineStr">
@@ -2932,6 +2938,9 @@
       <c r="C164" s="7" t="n">
         <v>7</v>
       </c>
+      <c r="F164" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -2947,6 +2956,9 @@
       <c r="C165" t="n">
         <v>3</v>
       </c>
+      <c r="F165" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -2962,6 +2974,9 @@
       <c r="C166" t="n">
         <v>1</v>
       </c>
+      <c r="F166" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -2977,6 +2992,9 @@
       <c r="C167" t="n">
         <v>3</v>
       </c>
+      <c r="F167" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -2992,6 +3010,9 @@
       <c r="C168" t="n">
         <v>1</v>
       </c>
+      <c r="F168" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -3008,7 +3029,7 @@
         <v>10</v>
       </c>
       <c r="F169" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="170">
@@ -3025,6 +3046,9 @@
       <c r="C170" t="n">
         <v>4</v>
       </c>
+      <c r="F170" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -3041,7 +3065,7 @@
         <v>4</v>
       </c>
       <c r="F171" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="172" customFormat="1" s="9"/>
@@ -3059,6 +3083,9 @@
       <c r="C173" s="7" t="n">
         <v>8</v>
       </c>
+      <c r="F173" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -3074,6 +3101,9 @@
       <c r="C174" t="n">
         <v>4</v>
       </c>
+      <c r="F174" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -3089,6 +3119,9 @@
       <c r="C175" t="n">
         <v>2</v>
       </c>
+      <c r="F175" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -3104,6 +3137,9 @@
       <c r="C176" t="n">
         <v>4</v>
       </c>
+      <c r="F176" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -3119,6 +3155,9 @@
       <c r="C177" t="n">
         <v>2</v>
       </c>
+      <c r="F177" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="13" t="inlineStr">
@@ -3142,6 +3181,9 @@
           <t>compo 1pw</t>
         </is>
       </c>
+      <c r="F178" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -3157,6 +3199,9 @@
       <c r="C179" t="n">
         <v>5</v>
       </c>
+      <c r="F179" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="13" t="inlineStr">
@@ -3180,6 +3225,9 @@
           <t>compo 1pw</t>
         </is>
       </c>
+      <c r="F180" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -3215,6 +3263,9 @@
           <t>compo 1pw</t>
         </is>
       </c>
+      <c r="F182" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -3229,7 +3280,7 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="13" t="inlineStr">
+      <c r="A184" t="inlineStr">
         <is>
           <t>16.05.2025</t>
         </is>
@@ -3253,7 +3304,7 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" s="13" t="inlineStr">
+      <c r="A186" t="inlineStr">
         <is>
           <t>16.05.2025</t>
         </is>
@@ -3264,7 +3315,7 @@
         </is>
       </c>
     </row>
-    <row r="187"/>
+    <row r="187" customFormat="1" s="17"/>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
@@ -3276,6 +3327,12 @@
           <t>Calathea Medalion</t>
         </is>
       </c>
+      <c r="C188" t="n">
+        <v>9</v>
+      </c>
+      <c r="F188" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -3288,6 +3345,12 @@
           <t>Calathea Orbifolia</t>
         </is>
       </c>
+      <c r="C189" t="n">
+        <v>5</v>
+      </c>
+      <c r="F189" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -3300,6 +3363,12 @@
           <t>Epiprenum Aureum</t>
         </is>
       </c>
+      <c r="C190" t="n">
+        <v>3</v>
+      </c>
+      <c r="F190" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -3312,6 +3381,12 @@
           <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
+      <c r="C191" t="n">
+        <v>5</v>
+      </c>
+      <c r="F191" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -3324,6 +3399,12 @@
           <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
+      <c r="C192" t="n">
+        <v>3</v>
+      </c>
+      <c r="F192" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -3336,6 +3417,12 @@
           <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
+      <c r="C193" t="n">
+        <v>1</v>
+      </c>
+      <c r="F193" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -3348,6 +3435,12 @@
           <t>Coffea Arabica</t>
         </is>
       </c>
+      <c r="C194" t="n">
+        <v>6</v>
+      </c>
+      <c r="F194" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -3360,17 +3453,37 @@
           <t>Monstera Adenossii</t>
         </is>
       </c>
+      <c r="C195" t="n">
+        <v>1</v>
+      </c>
+      <c r="F195" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="196">
-      <c r="A196" t="inlineStr">
+      <c r="A196" s="13" t="inlineStr">
         <is>
           <t>17.05.2025</t>
         </is>
       </c>
-      <c r="B196" t="inlineStr">
+      <c r="B196" s="13" t="inlineStr">
         <is>
           <t>Ficus Elastica Abidjan</t>
         </is>
+      </c>
+      <c r="C196" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D196" t="n">
+        <v>500</v>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>compo 1pw</t>
+        </is>
+      </c>
+      <c r="F196" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="197">
@@ -3383,6 +3496,12 @@
         <is>
           <t>Calathea Ornata</t>
         </is>
+      </c>
+      <c r="C197" t="n">
+        <v>1</v>
+      </c>
+      <c r="F197" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="198">

</xml_diff>

<commit_message>
improved pllt function for missed waterings
</commit_message>
<xml_diff>
--- a/data/blumen_data.xlsx
+++ b/data/blumen_data.xlsx
@@ -9,14 +9,14 @@
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -46,6 +46,13 @@
       <i val="1"/>
       <color rgb="FF216D20"/>
       <sz val="24"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -98,7 +105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -124,6 +131,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -470,8 +478,8 @@
   <dimension ref="A1:AB322"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E204" sqref="E204"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1623,6 +1631,9 @@
       <c r="C77" s="7" t="n">
         <v>8</v>
       </c>
+      <c r="D77" s="17" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
@@ -2309,6 +2320,9 @@
       </c>
       <c r="C122" t="n">
         <v>4</v>
+      </c>
+      <c r="D122" s="17" t="n">
+        <v>200</v>
       </c>
       <c r="F122" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
removed mocked data for missed waterings
</commit_message>
<xml_diff>
--- a/data/blumen_data.xlsx
+++ b/data/blumen_data.xlsx
@@ -478,8 +478,8 @@
   <dimension ref="A1:AB322"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F74" sqref="F74"/>
+      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F214" sqref="F214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1631,9 +1631,7 @@
       <c r="C77" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="D77" s="17" t="n">
-        <v>200</v>
-      </c>
+      <c r="D77" s="17" t="n"/>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
@@ -2321,9 +2319,7 @@
       <c r="C122" t="n">
         <v>4</v>
       </c>
-      <c r="D122" s="17" t="n">
-        <v>200</v>
-      </c>
+      <c r="D122" s="17" t="n"/>
       <c r="F122" t="n">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
added neemoil and changed watering day symbol
</commit_message>
<xml_diff>
--- a/data/blumen_data.xlsx
+++ b/data/blumen_data.xlsx
@@ -482,11 +482,11 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB397"/>
+  <dimension ref="A1:AC397"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G237" sqref="G237"/>
+      <pane ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H275" sqref="H275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -497,40 +497,41 @@
     <col width="7.85546875" customWidth="1" min="4" max="4"/>
     <col width="15.140625" customWidth="1" min="5" max="6"/>
     <col width="8.5703125" customWidth="1" min="7" max="7"/>
-    <col width="11.42578125" customWidth="1" min="8" max="8"/>
-    <col width="74.28515625" customWidth="1" min="9" max="9"/>
-    <col width="42" customWidth="1" min="10" max="11"/>
-    <col width="27" customWidth="1" min="12" max="12"/>
-    <col width="42" customWidth="1" min="13" max="13"/>
-    <col width="15.7109375" customWidth="1" min="14" max="14"/>
-    <col width="26.7109375" customWidth="1" min="15" max="15"/>
-    <col width="22.28515625" customWidth="1" min="16" max="16"/>
-    <col width="27.5703125" customWidth="1" min="17" max="17"/>
-    <col width="37.5703125" customWidth="1" min="18" max="19"/>
-    <col width="38.85546875" customWidth="1" min="20" max="20"/>
-    <col width="37" customWidth="1" min="21" max="21"/>
-    <col width="31.5703125" customWidth="1" min="22" max="22"/>
-    <col width="27.85546875" customWidth="1" min="23" max="23"/>
-    <col width="26.42578125" customWidth="1" min="24" max="24"/>
-    <col width="29" customWidth="1" min="25" max="25"/>
-    <col width="37.28515625" customWidth="1" min="26" max="28"/>
-    <col width="36.42578125" customWidth="1" min="29" max="29"/>
-    <col width="28.5703125" customWidth="1" min="30" max="30"/>
-    <col width="30.140625" customWidth="1" min="31" max="32"/>
-    <col width="30.28515625" customWidth="1" min="33" max="33"/>
-    <col width="31" customWidth="1" min="34" max="34"/>
-    <col width="39.140625" customWidth="1" min="35" max="35"/>
-    <col width="41.7109375" customWidth="1" min="36" max="36"/>
-    <col width="39.5703125" customWidth="1" min="37" max="37"/>
-    <col width="29.42578125" customWidth="1" min="38" max="38"/>
-    <col width="30.28515625" customWidth="1" min="39" max="39"/>
-    <col width="25.85546875" customWidth="1" min="40" max="40"/>
-    <col width="30" customWidth="1" min="41" max="41"/>
-    <col width="37.7109375" customWidth="1" min="42" max="42"/>
-    <col width="36" customWidth="1" min="43" max="43"/>
-    <col width="37.7109375" customWidth="1" min="44" max="44"/>
-    <col width="37.28515625" customWidth="1" min="45" max="45"/>
-    <col width="38.5703125" customWidth="1" min="46" max="46"/>
+    <col width="11.5703125" customWidth="1" min="8" max="8"/>
+    <col width="11.42578125" customWidth="1" min="9" max="9"/>
+    <col width="74.28515625" customWidth="1" min="10" max="10"/>
+    <col width="42" customWidth="1" min="11" max="12"/>
+    <col width="27" customWidth="1" min="13" max="13"/>
+    <col width="42" customWidth="1" min="14" max="14"/>
+    <col width="15.7109375" customWidth="1" min="15" max="15"/>
+    <col width="26.7109375" customWidth="1" min="16" max="16"/>
+    <col width="22.28515625" customWidth="1" min="17" max="17"/>
+    <col width="27.5703125" customWidth="1" min="18" max="18"/>
+    <col width="37.5703125" customWidth="1" min="19" max="20"/>
+    <col width="38.85546875" customWidth="1" min="21" max="21"/>
+    <col width="37" customWidth="1" min="22" max="22"/>
+    <col width="31.5703125" customWidth="1" min="23" max="23"/>
+    <col width="27.85546875" customWidth="1" min="24" max="24"/>
+    <col width="26.42578125" customWidth="1" min="25" max="25"/>
+    <col width="29" customWidth="1" min="26" max="26"/>
+    <col width="37.28515625" customWidth="1" min="27" max="29"/>
+    <col width="36.42578125" customWidth="1" min="30" max="30"/>
+    <col width="28.5703125" customWidth="1" min="31" max="31"/>
+    <col width="30.140625" customWidth="1" min="32" max="33"/>
+    <col width="30.28515625" customWidth="1" min="34" max="34"/>
+    <col width="31" customWidth="1" min="35" max="35"/>
+    <col width="39.140625" customWidth="1" min="36" max="36"/>
+    <col width="41.7109375" customWidth="1" min="37" max="37"/>
+    <col width="39.5703125" customWidth="1" min="38" max="38"/>
+    <col width="29.42578125" customWidth="1" min="39" max="39"/>
+    <col width="30.28515625" customWidth="1" min="40" max="40"/>
+    <col width="25.85546875" customWidth="1" min="41" max="41"/>
+    <col width="30" customWidth="1" min="42" max="42"/>
+    <col width="37.7109375" customWidth="1" min="43" max="43"/>
+    <col width="36" customWidth="1" min="44" max="44"/>
+    <col width="37.7109375" customWidth="1" min="45" max="45"/>
+    <col width="37.28515625" customWidth="1" min="46" max="46"/>
+    <col width="38.5703125" customWidth="1" min="47" max="47"/>
   </cols>
   <sheetData>
     <row r="1" ht="53.25" customFormat="1" customHeight="1" s="6">
@@ -571,10 +572,15 @@
       </c>
       <c r="H1" s="6" t="inlineStr">
         <is>
+          <t>neemoil</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
           <t>size</t>
         </is>
       </c>
-      <c r="I1" s="6" t="inlineStr">
+      <c r="J1" s="6" t="inlineStr">
         <is>
           <t>condition</t>
         </is>
@@ -589,12 +595,12 @@
           <t>Calathea Medalion</t>
         </is>
       </c>
-      <c r="J2" s="15" t="inlineStr">
+      <c r="K2" s="15" t="inlineStr">
         <is>
           <t>Calathea veitchiana</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>https://www.epicgardening.com/calathea-varieties/</t>
         </is>
@@ -609,7 +615,7 @@
           <t>Calathea Orbifolia</t>
         </is>
       </c>
-      <c r="AB3" s="3" t="n"/>
+      <c r="AC3" s="3" t="n"/>
     </row>
     <row r="4" customFormat="1" s="1">
       <c r="A4" s="2" t="n">
@@ -623,7 +629,7 @@
       <c r="C4" t="n">
         <v>1</v>
       </c>
-      <c r="AB4" s="3" t="n"/>
+      <c r="AC4" s="3" t="n"/>
     </row>
     <row r="5" customFormat="1" s="1">
       <c r="A5" s="5" t="n">
@@ -640,7 +646,7 @@
       <c r="D5" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="AB5" s="3" t="n"/>
+      <c r="AC5" s="3" t="n"/>
     </row>
     <row r="6" customFormat="1" s="1">
       <c r="A6" s="5" t="n">
@@ -657,7 +663,7 @@
       <c r="D6" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="AB6" s="3" t="n"/>
+      <c r="AC6" s="3" t="n"/>
     </row>
     <row r="7" customFormat="1" s="1">
       <c r="A7" s="5" t="n">
@@ -674,7 +680,7 @@
       <c r="D7" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="AB7" s="3" t="n"/>
+      <c r="AC7" s="3" t="n"/>
     </row>
     <row r="8" customFormat="1" s="1">
       <c r="A8" s="2" t="n">
@@ -685,7 +691,7 @@
           <t>Coffea Arabica</t>
         </is>
       </c>
-      <c r="AB8" s="3" t="n"/>
+      <c r="AC8" s="3" t="n"/>
     </row>
     <row r="9" customFormat="1" s="1">
       <c r="A9" s="5" t="n">
@@ -702,7 +708,7 @@
       <c r="D9" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="AB9" s="3" t="n"/>
+      <c r="AC9" s="3" t="n"/>
     </row>
     <row r="10" customFormat="1" s="10">
       <c r="A10" s="8" t="n"/>
@@ -718,7 +724,8 @@
       <c r="K10" s="9" t="n"/>
       <c r="L10" s="9" t="n"/>
       <c r="M10" s="9" t="n"/>
-      <c r="AB10" s="11" t="n"/>
+      <c r="N10" s="9" t="n"/>
+      <c r="AC10" s="11" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -994,6 +1001,7 @@
           <t>ja</t>
         </is>
       </c>
+      <c r="H31" s="4" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
@@ -1025,6 +1033,7 @@
           <t>ja</t>
         </is>
       </c>
+      <c r="H33" s="4" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
@@ -1169,6 +1178,7 @@
           <t>ja</t>
         </is>
       </c>
+      <c r="H44" s="4" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
@@ -1206,6 +1216,7 @@
           <t>ja</t>
         </is>
       </c>
+      <c r="H47" s="4" t="n"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
@@ -1227,6 +1238,7 @@
           <t>ja</t>
         </is>
       </c>
+      <c r="H48" s="4" t="n"/>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
@@ -1284,6 +1296,7 @@
           <t>ja</t>
         </is>
       </c>
+      <c r="H52" s="4" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
@@ -1488,7 +1501,7 @@
       <c r="F67" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I67" s="7" t="inlineStr">
+      <c r="J67" s="7" t="inlineStr">
         <is>
           <t>hat angefangen blätter zu gelben und blätter haben angefangen sich zu krümmen</t>
         </is>
@@ -1620,7 +1633,7 @@
       <c r="F76" t="n">
         <v>1</v>
       </c>
-      <c r="I76" s="7" t="inlineStr">
+      <c r="J76" s="7" t="inlineStr">
         <is>
           <t>hat angefangen blätter zu gelben und blätter haben angefangen sich zu krümmen</t>
         </is>
@@ -1748,7 +1761,7 @@
       <c r="F85" t="n">
         <v>2</v>
       </c>
-      <c r="I85" s="7" t="inlineStr">
+      <c r="J85" s="7" t="inlineStr">
         <is>
           <t>hat angefangen blätter zu gelben und blätter haben angefangen sich zu krümmen</t>
         </is>
@@ -1790,7 +1803,7 @@
       <c r="C87" t="n">
         <v>2</v>
       </c>
-      <c r="I87" s="4" t="inlineStr">
+      <c r="J87" s="4" t="inlineStr">
         <is>
           <t>es hat sich links ein neuer ast angefangen zu bilden</t>
         </is>
@@ -4738,6 +4751,11 @@
           <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
+      <c r="H283" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -4762,6 +4780,11 @@
           <t>Monstera Adenossii</t>
         </is>
       </c>
+      <c r="H285" t="inlineStr">
+        <is>
+          <t>ja</t>
+        </is>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -4772,6 +4795,11 @@
       <c r="B286" t="inlineStr">
         <is>
           <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+      <c r="H286" t="inlineStr">
+        <is>
+          <t>ja</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented redirection from index to plants/overview
</commit_message>
<xml_diff>
--- a/data/blumen_data.xlsx
+++ b/data/blumen_data.xlsx
@@ -482,7 +482,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC397"/>
+  <dimension ref="A1:AC412"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
@@ -6047,6 +6047,175 @@
       </c>
     </row>
     <row r="397"/>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>31.05.2025</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>31.05.2025</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Calathea Orbifolia</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>31.05.2025</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Epiprenum Aureum</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>31.05.2025</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>31.05.2025</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>31.05.2025</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>31.05.2025</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Coffea Arabica</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>31.05.2025</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>31.05.2025</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>31.05.2025</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Calathea Ornata</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>31.05.2025</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Beaucarnea recurvata</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>31.05.2025</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Nephrolepis obliterata</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>31.05.2025</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>31.05.2025</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+    </row>
+    <row r="412"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new plant pictures
</commit_message>
<xml_diff>
--- a/data/blumen_data.xlsx
+++ b/data/blumen_data.xlsx
@@ -485,11 +485,11 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC757"/>
+  <dimension ref="A1:AC787"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A580" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F591" sqref="F591"/>
+      <pane ySplit="1" topLeftCell="A595" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E619" sqref="E619"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -8416,24 +8416,25 @@
           <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
-    </row>
-    <row r="597" customFormat="1" s="7">
-      <c r="A597" s="7" t="inlineStr">
+      <c r="C596" s="7" t="n"/>
+      <c r="D596" s="7" t="n">
+        <v>300</v>
+      </c>
+      <c r="E596" s="13" t="inlineStr">
+        <is>
+          <t>compo 1pw</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
         <is>
           <t>13.06.2025</t>
         </is>
       </c>
-      <c r="B597" s="7" t="inlineStr">
+      <c r="B597" t="inlineStr">
         <is>
           <t>Scindapsus Treubii Moonlight</t>
-        </is>
-      </c>
-      <c r="D597" s="7" t="n">
-        <v>300</v>
-      </c>
-      <c r="E597" s="13" t="inlineStr">
-        <is>
-          <t>compo 1pw</t>
         </is>
       </c>
     </row>
@@ -8763,15 +8764,23 @@
         </is>
       </c>
     </row>
-    <row r="627">
-      <c r="A627" t="inlineStr">
+    <row r="627" customFormat="1" s="7">
+      <c r="A627" s="7" t="inlineStr">
         <is>
           <t>15.06.2025</t>
         </is>
       </c>
-      <c r="B627" t="inlineStr">
+      <c r="B627" s="7" t="inlineStr">
         <is>
           <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+      <c r="D627" s="7" t="n">
+        <v>300</v>
+      </c>
+      <c r="E627" s="13" t="inlineStr">
+        <is>
+          <t>compo 1pw</t>
         </is>
       </c>
     </row>
@@ -8799,15 +8808,23 @@
         </is>
       </c>
     </row>
-    <row r="630">
-      <c r="A630" t="inlineStr">
+    <row r="630" customFormat="1" s="7">
+      <c r="A630" s="7" t="inlineStr">
         <is>
           <t>15.06.2025</t>
         </is>
       </c>
-      <c r="B630" t="inlineStr">
+      <c r="B630" s="7" t="inlineStr">
         <is>
           <t>Monstera Adenossii</t>
+        </is>
+      </c>
+      <c r="D630" s="7" t="n">
+        <v>400</v>
+      </c>
+      <c r="E630" s="13" t="inlineStr">
+        <is>
+          <t>compo 1pw</t>
         </is>
       </c>
     </row>
@@ -10236,6 +10253,428 @@
       </c>
     </row>
     <row r="757"/>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>21.06.2025</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>21.06.2025</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Calathea Orbifolia</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>21.06.2025</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>21.06.2025</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>21.06.2025</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>21.06.2025</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>21.06.2025</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Coffea Arabica</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>21.06.2025</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>21.06.2025</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>21.06.2025</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Calathea Ornata</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>21.06.2025</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Beaucarnea recurvata</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>21.06.2025</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Nephrolepis obliterata</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>21.06.2025</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>21.06.2025</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+    </row>
+    <row r="772"/>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>22.06.2025</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr"/>
+      <c r="D773" t="inlineStr"/>
+      <c r="E773" t="inlineStr"/>
+      <c r="F773" t="inlineStr"/>
+      <c r="G773" t="inlineStr"/>
+      <c r="H773" t="inlineStr"/>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>22.06.2025</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Calathea Orbifolia</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr"/>
+      <c r="D774" t="inlineStr"/>
+      <c r="E774" t="inlineStr"/>
+      <c r="F774" t="inlineStr"/>
+      <c r="G774" t="inlineStr"/>
+      <c r="H774" t="inlineStr"/>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>22.06.2025</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr"/>
+      <c r="D775" t="inlineStr"/>
+      <c r="E775" t="inlineStr"/>
+      <c r="F775" t="inlineStr"/>
+      <c r="G775" t="inlineStr"/>
+      <c r="H775" t="inlineStr"/>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>22.06.2025</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr"/>
+      <c r="D776" t="inlineStr"/>
+      <c r="E776" t="inlineStr"/>
+      <c r="F776" t="inlineStr"/>
+      <c r="G776" t="inlineStr"/>
+      <c r="H776" t="inlineStr"/>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>22.06.2025</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr"/>
+      <c r="D777" t="inlineStr"/>
+      <c r="E777" t="inlineStr"/>
+      <c r="F777" t="inlineStr"/>
+      <c r="G777" t="inlineStr"/>
+      <c r="H777" t="inlineStr"/>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>22.06.2025</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr"/>
+      <c r="D778" t="inlineStr"/>
+      <c r="E778" t="inlineStr"/>
+      <c r="F778" t="inlineStr"/>
+      <c r="G778" t="inlineStr"/>
+      <c r="H778" t="inlineStr"/>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>22.06.2025</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Coffea Arabica</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr"/>
+      <c r="D779" t="inlineStr"/>
+      <c r="E779" t="inlineStr"/>
+      <c r="F779" t="inlineStr"/>
+      <c r="G779" t="inlineStr"/>
+      <c r="H779" t="inlineStr"/>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>22.06.2025</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr"/>
+      <c r="D780" t="inlineStr"/>
+      <c r="E780" t="inlineStr"/>
+      <c r="F780" t="inlineStr"/>
+      <c r="G780" t="inlineStr"/>
+      <c r="H780" t="inlineStr"/>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>22.06.2025</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr"/>
+      <c r="D781" t="inlineStr"/>
+      <c r="E781" t="inlineStr"/>
+      <c r="F781" t="inlineStr"/>
+      <c r="G781" t="inlineStr"/>
+      <c r="H781" t="inlineStr"/>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>22.06.2025</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Calathea Ornata</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr"/>
+      <c r="D782" t="inlineStr"/>
+      <c r="E782" t="inlineStr"/>
+      <c r="F782" t="inlineStr"/>
+      <c r="G782" t="inlineStr"/>
+      <c r="H782" t="inlineStr"/>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>22.06.2025</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Beaucarnea recurvata</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr"/>
+      <c r="D783" t="inlineStr"/>
+      <c r="E783" t="inlineStr"/>
+      <c r="F783" t="inlineStr"/>
+      <c r="G783" t="inlineStr"/>
+      <c r="H783" t="inlineStr"/>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>22.06.2025</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Nephrolepis obliterata</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr"/>
+      <c r="D784" t="inlineStr"/>
+      <c r="E784" t="inlineStr"/>
+      <c r="F784" t="inlineStr"/>
+      <c r="G784" t="inlineStr"/>
+      <c r="H784" t="inlineStr"/>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>22.06.2025</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr"/>
+      <c r="D785" t="inlineStr"/>
+      <c r="E785" t="inlineStr"/>
+      <c r="F785" t="inlineStr"/>
+      <c r="G785" t="inlineStr"/>
+      <c r="H785" t="inlineStr"/>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>22.06.2025</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr"/>
+      <c r="D786" t="inlineStr"/>
+      <c r="E786" t="inlineStr"/>
+      <c r="F786" t="inlineStr"/>
+      <c r="G786" t="inlineStr"/>
+      <c r="H786" t="inlineStr"/>
+    </row>
+    <row r="787"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed some unnesessary sql params
</commit_message>
<xml_diff>
--- a/data/blumen_data.xlsx
+++ b/data/blumen_data.xlsx
@@ -490,7 +490,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD2758"/>
+  <dimension ref="A1:AD2928"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1068" activePane="bottomLeft" state="frozen"/>
@@ -31699,13 +31699,6 @@
           <t>Calathea Medalion</t>
         </is>
       </c>
-      <c r="C2674" t="inlineStr"/>
-      <c r="D2674" t="inlineStr"/>
-      <c r="E2674" t="inlineStr"/>
-      <c r="F2674" t="inlineStr"/>
-      <c r="G2674" t="inlineStr"/>
-      <c r="H2674" t="inlineStr"/>
-      <c r="I2674" t="inlineStr"/>
     </row>
     <row r="2675">
       <c r="A2675" t="inlineStr">
@@ -31718,13 +31711,6 @@
           <t>Epipremnum Aureum</t>
         </is>
       </c>
-      <c r="C2675" t="inlineStr"/>
-      <c r="D2675" t="inlineStr"/>
-      <c r="E2675" t="inlineStr"/>
-      <c r="F2675" t="inlineStr"/>
-      <c r="G2675" t="inlineStr"/>
-      <c r="H2675" t="inlineStr"/>
-      <c r="I2675" t="inlineStr"/>
     </row>
     <row r="2676">
       <c r="A2676" t="inlineStr">
@@ -31737,13 +31723,6 @@
           <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
-      <c r="C2676" t="inlineStr"/>
-      <c r="D2676" t="inlineStr"/>
-      <c r="E2676" t="inlineStr"/>
-      <c r="F2676" t="inlineStr"/>
-      <c r="G2676" t="inlineStr"/>
-      <c r="H2676" t="inlineStr"/>
-      <c r="I2676" t="inlineStr"/>
     </row>
     <row r="2677">
       <c r="A2677" t="inlineStr">
@@ -31756,13 +31735,6 @@
           <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
-      <c r="C2677" t="inlineStr"/>
-      <c r="D2677" t="inlineStr"/>
-      <c r="E2677" t="inlineStr"/>
-      <c r="F2677" t="inlineStr"/>
-      <c r="G2677" t="inlineStr"/>
-      <c r="H2677" t="inlineStr"/>
-      <c r="I2677" t="inlineStr"/>
     </row>
     <row r="2678">
       <c r="A2678" t="inlineStr">
@@ -31775,13 +31747,6 @@
           <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
-      <c r="C2678" t="inlineStr"/>
-      <c r="D2678" t="inlineStr"/>
-      <c r="E2678" t="inlineStr"/>
-      <c r="F2678" t="inlineStr"/>
-      <c r="G2678" t="inlineStr"/>
-      <c r="H2678" t="inlineStr"/>
-      <c r="I2678" t="inlineStr"/>
     </row>
     <row r="2679">
       <c r="A2679" t="inlineStr">
@@ -31794,13 +31759,6 @@
           <t>Monstera Adenossii</t>
         </is>
       </c>
-      <c r="C2679" t="inlineStr"/>
-      <c r="D2679" t="inlineStr"/>
-      <c r="E2679" t="inlineStr"/>
-      <c r="F2679" t="inlineStr"/>
-      <c r="G2679" t="inlineStr"/>
-      <c r="H2679" t="inlineStr"/>
-      <c r="I2679" t="inlineStr"/>
     </row>
     <row r="2680">
       <c r="A2680" t="inlineStr">
@@ -31813,13 +31771,6 @@
           <t>Ficus Elastica Abidjan</t>
         </is>
       </c>
-      <c r="C2680" t="inlineStr"/>
-      <c r="D2680" t="inlineStr"/>
-      <c r="E2680" t="inlineStr"/>
-      <c r="F2680" t="inlineStr"/>
-      <c r="G2680" t="inlineStr"/>
-      <c r="H2680" t="inlineStr"/>
-      <c r="I2680" t="inlineStr"/>
     </row>
     <row r="2681">
       <c r="A2681" t="inlineStr">
@@ -31832,13 +31783,6 @@
           <t>Peperomia Hope</t>
         </is>
       </c>
-      <c r="C2681" t="inlineStr"/>
-      <c r="D2681" t="inlineStr"/>
-      <c r="E2681" t="inlineStr"/>
-      <c r="F2681" t="inlineStr"/>
-      <c r="G2681" t="inlineStr"/>
-      <c r="H2681" t="inlineStr"/>
-      <c r="I2681" t="inlineStr"/>
     </row>
     <row r="2682">
       <c r="A2682" t="inlineStr">
@@ -31851,13 +31795,6 @@
           <t>Hoya Mathilde</t>
         </is>
       </c>
-      <c r="C2682" t="inlineStr"/>
-      <c r="D2682" t="inlineStr"/>
-      <c r="E2682" t="inlineStr"/>
-      <c r="F2682" t="inlineStr"/>
-      <c r="G2682" t="inlineStr"/>
-      <c r="H2682" t="inlineStr"/>
-      <c r="I2682" t="inlineStr"/>
     </row>
     <row r="2683">
       <c r="A2683" t="inlineStr">
@@ -31870,13 +31807,6 @@
           <t>Epipremnum Pinnatum Blue</t>
         </is>
       </c>
-      <c r="C2683" t="inlineStr"/>
-      <c r="D2683" t="inlineStr"/>
-      <c r="E2683" t="inlineStr"/>
-      <c r="F2683" t="inlineStr"/>
-      <c r="G2683" t="inlineStr"/>
-      <c r="H2683" t="inlineStr"/>
-      <c r="I2683" t="inlineStr"/>
     </row>
     <row r="2684">
       <c r="A2684" t="inlineStr">
@@ -31889,13 +31819,6 @@
           <t>Sansevieria Laurentii</t>
         </is>
       </c>
-      <c r="C2684" t="inlineStr"/>
-      <c r="D2684" t="inlineStr"/>
-      <c r="E2684" t="inlineStr"/>
-      <c r="F2684" t="inlineStr"/>
-      <c r="G2684" t="inlineStr"/>
-      <c r="H2684" t="inlineStr"/>
-      <c r="I2684" t="inlineStr"/>
     </row>
     <row r="2685">
       <c r="A2685" t="inlineStr">
@@ -31908,13 +31831,6 @@
           <t>Epipremnum Aureum Saal</t>
         </is>
       </c>
-      <c r="C2685" t="inlineStr"/>
-      <c r="D2685" t="inlineStr"/>
-      <c r="E2685" t="inlineStr"/>
-      <c r="F2685" t="inlineStr"/>
-      <c r="G2685" t="inlineStr"/>
-      <c r="H2685" t="inlineStr"/>
-      <c r="I2685" t="inlineStr"/>
     </row>
     <row r="2686">
       <c r="A2686" t="inlineStr">
@@ -31927,13 +31843,6 @@
           <t>Monstera Deliciosa Variegata</t>
         </is>
       </c>
-      <c r="C2686" t="inlineStr"/>
-      <c r="D2686" t="inlineStr"/>
-      <c r="E2686" t="inlineStr"/>
-      <c r="F2686" t="inlineStr"/>
-      <c r="G2686" t="inlineStr"/>
-      <c r="H2686" t="inlineStr"/>
-      <c r="I2686" t="inlineStr"/>
     </row>
     <row r="2687">
       <c r="A2687" t="inlineStr">
@@ -31946,13 +31855,6 @@
           <t>Pachira Aquatica</t>
         </is>
       </c>
-      <c r="C2687" t="inlineStr"/>
-      <c r="D2687" t="inlineStr"/>
-      <c r="E2687" t="inlineStr"/>
-      <c r="F2687" t="inlineStr"/>
-      <c r="G2687" t="inlineStr"/>
-      <c r="H2687" t="inlineStr"/>
-      <c r="I2687" t="inlineStr"/>
     </row>
     <row r="2688">
       <c r="A2688" t="inlineStr">
@@ -31965,13 +31867,6 @@
           <t xml:space="preserve">Monstera Deliciosa </t>
         </is>
       </c>
-      <c r="C2688" t="inlineStr"/>
-      <c r="D2688" t="inlineStr"/>
-      <c r="E2688" t="inlineStr"/>
-      <c r="F2688" t="inlineStr"/>
-      <c r="G2688" t="inlineStr"/>
-      <c r="H2688" t="inlineStr"/>
-      <c r="I2688" t="inlineStr"/>
     </row>
     <row r="2689">
       <c r="A2689" t="inlineStr">
@@ -31984,13 +31879,6 @@
           <t>Philodendron Imperial Red</t>
         </is>
       </c>
-      <c r="C2689" t="inlineStr"/>
-      <c r="D2689" t="inlineStr"/>
-      <c r="E2689" t="inlineStr"/>
-      <c r="F2689" t="inlineStr"/>
-      <c r="G2689" t="inlineStr"/>
-      <c r="H2689" t="inlineStr"/>
-      <c r="I2689" t="inlineStr"/>
     </row>
     <row r="2690"/>
     <row r="2691">
@@ -32004,13 +31892,6 @@
           <t>Calathea Medalion</t>
         </is>
       </c>
-      <c r="C2691" t="inlineStr"/>
-      <c r="D2691" t="inlineStr"/>
-      <c r="E2691" t="inlineStr"/>
-      <c r="F2691" t="inlineStr"/>
-      <c r="G2691" t="inlineStr"/>
-      <c r="H2691" t="inlineStr"/>
-      <c r="I2691" t="inlineStr"/>
     </row>
     <row r="2692">
       <c r="A2692" t="inlineStr">
@@ -32023,13 +31904,6 @@
           <t>Epipremnum Aureum</t>
         </is>
       </c>
-      <c r="C2692" t="inlineStr"/>
-      <c r="D2692" t="inlineStr"/>
-      <c r="E2692" t="inlineStr"/>
-      <c r="F2692" t="inlineStr"/>
-      <c r="G2692" t="inlineStr"/>
-      <c r="H2692" t="inlineStr"/>
-      <c r="I2692" t="inlineStr"/>
     </row>
     <row r="2693">
       <c r="A2693" t="inlineStr">
@@ -32042,13 +31916,6 @@
           <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
-      <c r="C2693" t="inlineStr"/>
-      <c r="D2693" t="inlineStr"/>
-      <c r="E2693" t="inlineStr"/>
-      <c r="F2693" t="inlineStr"/>
-      <c r="G2693" t="inlineStr"/>
-      <c r="H2693" t="inlineStr"/>
-      <c r="I2693" t="inlineStr"/>
     </row>
     <row r="2694">
       <c r="A2694" t="inlineStr">
@@ -32061,13 +31928,6 @@
           <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
-      <c r="C2694" t="inlineStr"/>
-      <c r="D2694" t="inlineStr"/>
-      <c r="E2694" t="inlineStr"/>
-      <c r="F2694" t="inlineStr"/>
-      <c r="G2694" t="inlineStr"/>
-      <c r="H2694" t="inlineStr"/>
-      <c r="I2694" t="inlineStr"/>
     </row>
     <row r="2695">
       <c r="A2695" t="inlineStr">
@@ -32080,13 +31940,6 @@
           <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
-      <c r="C2695" t="inlineStr"/>
-      <c r="D2695" t="inlineStr"/>
-      <c r="E2695" t="inlineStr"/>
-      <c r="F2695" t="inlineStr"/>
-      <c r="G2695" t="inlineStr"/>
-      <c r="H2695" t="inlineStr"/>
-      <c r="I2695" t="inlineStr"/>
     </row>
     <row r="2696">
       <c r="A2696" t="inlineStr">
@@ -32099,13 +31952,6 @@
           <t>Monstera Adenossii</t>
         </is>
       </c>
-      <c r="C2696" t="inlineStr"/>
-      <c r="D2696" t="inlineStr"/>
-      <c r="E2696" t="inlineStr"/>
-      <c r="F2696" t="inlineStr"/>
-      <c r="G2696" t="inlineStr"/>
-      <c r="H2696" t="inlineStr"/>
-      <c r="I2696" t="inlineStr"/>
     </row>
     <row r="2697">
       <c r="A2697" t="inlineStr">
@@ -32118,13 +31964,6 @@
           <t>Ficus Elastica Abidjan</t>
         </is>
       </c>
-      <c r="C2697" t="inlineStr"/>
-      <c r="D2697" t="inlineStr"/>
-      <c r="E2697" t="inlineStr"/>
-      <c r="F2697" t="inlineStr"/>
-      <c r="G2697" t="inlineStr"/>
-      <c r="H2697" t="inlineStr"/>
-      <c r="I2697" t="inlineStr"/>
     </row>
     <row r="2698">
       <c r="A2698" t="inlineStr">
@@ -32137,13 +31976,6 @@
           <t>Peperomia Hope</t>
         </is>
       </c>
-      <c r="C2698" t="inlineStr"/>
-      <c r="D2698" t="inlineStr"/>
-      <c r="E2698" t="inlineStr"/>
-      <c r="F2698" t="inlineStr"/>
-      <c r="G2698" t="inlineStr"/>
-      <c r="H2698" t="inlineStr"/>
-      <c r="I2698" t="inlineStr"/>
     </row>
     <row r="2699">
       <c r="A2699" t="inlineStr">
@@ -32156,13 +31988,6 @@
           <t>Hoya Mathilde</t>
         </is>
       </c>
-      <c r="C2699" t="inlineStr"/>
-      <c r="D2699" t="inlineStr"/>
-      <c r="E2699" t="inlineStr"/>
-      <c r="F2699" t="inlineStr"/>
-      <c r="G2699" t="inlineStr"/>
-      <c r="H2699" t="inlineStr"/>
-      <c r="I2699" t="inlineStr"/>
     </row>
     <row r="2700">
       <c r="A2700" t="inlineStr">
@@ -32175,13 +32000,6 @@
           <t>Epipremnum Pinnatum Blue</t>
         </is>
       </c>
-      <c r="C2700" t="inlineStr"/>
-      <c r="D2700" t="inlineStr"/>
-      <c r="E2700" t="inlineStr"/>
-      <c r="F2700" t="inlineStr"/>
-      <c r="G2700" t="inlineStr"/>
-      <c r="H2700" t="inlineStr"/>
-      <c r="I2700" t="inlineStr"/>
     </row>
     <row r="2701">
       <c r="A2701" t="inlineStr">
@@ -32194,13 +32012,6 @@
           <t>Sansevieria Laurentii</t>
         </is>
       </c>
-      <c r="C2701" t="inlineStr"/>
-      <c r="D2701" t="inlineStr"/>
-      <c r="E2701" t="inlineStr"/>
-      <c r="F2701" t="inlineStr"/>
-      <c r="G2701" t="inlineStr"/>
-      <c r="H2701" t="inlineStr"/>
-      <c r="I2701" t="inlineStr"/>
     </row>
     <row r="2702">
       <c r="A2702" t="inlineStr">
@@ -32213,13 +32024,6 @@
           <t>Epipremnum Aureum Saal</t>
         </is>
       </c>
-      <c r="C2702" t="inlineStr"/>
-      <c r="D2702" t="inlineStr"/>
-      <c r="E2702" t="inlineStr"/>
-      <c r="F2702" t="inlineStr"/>
-      <c r="G2702" t="inlineStr"/>
-      <c r="H2702" t="inlineStr"/>
-      <c r="I2702" t="inlineStr"/>
     </row>
     <row r="2703">
       <c r="A2703" t="inlineStr">
@@ -32232,13 +32036,6 @@
           <t>Monstera Deliciosa Variegata</t>
         </is>
       </c>
-      <c r="C2703" t="inlineStr"/>
-      <c r="D2703" t="inlineStr"/>
-      <c r="E2703" t="inlineStr"/>
-      <c r="F2703" t="inlineStr"/>
-      <c r="G2703" t="inlineStr"/>
-      <c r="H2703" t="inlineStr"/>
-      <c r="I2703" t="inlineStr"/>
     </row>
     <row r="2704">
       <c r="A2704" t="inlineStr">
@@ -32251,13 +32048,6 @@
           <t>Pachira Aquatica</t>
         </is>
       </c>
-      <c r="C2704" t="inlineStr"/>
-      <c r="D2704" t="inlineStr"/>
-      <c r="E2704" t="inlineStr"/>
-      <c r="F2704" t="inlineStr"/>
-      <c r="G2704" t="inlineStr"/>
-      <c r="H2704" t="inlineStr"/>
-      <c r="I2704" t="inlineStr"/>
     </row>
     <row r="2705">
       <c r="A2705" t="inlineStr">
@@ -32270,13 +32060,6 @@
           <t xml:space="preserve">Monstera Deliciosa </t>
         </is>
       </c>
-      <c r="C2705" t="inlineStr"/>
-      <c r="D2705" t="inlineStr"/>
-      <c r="E2705" t="inlineStr"/>
-      <c r="F2705" t="inlineStr"/>
-      <c r="G2705" t="inlineStr"/>
-      <c r="H2705" t="inlineStr"/>
-      <c r="I2705" t="inlineStr"/>
     </row>
     <row r="2706">
       <c r="A2706" t="inlineStr">
@@ -32289,13 +32072,6 @@
           <t>Philodendron Imperial Red</t>
         </is>
       </c>
-      <c r="C2706" t="inlineStr"/>
-      <c r="D2706" t="inlineStr"/>
-      <c r="E2706" t="inlineStr"/>
-      <c r="F2706" t="inlineStr"/>
-      <c r="G2706" t="inlineStr"/>
-      <c r="H2706" t="inlineStr"/>
-      <c r="I2706" t="inlineStr"/>
     </row>
     <row r="2707"/>
     <row r="2708">
@@ -32309,13 +32085,6 @@
           <t>Calathea Medalion</t>
         </is>
       </c>
-      <c r="C2708" t="inlineStr"/>
-      <c r="D2708" t="inlineStr"/>
-      <c r="E2708" t="inlineStr"/>
-      <c r="F2708" t="inlineStr"/>
-      <c r="G2708" t="inlineStr"/>
-      <c r="H2708" t="inlineStr"/>
-      <c r="I2708" t="inlineStr"/>
     </row>
     <row r="2709">
       <c r="A2709" t="inlineStr">
@@ -32328,13 +32097,6 @@
           <t>Epipremnum Aureum</t>
         </is>
       </c>
-      <c r="C2709" t="inlineStr"/>
-      <c r="D2709" t="inlineStr"/>
-      <c r="E2709" t="inlineStr"/>
-      <c r="F2709" t="inlineStr"/>
-      <c r="G2709" t="inlineStr"/>
-      <c r="H2709" t="inlineStr"/>
-      <c r="I2709" t="inlineStr"/>
     </row>
     <row r="2710">
       <c r="A2710" t="inlineStr">
@@ -32347,13 +32109,6 @@
           <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
-      <c r="C2710" t="inlineStr"/>
-      <c r="D2710" t="inlineStr"/>
-      <c r="E2710" t="inlineStr"/>
-      <c r="F2710" t="inlineStr"/>
-      <c r="G2710" t="inlineStr"/>
-      <c r="H2710" t="inlineStr"/>
-      <c r="I2710" t="inlineStr"/>
     </row>
     <row r="2711">
       <c r="A2711" t="inlineStr">
@@ -32366,13 +32121,6 @@
           <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
-      <c r="C2711" t="inlineStr"/>
-      <c r="D2711" t="inlineStr"/>
-      <c r="E2711" t="inlineStr"/>
-      <c r="F2711" t="inlineStr"/>
-      <c r="G2711" t="inlineStr"/>
-      <c r="H2711" t="inlineStr"/>
-      <c r="I2711" t="inlineStr"/>
     </row>
     <row r="2712">
       <c r="A2712" t="inlineStr">
@@ -32385,13 +32133,6 @@
           <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
-      <c r="C2712" t="inlineStr"/>
-      <c r="D2712" t="inlineStr"/>
-      <c r="E2712" t="inlineStr"/>
-      <c r="F2712" t="inlineStr"/>
-      <c r="G2712" t="inlineStr"/>
-      <c r="H2712" t="inlineStr"/>
-      <c r="I2712" t="inlineStr"/>
     </row>
     <row r="2713">
       <c r="A2713" t="inlineStr">
@@ -32404,13 +32145,6 @@
           <t>Monstera Adenossii</t>
         </is>
       </c>
-      <c r="C2713" t="inlineStr"/>
-      <c r="D2713" t="inlineStr"/>
-      <c r="E2713" t="inlineStr"/>
-      <c r="F2713" t="inlineStr"/>
-      <c r="G2713" t="inlineStr"/>
-      <c r="H2713" t="inlineStr"/>
-      <c r="I2713" t="inlineStr"/>
     </row>
     <row r="2714">
       <c r="A2714" t="inlineStr">
@@ -32423,13 +32157,6 @@
           <t>Ficus Elastica Abidjan</t>
         </is>
       </c>
-      <c r="C2714" t="inlineStr"/>
-      <c r="D2714" t="inlineStr"/>
-      <c r="E2714" t="inlineStr"/>
-      <c r="F2714" t="inlineStr"/>
-      <c r="G2714" t="inlineStr"/>
-      <c r="H2714" t="inlineStr"/>
-      <c r="I2714" t="inlineStr"/>
     </row>
     <row r="2715">
       <c r="A2715" t="inlineStr">
@@ -32442,13 +32169,6 @@
           <t>Peperomia Hope</t>
         </is>
       </c>
-      <c r="C2715" t="inlineStr"/>
-      <c r="D2715" t="inlineStr"/>
-      <c r="E2715" t="inlineStr"/>
-      <c r="F2715" t="inlineStr"/>
-      <c r="G2715" t="inlineStr"/>
-      <c r="H2715" t="inlineStr"/>
-      <c r="I2715" t="inlineStr"/>
     </row>
     <row r="2716">
       <c r="A2716" t="inlineStr">
@@ -32461,13 +32181,6 @@
           <t>Hoya Mathilde</t>
         </is>
       </c>
-      <c r="C2716" t="inlineStr"/>
-      <c r="D2716" t="inlineStr"/>
-      <c r="E2716" t="inlineStr"/>
-      <c r="F2716" t="inlineStr"/>
-      <c r="G2716" t="inlineStr"/>
-      <c r="H2716" t="inlineStr"/>
-      <c r="I2716" t="inlineStr"/>
     </row>
     <row r="2717">
       <c r="A2717" t="inlineStr">
@@ -32480,13 +32193,6 @@
           <t>Epipremnum Pinnatum Blue</t>
         </is>
       </c>
-      <c r="C2717" t="inlineStr"/>
-      <c r="D2717" t="inlineStr"/>
-      <c r="E2717" t="inlineStr"/>
-      <c r="F2717" t="inlineStr"/>
-      <c r="G2717" t="inlineStr"/>
-      <c r="H2717" t="inlineStr"/>
-      <c r="I2717" t="inlineStr"/>
     </row>
     <row r="2718">
       <c r="A2718" t="inlineStr">
@@ -32499,13 +32205,6 @@
           <t>Sansevieria Laurentii</t>
         </is>
       </c>
-      <c r="C2718" t="inlineStr"/>
-      <c r="D2718" t="inlineStr"/>
-      <c r="E2718" t="inlineStr"/>
-      <c r="F2718" t="inlineStr"/>
-      <c r="G2718" t="inlineStr"/>
-      <c r="H2718" t="inlineStr"/>
-      <c r="I2718" t="inlineStr"/>
     </row>
     <row r="2719">
       <c r="A2719" t="inlineStr">
@@ -32518,13 +32217,6 @@
           <t>Epipremnum Aureum Saal</t>
         </is>
       </c>
-      <c r="C2719" t="inlineStr"/>
-      <c r="D2719" t="inlineStr"/>
-      <c r="E2719" t="inlineStr"/>
-      <c r="F2719" t="inlineStr"/>
-      <c r="G2719" t="inlineStr"/>
-      <c r="H2719" t="inlineStr"/>
-      <c r="I2719" t="inlineStr"/>
     </row>
     <row r="2720">
       <c r="A2720" t="inlineStr">
@@ -32537,13 +32229,6 @@
           <t>Monstera Deliciosa Variegata</t>
         </is>
       </c>
-      <c r="C2720" t="inlineStr"/>
-      <c r="D2720" t="inlineStr"/>
-      <c r="E2720" t="inlineStr"/>
-      <c r="F2720" t="inlineStr"/>
-      <c r="G2720" t="inlineStr"/>
-      <c r="H2720" t="inlineStr"/>
-      <c r="I2720" t="inlineStr"/>
     </row>
     <row r="2721">
       <c r="A2721" t="inlineStr">
@@ -32556,13 +32241,6 @@
           <t>Pachira Aquatica</t>
         </is>
       </c>
-      <c r="C2721" t="inlineStr"/>
-      <c r="D2721" t="inlineStr"/>
-      <c r="E2721" t="inlineStr"/>
-      <c r="F2721" t="inlineStr"/>
-      <c r="G2721" t="inlineStr"/>
-      <c r="H2721" t="inlineStr"/>
-      <c r="I2721" t="inlineStr"/>
     </row>
     <row r="2722">
       <c r="A2722" t="inlineStr">
@@ -32575,13 +32253,6 @@
           <t xml:space="preserve">Monstera Deliciosa </t>
         </is>
       </c>
-      <c r="C2722" t="inlineStr"/>
-      <c r="D2722" t="inlineStr"/>
-      <c r="E2722" t="inlineStr"/>
-      <c r="F2722" t="inlineStr"/>
-      <c r="G2722" t="inlineStr"/>
-      <c r="H2722" t="inlineStr"/>
-      <c r="I2722" t="inlineStr"/>
     </row>
     <row r="2723">
       <c r="A2723" t="inlineStr">
@@ -32594,13 +32265,6 @@
           <t>Philodendron Imperial Red</t>
         </is>
       </c>
-      <c r="C2723" t="inlineStr"/>
-      <c r="D2723" t="inlineStr"/>
-      <c r="E2723" t="inlineStr"/>
-      <c r="F2723" t="inlineStr"/>
-      <c r="G2723" t="inlineStr"/>
-      <c r="H2723" t="inlineStr"/>
-      <c r="I2723" t="inlineStr"/>
     </row>
     <row r="2724"/>
     <row r="2725">
@@ -32614,13 +32278,6 @@
           <t>Calathea Medalion</t>
         </is>
       </c>
-      <c r="C2725" t="inlineStr"/>
-      <c r="D2725" t="inlineStr"/>
-      <c r="E2725" t="inlineStr"/>
-      <c r="F2725" t="inlineStr"/>
-      <c r="G2725" t="inlineStr"/>
-      <c r="H2725" t="inlineStr"/>
-      <c r="I2725" t="inlineStr"/>
     </row>
     <row r="2726">
       <c r="A2726" t="inlineStr">
@@ -32633,13 +32290,6 @@
           <t>Epipremnum Aureum</t>
         </is>
       </c>
-      <c r="C2726" t="inlineStr"/>
-      <c r="D2726" t="inlineStr"/>
-      <c r="E2726" t="inlineStr"/>
-      <c r="F2726" t="inlineStr"/>
-      <c r="G2726" t="inlineStr"/>
-      <c r="H2726" t="inlineStr"/>
-      <c r="I2726" t="inlineStr"/>
     </row>
     <row r="2727">
       <c r="A2727" t="inlineStr">
@@ -32652,13 +32302,6 @@
           <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
-      <c r="C2727" t="inlineStr"/>
-      <c r="D2727" t="inlineStr"/>
-      <c r="E2727" t="inlineStr"/>
-      <c r="F2727" t="inlineStr"/>
-      <c r="G2727" t="inlineStr"/>
-      <c r="H2727" t="inlineStr"/>
-      <c r="I2727" t="inlineStr"/>
     </row>
     <row r="2728">
       <c r="A2728" t="inlineStr">
@@ -32671,13 +32314,6 @@
           <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
-      <c r="C2728" t="inlineStr"/>
-      <c r="D2728" t="inlineStr"/>
-      <c r="E2728" t="inlineStr"/>
-      <c r="F2728" t="inlineStr"/>
-      <c r="G2728" t="inlineStr"/>
-      <c r="H2728" t="inlineStr"/>
-      <c r="I2728" t="inlineStr"/>
     </row>
     <row r="2729">
       <c r="A2729" t="inlineStr">
@@ -32690,13 +32326,6 @@
           <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
-      <c r="C2729" t="inlineStr"/>
-      <c r="D2729" t="inlineStr"/>
-      <c r="E2729" t="inlineStr"/>
-      <c r="F2729" t="inlineStr"/>
-      <c r="G2729" t="inlineStr"/>
-      <c r="H2729" t="inlineStr"/>
-      <c r="I2729" t="inlineStr"/>
     </row>
     <row r="2730">
       <c r="A2730" t="inlineStr">
@@ -32709,13 +32338,6 @@
           <t>Monstera Adenossii</t>
         </is>
       </c>
-      <c r="C2730" t="inlineStr"/>
-      <c r="D2730" t="inlineStr"/>
-      <c r="E2730" t="inlineStr"/>
-      <c r="F2730" t="inlineStr"/>
-      <c r="G2730" t="inlineStr"/>
-      <c r="H2730" t="inlineStr"/>
-      <c r="I2730" t="inlineStr"/>
     </row>
     <row r="2731">
       <c r="A2731" t="inlineStr">
@@ -32728,13 +32350,6 @@
           <t>Ficus Elastica Abidjan</t>
         </is>
       </c>
-      <c r="C2731" t="inlineStr"/>
-      <c r="D2731" t="inlineStr"/>
-      <c r="E2731" t="inlineStr"/>
-      <c r="F2731" t="inlineStr"/>
-      <c r="G2731" t="inlineStr"/>
-      <c r="H2731" t="inlineStr"/>
-      <c r="I2731" t="inlineStr"/>
     </row>
     <row r="2732">
       <c r="A2732" t="inlineStr">
@@ -32747,13 +32362,6 @@
           <t>Peperomia Hope</t>
         </is>
       </c>
-      <c r="C2732" t="inlineStr"/>
-      <c r="D2732" t="inlineStr"/>
-      <c r="E2732" t="inlineStr"/>
-      <c r="F2732" t="inlineStr"/>
-      <c r="G2732" t="inlineStr"/>
-      <c r="H2732" t="inlineStr"/>
-      <c r="I2732" t="inlineStr"/>
     </row>
     <row r="2733">
       <c r="A2733" t="inlineStr">
@@ -32766,13 +32374,6 @@
           <t>Hoya Mathilde</t>
         </is>
       </c>
-      <c r="C2733" t="inlineStr"/>
-      <c r="D2733" t="inlineStr"/>
-      <c r="E2733" t="inlineStr"/>
-      <c r="F2733" t="inlineStr"/>
-      <c r="G2733" t="inlineStr"/>
-      <c r="H2733" t="inlineStr"/>
-      <c r="I2733" t="inlineStr"/>
     </row>
     <row r="2734">
       <c r="A2734" t="inlineStr">
@@ -32785,13 +32386,6 @@
           <t>Epipremnum Pinnatum Blue</t>
         </is>
       </c>
-      <c r="C2734" t="inlineStr"/>
-      <c r="D2734" t="inlineStr"/>
-      <c r="E2734" t="inlineStr"/>
-      <c r="F2734" t="inlineStr"/>
-      <c r="G2734" t="inlineStr"/>
-      <c r="H2734" t="inlineStr"/>
-      <c r="I2734" t="inlineStr"/>
     </row>
     <row r="2735">
       <c r="A2735" t="inlineStr">
@@ -32804,13 +32398,6 @@
           <t>Sansevieria Laurentii</t>
         </is>
       </c>
-      <c r="C2735" t="inlineStr"/>
-      <c r="D2735" t="inlineStr"/>
-      <c r="E2735" t="inlineStr"/>
-      <c r="F2735" t="inlineStr"/>
-      <c r="G2735" t="inlineStr"/>
-      <c r="H2735" t="inlineStr"/>
-      <c r="I2735" t="inlineStr"/>
     </row>
     <row r="2736">
       <c r="A2736" t="inlineStr">
@@ -32823,13 +32410,6 @@
           <t>Epipremnum Aureum Saal</t>
         </is>
       </c>
-      <c r="C2736" t="inlineStr"/>
-      <c r="D2736" t="inlineStr"/>
-      <c r="E2736" t="inlineStr"/>
-      <c r="F2736" t="inlineStr"/>
-      <c r="G2736" t="inlineStr"/>
-      <c r="H2736" t="inlineStr"/>
-      <c r="I2736" t="inlineStr"/>
     </row>
     <row r="2737">
       <c r="A2737" t="inlineStr">
@@ -32842,13 +32422,6 @@
           <t>Monstera Deliciosa Variegata</t>
         </is>
       </c>
-      <c r="C2737" t="inlineStr"/>
-      <c r="D2737" t="inlineStr"/>
-      <c r="E2737" t="inlineStr"/>
-      <c r="F2737" t="inlineStr"/>
-      <c r="G2737" t="inlineStr"/>
-      <c r="H2737" t="inlineStr"/>
-      <c r="I2737" t="inlineStr"/>
     </row>
     <row r="2738">
       <c r="A2738" t="inlineStr">
@@ -32861,13 +32434,6 @@
           <t>Pachira Aquatica</t>
         </is>
       </c>
-      <c r="C2738" t="inlineStr"/>
-      <c r="D2738" t="inlineStr"/>
-      <c r="E2738" t="inlineStr"/>
-      <c r="F2738" t="inlineStr"/>
-      <c r="G2738" t="inlineStr"/>
-      <c r="H2738" t="inlineStr"/>
-      <c r="I2738" t="inlineStr"/>
     </row>
     <row r="2739">
       <c r="A2739" t="inlineStr">
@@ -32880,13 +32446,6 @@
           <t xml:space="preserve">Monstera Deliciosa </t>
         </is>
       </c>
-      <c r="C2739" t="inlineStr"/>
-      <c r="D2739" t="inlineStr"/>
-      <c r="E2739" t="inlineStr"/>
-      <c r="F2739" t="inlineStr"/>
-      <c r="G2739" t="inlineStr"/>
-      <c r="H2739" t="inlineStr"/>
-      <c r="I2739" t="inlineStr"/>
     </row>
     <row r="2740">
       <c r="A2740" t="inlineStr">
@@ -32899,13 +32458,6 @@
           <t>Philodendron Imperial Red</t>
         </is>
       </c>
-      <c r="C2740" t="inlineStr"/>
-      <c r="D2740" t="inlineStr"/>
-      <c r="E2740" t="inlineStr"/>
-      <c r="F2740" t="inlineStr"/>
-      <c r="G2740" t="inlineStr"/>
-      <c r="H2740" t="inlineStr"/>
-      <c r="I2740" t="inlineStr"/>
     </row>
     <row r="2741"/>
     <row r="2742">
@@ -32919,13 +32471,6 @@
           <t>Calathea Medalion</t>
         </is>
       </c>
-      <c r="C2742" t="inlineStr"/>
-      <c r="D2742" t="inlineStr"/>
-      <c r="E2742" t="inlineStr"/>
-      <c r="F2742" t="inlineStr"/>
-      <c r="G2742" t="inlineStr"/>
-      <c r="H2742" t="inlineStr"/>
-      <c r="I2742" t="inlineStr"/>
     </row>
     <row r="2743">
       <c r="A2743" t="inlineStr">
@@ -32938,13 +32483,6 @@
           <t>Epipremnum Aureum</t>
         </is>
       </c>
-      <c r="C2743" t="inlineStr"/>
-      <c r="D2743" t="inlineStr"/>
-      <c r="E2743" t="inlineStr"/>
-      <c r="F2743" t="inlineStr"/>
-      <c r="G2743" t="inlineStr"/>
-      <c r="H2743" t="inlineStr"/>
-      <c r="I2743" t="inlineStr"/>
     </row>
     <row r="2744">
       <c r="A2744" t="inlineStr">
@@ -32957,13 +32495,6 @@
           <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
-      <c r="C2744" t="inlineStr"/>
-      <c r="D2744" t="inlineStr"/>
-      <c r="E2744" t="inlineStr"/>
-      <c r="F2744" t="inlineStr"/>
-      <c r="G2744" t="inlineStr"/>
-      <c r="H2744" t="inlineStr"/>
-      <c r="I2744" t="inlineStr"/>
     </row>
     <row r="2745">
       <c r="A2745" t="inlineStr">
@@ -32976,13 +32507,6 @@
           <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
-      <c r="C2745" t="inlineStr"/>
-      <c r="D2745" t="inlineStr"/>
-      <c r="E2745" t="inlineStr"/>
-      <c r="F2745" t="inlineStr"/>
-      <c r="G2745" t="inlineStr"/>
-      <c r="H2745" t="inlineStr"/>
-      <c r="I2745" t="inlineStr"/>
     </row>
     <row r="2746">
       <c r="A2746" t="inlineStr">
@@ -32995,13 +32519,6 @@
           <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
-      <c r="C2746" t="inlineStr"/>
-      <c r="D2746" t="inlineStr"/>
-      <c r="E2746" t="inlineStr"/>
-      <c r="F2746" t="inlineStr"/>
-      <c r="G2746" t="inlineStr"/>
-      <c r="H2746" t="inlineStr"/>
-      <c r="I2746" t="inlineStr"/>
     </row>
     <row r="2747">
       <c r="A2747" t="inlineStr">
@@ -33014,13 +32531,6 @@
           <t>Monstera Adenossii</t>
         </is>
       </c>
-      <c r="C2747" t="inlineStr"/>
-      <c r="D2747" t="inlineStr"/>
-      <c r="E2747" t="inlineStr"/>
-      <c r="F2747" t="inlineStr"/>
-      <c r="G2747" t="inlineStr"/>
-      <c r="H2747" t="inlineStr"/>
-      <c r="I2747" t="inlineStr"/>
     </row>
     <row r="2748">
       <c r="A2748" t="inlineStr">
@@ -33033,13 +32543,6 @@
           <t>Ficus Elastica Abidjan</t>
         </is>
       </c>
-      <c r="C2748" t="inlineStr"/>
-      <c r="D2748" t="inlineStr"/>
-      <c r="E2748" t="inlineStr"/>
-      <c r="F2748" t="inlineStr"/>
-      <c r="G2748" t="inlineStr"/>
-      <c r="H2748" t="inlineStr"/>
-      <c r="I2748" t="inlineStr"/>
     </row>
     <row r="2749">
       <c r="A2749" t="inlineStr">
@@ -33052,13 +32555,6 @@
           <t>Peperomia Hope</t>
         </is>
       </c>
-      <c r="C2749" t="inlineStr"/>
-      <c r="D2749" t="inlineStr"/>
-      <c r="E2749" t="inlineStr"/>
-      <c r="F2749" t="inlineStr"/>
-      <c r="G2749" t="inlineStr"/>
-      <c r="H2749" t="inlineStr"/>
-      <c r="I2749" t="inlineStr"/>
     </row>
     <row r="2750">
       <c r="A2750" t="inlineStr">
@@ -33071,13 +32567,6 @@
           <t>Hoya Mathilde</t>
         </is>
       </c>
-      <c r="C2750" t="inlineStr"/>
-      <c r="D2750" t="inlineStr"/>
-      <c r="E2750" t="inlineStr"/>
-      <c r="F2750" t="inlineStr"/>
-      <c r="G2750" t="inlineStr"/>
-      <c r="H2750" t="inlineStr"/>
-      <c r="I2750" t="inlineStr"/>
     </row>
     <row r="2751">
       <c r="A2751" t="inlineStr">
@@ -33090,13 +32579,6 @@
           <t>Epipremnum Pinnatum Blue</t>
         </is>
       </c>
-      <c r="C2751" t="inlineStr"/>
-      <c r="D2751" t="inlineStr"/>
-      <c r="E2751" t="inlineStr"/>
-      <c r="F2751" t="inlineStr"/>
-      <c r="G2751" t="inlineStr"/>
-      <c r="H2751" t="inlineStr"/>
-      <c r="I2751" t="inlineStr"/>
     </row>
     <row r="2752">
       <c r="A2752" t="inlineStr">
@@ -33109,13 +32591,6 @@
           <t>Sansevieria Laurentii</t>
         </is>
       </c>
-      <c r="C2752" t="inlineStr"/>
-      <c r="D2752" t="inlineStr"/>
-      <c r="E2752" t="inlineStr"/>
-      <c r="F2752" t="inlineStr"/>
-      <c r="G2752" t="inlineStr"/>
-      <c r="H2752" t="inlineStr"/>
-      <c r="I2752" t="inlineStr"/>
     </row>
     <row r="2753">
       <c r="A2753" t="inlineStr">
@@ -33128,13 +32603,6 @@
           <t>Epipremnum Aureum Saal</t>
         </is>
       </c>
-      <c r="C2753" t="inlineStr"/>
-      <c r="D2753" t="inlineStr"/>
-      <c r="E2753" t="inlineStr"/>
-      <c r="F2753" t="inlineStr"/>
-      <c r="G2753" t="inlineStr"/>
-      <c r="H2753" t="inlineStr"/>
-      <c r="I2753" t="inlineStr"/>
     </row>
     <row r="2754">
       <c r="A2754" t="inlineStr">
@@ -33147,13 +32615,6 @@
           <t>Monstera Deliciosa Variegata</t>
         </is>
       </c>
-      <c r="C2754" t="inlineStr"/>
-      <c r="D2754" t="inlineStr"/>
-      <c r="E2754" t="inlineStr"/>
-      <c r="F2754" t="inlineStr"/>
-      <c r="G2754" t="inlineStr"/>
-      <c r="H2754" t="inlineStr"/>
-      <c r="I2754" t="inlineStr"/>
     </row>
     <row r="2755">
       <c r="A2755" t="inlineStr">
@@ -33166,13 +32627,6 @@
           <t>Pachira Aquatica</t>
         </is>
       </c>
-      <c r="C2755" t="inlineStr"/>
-      <c r="D2755" t="inlineStr"/>
-      <c r="E2755" t="inlineStr"/>
-      <c r="F2755" t="inlineStr"/>
-      <c r="G2755" t="inlineStr"/>
-      <c r="H2755" t="inlineStr"/>
-      <c r="I2755" t="inlineStr"/>
     </row>
     <row r="2756">
       <c r="A2756" t="inlineStr">
@@ -33185,13 +32639,6 @@
           <t xml:space="preserve">Monstera Deliciosa </t>
         </is>
       </c>
-      <c r="C2756" t="inlineStr"/>
-      <c r="D2756" t="inlineStr"/>
-      <c r="E2756" t="inlineStr"/>
-      <c r="F2756" t="inlineStr"/>
-      <c r="G2756" t="inlineStr"/>
-      <c r="H2756" t="inlineStr"/>
-      <c r="I2756" t="inlineStr"/>
     </row>
     <row r="2757">
       <c r="A2757" t="inlineStr">
@@ -33204,15 +32651,2498 @@
           <t>Philodendron Imperial Red</t>
         </is>
       </c>
-      <c r="C2757" t="inlineStr"/>
-      <c r="D2757" t="inlineStr"/>
-      <c r="E2757" t="inlineStr"/>
-      <c r="F2757" t="inlineStr"/>
-      <c r="G2757" t="inlineStr"/>
-      <c r="H2757" t="inlineStr"/>
-      <c r="I2757" t="inlineStr"/>
     </row>
     <row r="2758"/>
+    <row r="2759">
+      <c r="A2759" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2759" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+    </row>
+    <row r="2760">
+      <c r="A2760" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2760" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+    </row>
+    <row r="2761">
+      <c r="A2761" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2761" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+    </row>
+    <row r="2762">
+      <c r="A2762" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2762" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+    </row>
+    <row r="2763">
+      <c r="A2763" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2763" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+    </row>
+    <row r="2764">
+      <c r="A2764" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2764" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+    </row>
+    <row r="2765">
+      <c r="A2765" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2765" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+    </row>
+    <row r="2766">
+      <c r="A2766" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2766" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+    </row>
+    <row r="2767">
+      <c r="A2767" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2767" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+    </row>
+    <row r="2768">
+      <c r="A2768" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2768" t="inlineStr">
+        <is>
+          <t>Epipremnum Pinnatum Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="2769">
+      <c r="A2769" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2769" t="inlineStr">
+        <is>
+          <t>Sansevieria Laurentii</t>
+        </is>
+      </c>
+    </row>
+    <row r="2770">
+      <c r="A2770" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2770" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum Saal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2771">
+      <c r="A2771" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2771" t="inlineStr">
+        <is>
+          <t>Monstera Deliciosa Variegata</t>
+        </is>
+      </c>
+    </row>
+    <row r="2772">
+      <c r="A2772" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2772" t="inlineStr">
+        <is>
+          <t>Pachira Aquatica</t>
+        </is>
+      </c>
+    </row>
+    <row r="2773">
+      <c r="A2773" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2773" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monstera Deliciosa </t>
+        </is>
+      </c>
+    </row>
+    <row r="2774">
+      <c r="A2774" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2774" t="inlineStr">
+        <is>
+          <t>Philodendron Imperial Red</t>
+        </is>
+      </c>
+    </row>
+    <row r="2775"/>
+    <row r="2776">
+      <c r="A2776" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2776" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+    </row>
+    <row r="2777">
+      <c r="A2777" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2777" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+    </row>
+    <row r="2778">
+      <c r="A2778" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2778" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+    </row>
+    <row r="2779">
+      <c r="A2779" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2779" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+    </row>
+    <row r="2780">
+      <c r="A2780" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2780" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+    </row>
+    <row r="2781">
+      <c r="A2781" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2781" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+    </row>
+    <row r="2782">
+      <c r="A2782" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2782" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+    </row>
+    <row r="2783">
+      <c r="A2783" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2783" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+    </row>
+    <row r="2784">
+      <c r="A2784" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2784" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+    </row>
+    <row r="2785">
+      <c r="A2785" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2785" t="inlineStr">
+        <is>
+          <t>Epipremnum Pinnatum Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="2786">
+      <c r="A2786" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2786" t="inlineStr">
+        <is>
+          <t>Sansevieria Laurentii</t>
+        </is>
+      </c>
+    </row>
+    <row r="2787">
+      <c r="A2787" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2787" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum Saal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2788">
+      <c r="A2788" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2788" t="inlineStr">
+        <is>
+          <t>Monstera Deliciosa Variegata</t>
+        </is>
+      </c>
+    </row>
+    <row r="2789">
+      <c r="A2789" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2789" t="inlineStr">
+        <is>
+          <t>Pachira Aquatica</t>
+        </is>
+      </c>
+    </row>
+    <row r="2790">
+      <c r="A2790" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2790" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monstera Deliciosa </t>
+        </is>
+      </c>
+    </row>
+    <row r="2791">
+      <c r="A2791" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2791" t="inlineStr">
+        <is>
+          <t>Philodendron Imperial Red</t>
+        </is>
+      </c>
+    </row>
+    <row r="2792"/>
+    <row r="2793">
+      <c r="A2793" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2793" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+    </row>
+    <row r="2794">
+      <c r="A2794" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2794" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+    </row>
+    <row r="2795">
+      <c r="A2795" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2795" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+    </row>
+    <row r="2796">
+      <c r="A2796" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2796" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+    </row>
+    <row r="2797">
+      <c r="A2797" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2797" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+    </row>
+    <row r="2798">
+      <c r="A2798" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2798" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+    </row>
+    <row r="2799">
+      <c r="A2799" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2799" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+    </row>
+    <row r="2800">
+      <c r="A2800" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2800" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+    </row>
+    <row r="2801">
+      <c r="A2801" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2801" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+    </row>
+    <row r="2802">
+      <c r="A2802" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2802" t="inlineStr">
+        <is>
+          <t>Epipremnum Pinnatum Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="2803">
+      <c r="A2803" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2803" t="inlineStr">
+        <is>
+          <t>Sansevieria Laurentii</t>
+        </is>
+      </c>
+    </row>
+    <row r="2804">
+      <c r="A2804" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2804" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum Saal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2805">
+      <c r="A2805" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2805" t="inlineStr">
+        <is>
+          <t>Monstera Deliciosa Variegata</t>
+        </is>
+      </c>
+    </row>
+    <row r="2806">
+      <c r="A2806" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2806" t="inlineStr">
+        <is>
+          <t>Pachira Aquatica</t>
+        </is>
+      </c>
+    </row>
+    <row r="2807">
+      <c r="A2807" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2807" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monstera Deliciosa </t>
+        </is>
+      </c>
+    </row>
+    <row r="2808">
+      <c r="A2808" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2808" t="inlineStr">
+        <is>
+          <t>Philodendron Imperial Red</t>
+        </is>
+      </c>
+    </row>
+    <row r="2809"/>
+    <row r="2810">
+      <c r="A2810" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2810" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+    </row>
+    <row r="2811">
+      <c r="A2811" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2811" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+    </row>
+    <row r="2812">
+      <c r="A2812" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2812" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+    </row>
+    <row r="2813">
+      <c r="A2813" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2813" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+    </row>
+    <row r="2814">
+      <c r="A2814" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2814" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+    </row>
+    <row r="2815">
+      <c r="A2815" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2815" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+    </row>
+    <row r="2816">
+      <c r="A2816" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2816" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+    </row>
+    <row r="2817">
+      <c r="A2817" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2817" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+    </row>
+    <row r="2818">
+      <c r="A2818" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2818" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+    </row>
+    <row r="2819">
+      <c r="A2819" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2819" t="inlineStr">
+        <is>
+          <t>Epipremnum Pinnatum Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="2820">
+      <c r="A2820" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2820" t="inlineStr">
+        <is>
+          <t>Sansevieria Laurentii</t>
+        </is>
+      </c>
+    </row>
+    <row r="2821">
+      <c r="A2821" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2821" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum Saal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2822">
+      <c r="A2822" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2822" t="inlineStr">
+        <is>
+          <t>Monstera Deliciosa Variegata</t>
+        </is>
+      </c>
+    </row>
+    <row r="2823">
+      <c r="A2823" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2823" t="inlineStr">
+        <is>
+          <t>Pachira Aquatica</t>
+        </is>
+      </c>
+    </row>
+    <row r="2824">
+      <c r="A2824" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2824" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monstera Deliciosa </t>
+        </is>
+      </c>
+    </row>
+    <row r="2825">
+      <c r="A2825" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2825" t="inlineStr">
+        <is>
+          <t>Philodendron Imperial Red</t>
+        </is>
+      </c>
+    </row>
+    <row r="2826"/>
+    <row r="2827">
+      <c r="A2827" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2827" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+    </row>
+    <row r="2828">
+      <c r="A2828" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2828" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+    </row>
+    <row r="2829">
+      <c r="A2829" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2829" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+    </row>
+    <row r="2830">
+      <c r="A2830" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2830" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+    </row>
+    <row r="2831">
+      <c r="A2831" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2831" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+    </row>
+    <row r="2832">
+      <c r="A2832" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2832" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+    </row>
+    <row r="2833">
+      <c r="A2833" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2833" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+    </row>
+    <row r="2834">
+      <c r="A2834" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2834" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+    </row>
+    <row r="2835">
+      <c r="A2835" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2835" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+    </row>
+    <row r="2836">
+      <c r="A2836" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2836" t="inlineStr">
+        <is>
+          <t>Epipremnum Pinnatum Blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="2837">
+      <c r="A2837" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2837" t="inlineStr">
+        <is>
+          <t>Sansevieria Laurentii</t>
+        </is>
+      </c>
+    </row>
+    <row r="2838">
+      <c r="A2838" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2838" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum Saal</t>
+        </is>
+      </c>
+    </row>
+    <row r="2839">
+      <c r="A2839" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2839" t="inlineStr">
+        <is>
+          <t>Monstera Deliciosa Variegata</t>
+        </is>
+      </c>
+    </row>
+    <row r="2840">
+      <c r="A2840" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2840" t="inlineStr">
+        <is>
+          <t>Pachira Aquatica</t>
+        </is>
+      </c>
+    </row>
+    <row r="2841">
+      <c r="A2841" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2841" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monstera Deliciosa </t>
+        </is>
+      </c>
+    </row>
+    <row r="2842">
+      <c r="A2842" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2842" t="inlineStr">
+        <is>
+          <t>Philodendron Imperial Red</t>
+        </is>
+      </c>
+    </row>
+    <row r="2843"/>
+    <row r="2844">
+      <c r="A2844" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2844" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+      <c r="C2844" t="inlineStr"/>
+      <c r="D2844" t="inlineStr"/>
+      <c r="E2844" t="inlineStr"/>
+      <c r="F2844" t="inlineStr"/>
+      <c r="G2844" t="inlineStr"/>
+      <c r="H2844" t="inlineStr"/>
+      <c r="I2844" t="inlineStr"/>
+    </row>
+    <row r="2845">
+      <c r="A2845" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2845" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+      <c r="C2845" t="inlineStr"/>
+      <c r="D2845" t="inlineStr"/>
+      <c r="E2845" t="inlineStr"/>
+      <c r="F2845" t="inlineStr"/>
+      <c r="G2845" t="inlineStr"/>
+      <c r="H2845" t="inlineStr"/>
+      <c r="I2845" t="inlineStr"/>
+    </row>
+    <row r="2846">
+      <c r="A2846" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2846" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+      <c r="C2846" t="inlineStr"/>
+      <c r="D2846" t="inlineStr"/>
+      <c r="E2846" t="inlineStr"/>
+      <c r="F2846" t="inlineStr"/>
+      <c r="G2846" t="inlineStr"/>
+      <c r="H2846" t="inlineStr"/>
+      <c r="I2846" t="inlineStr"/>
+    </row>
+    <row r="2847">
+      <c r="A2847" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2847" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+      <c r="C2847" t="inlineStr"/>
+      <c r="D2847" t="inlineStr"/>
+      <c r="E2847" t="inlineStr"/>
+      <c r="F2847" t="inlineStr"/>
+      <c r="G2847" t="inlineStr"/>
+      <c r="H2847" t="inlineStr"/>
+      <c r="I2847" t="inlineStr"/>
+    </row>
+    <row r="2848">
+      <c r="A2848" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2848" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+      <c r="C2848" t="inlineStr"/>
+      <c r="D2848" t="inlineStr"/>
+      <c r="E2848" t="inlineStr"/>
+      <c r="F2848" t="inlineStr"/>
+      <c r="G2848" t="inlineStr"/>
+      <c r="H2848" t="inlineStr"/>
+      <c r="I2848" t="inlineStr"/>
+    </row>
+    <row r="2849">
+      <c r="A2849" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2849" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+      <c r="C2849" t="inlineStr"/>
+      <c r="D2849" t="inlineStr"/>
+      <c r="E2849" t="inlineStr"/>
+      <c r="F2849" t="inlineStr"/>
+      <c r="G2849" t="inlineStr"/>
+      <c r="H2849" t="inlineStr"/>
+      <c r="I2849" t="inlineStr"/>
+    </row>
+    <row r="2850">
+      <c r="A2850" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2850" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+      <c r="C2850" t="inlineStr"/>
+      <c r="D2850" t="inlineStr"/>
+      <c r="E2850" t="inlineStr"/>
+      <c r="F2850" t="inlineStr"/>
+      <c r="G2850" t="inlineStr"/>
+      <c r="H2850" t="inlineStr"/>
+      <c r="I2850" t="inlineStr"/>
+    </row>
+    <row r="2851">
+      <c r="A2851" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2851" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+      <c r="C2851" t="inlineStr"/>
+      <c r="D2851" t="inlineStr"/>
+      <c r="E2851" t="inlineStr"/>
+      <c r="F2851" t="inlineStr"/>
+      <c r="G2851" t="inlineStr"/>
+      <c r="H2851" t="inlineStr"/>
+      <c r="I2851" t="inlineStr"/>
+    </row>
+    <row r="2852">
+      <c r="A2852" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2852" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+      <c r="C2852" t="inlineStr"/>
+      <c r="D2852" t="inlineStr"/>
+      <c r="E2852" t="inlineStr"/>
+      <c r="F2852" t="inlineStr"/>
+      <c r="G2852" t="inlineStr"/>
+      <c r="H2852" t="inlineStr"/>
+      <c r="I2852" t="inlineStr"/>
+    </row>
+    <row r="2853">
+      <c r="A2853" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2853" t="inlineStr">
+        <is>
+          <t>Epipremnum Pinnatum Blue</t>
+        </is>
+      </c>
+      <c r="C2853" t="inlineStr"/>
+      <c r="D2853" t="inlineStr"/>
+      <c r="E2853" t="inlineStr"/>
+      <c r="F2853" t="inlineStr"/>
+      <c r="G2853" t="inlineStr"/>
+      <c r="H2853" t="inlineStr"/>
+      <c r="I2853" t="inlineStr"/>
+    </row>
+    <row r="2854">
+      <c r="A2854" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2854" t="inlineStr">
+        <is>
+          <t>Sansevieria Laurentii</t>
+        </is>
+      </c>
+      <c r="C2854" t="inlineStr"/>
+      <c r="D2854" t="inlineStr"/>
+      <c r="E2854" t="inlineStr"/>
+      <c r="F2854" t="inlineStr"/>
+      <c r="G2854" t="inlineStr"/>
+      <c r="H2854" t="inlineStr"/>
+      <c r="I2854" t="inlineStr"/>
+    </row>
+    <row r="2855">
+      <c r="A2855" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2855" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum Saal</t>
+        </is>
+      </c>
+      <c r="C2855" t="inlineStr"/>
+      <c r="D2855" t="inlineStr"/>
+      <c r="E2855" t="inlineStr"/>
+      <c r="F2855" t="inlineStr"/>
+      <c r="G2855" t="inlineStr"/>
+      <c r="H2855" t="inlineStr"/>
+      <c r="I2855" t="inlineStr"/>
+    </row>
+    <row r="2856">
+      <c r="A2856" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2856" t="inlineStr">
+        <is>
+          <t>Monstera Deliciosa Variegata</t>
+        </is>
+      </c>
+      <c r="C2856" t="inlineStr"/>
+      <c r="D2856" t="inlineStr"/>
+      <c r="E2856" t="inlineStr"/>
+      <c r="F2856" t="inlineStr"/>
+      <c r="G2856" t="inlineStr"/>
+      <c r="H2856" t="inlineStr"/>
+      <c r="I2856" t="inlineStr"/>
+    </row>
+    <row r="2857">
+      <c r="A2857" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2857" t="inlineStr">
+        <is>
+          <t>Pachira Aquatica</t>
+        </is>
+      </c>
+      <c r="C2857" t="inlineStr"/>
+      <c r="D2857" t="inlineStr"/>
+      <c r="E2857" t="inlineStr"/>
+      <c r="F2857" t="inlineStr"/>
+      <c r="G2857" t="inlineStr"/>
+      <c r="H2857" t="inlineStr"/>
+      <c r="I2857" t="inlineStr"/>
+    </row>
+    <row r="2858">
+      <c r="A2858" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2858" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monstera Deliciosa </t>
+        </is>
+      </c>
+      <c r="C2858" t="inlineStr"/>
+      <c r="D2858" t="inlineStr"/>
+      <c r="E2858" t="inlineStr"/>
+      <c r="F2858" t="inlineStr"/>
+      <c r="G2858" t="inlineStr"/>
+      <c r="H2858" t="inlineStr"/>
+      <c r="I2858" t="inlineStr"/>
+    </row>
+    <row r="2859">
+      <c r="A2859" t="inlineStr">
+        <is>
+          <t>04.08.2025</t>
+        </is>
+      </c>
+      <c r="B2859" t="inlineStr">
+        <is>
+          <t>Philodendron Imperial Red</t>
+        </is>
+      </c>
+      <c r="C2859" t="inlineStr"/>
+      <c r="D2859" t="inlineStr"/>
+      <c r="E2859" t="inlineStr"/>
+      <c r="F2859" t="inlineStr"/>
+      <c r="G2859" t="inlineStr"/>
+      <c r="H2859" t="inlineStr"/>
+      <c r="I2859" t="inlineStr"/>
+    </row>
+    <row r="2860"/>
+    <row r="2861">
+      <c r="A2861" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2861" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+      <c r="C2861" t="inlineStr"/>
+      <c r="D2861" t="inlineStr"/>
+      <c r="E2861" t="inlineStr"/>
+      <c r="F2861" t="inlineStr"/>
+      <c r="G2861" t="inlineStr"/>
+      <c r="H2861" t="inlineStr"/>
+      <c r="I2861" t="inlineStr"/>
+    </row>
+    <row r="2862">
+      <c r="A2862" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2862" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+      <c r="C2862" t="inlineStr"/>
+      <c r="D2862" t="inlineStr"/>
+      <c r="E2862" t="inlineStr"/>
+      <c r="F2862" t="inlineStr"/>
+      <c r="G2862" t="inlineStr"/>
+      <c r="H2862" t="inlineStr"/>
+      <c r="I2862" t="inlineStr"/>
+    </row>
+    <row r="2863">
+      <c r="A2863" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2863" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+      <c r="C2863" t="inlineStr"/>
+      <c r="D2863" t="inlineStr"/>
+      <c r="E2863" t="inlineStr"/>
+      <c r="F2863" t="inlineStr"/>
+      <c r="G2863" t="inlineStr"/>
+      <c r="H2863" t="inlineStr"/>
+      <c r="I2863" t="inlineStr"/>
+    </row>
+    <row r="2864">
+      <c r="A2864" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2864" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+      <c r="C2864" t="inlineStr"/>
+      <c r="D2864" t="inlineStr"/>
+      <c r="E2864" t="inlineStr"/>
+      <c r="F2864" t="inlineStr"/>
+      <c r="G2864" t="inlineStr"/>
+      <c r="H2864" t="inlineStr"/>
+      <c r="I2864" t="inlineStr"/>
+    </row>
+    <row r="2865">
+      <c r="A2865" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2865" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+      <c r="C2865" t="inlineStr"/>
+      <c r="D2865" t="inlineStr"/>
+      <c r="E2865" t="inlineStr"/>
+      <c r="F2865" t="inlineStr"/>
+      <c r="G2865" t="inlineStr"/>
+      <c r="H2865" t="inlineStr"/>
+      <c r="I2865" t="inlineStr"/>
+    </row>
+    <row r="2866">
+      <c r="A2866" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2866" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+      <c r="C2866" t="inlineStr"/>
+      <c r="D2866" t="inlineStr"/>
+      <c r="E2866" t="inlineStr"/>
+      <c r="F2866" t="inlineStr"/>
+      <c r="G2866" t="inlineStr"/>
+      <c r="H2866" t="inlineStr"/>
+      <c r="I2866" t="inlineStr"/>
+    </row>
+    <row r="2867">
+      <c r="A2867" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2867" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+      <c r="C2867" t="inlineStr"/>
+      <c r="D2867" t="inlineStr"/>
+      <c r="E2867" t="inlineStr"/>
+      <c r="F2867" t="inlineStr"/>
+      <c r="G2867" t="inlineStr"/>
+      <c r="H2867" t="inlineStr"/>
+      <c r="I2867" t="inlineStr"/>
+    </row>
+    <row r="2868">
+      <c r="A2868" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2868" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+      <c r="C2868" t="inlineStr"/>
+      <c r="D2868" t="inlineStr"/>
+      <c r="E2868" t="inlineStr"/>
+      <c r="F2868" t="inlineStr"/>
+      <c r="G2868" t="inlineStr"/>
+      <c r="H2868" t="inlineStr"/>
+      <c r="I2868" t="inlineStr"/>
+    </row>
+    <row r="2869">
+      <c r="A2869" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2869" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+      <c r="C2869" t="inlineStr"/>
+      <c r="D2869" t="inlineStr"/>
+      <c r="E2869" t="inlineStr"/>
+      <c r="F2869" t="inlineStr"/>
+      <c r="G2869" t="inlineStr"/>
+      <c r="H2869" t="inlineStr"/>
+      <c r="I2869" t="inlineStr"/>
+    </row>
+    <row r="2870">
+      <c r="A2870" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2870" t="inlineStr">
+        <is>
+          <t>Epipremnum Pinnatum Blue</t>
+        </is>
+      </c>
+      <c r="C2870" t="inlineStr"/>
+      <c r="D2870" t="inlineStr"/>
+      <c r="E2870" t="inlineStr"/>
+      <c r="F2870" t="inlineStr"/>
+      <c r="G2870" t="inlineStr"/>
+      <c r="H2870" t="inlineStr"/>
+      <c r="I2870" t="inlineStr"/>
+    </row>
+    <row r="2871">
+      <c r="A2871" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2871" t="inlineStr">
+        <is>
+          <t>Sansevieria Laurentii</t>
+        </is>
+      </c>
+      <c r="C2871" t="inlineStr"/>
+      <c r="D2871" t="inlineStr"/>
+      <c r="E2871" t="inlineStr"/>
+      <c r="F2871" t="inlineStr"/>
+      <c r="G2871" t="inlineStr"/>
+      <c r="H2871" t="inlineStr"/>
+      <c r="I2871" t="inlineStr"/>
+    </row>
+    <row r="2872">
+      <c r="A2872" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2872" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum Saal</t>
+        </is>
+      </c>
+      <c r="C2872" t="inlineStr"/>
+      <c r="D2872" t="inlineStr"/>
+      <c r="E2872" t="inlineStr"/>
+      <c r="F2872" t="inlineStr"/>
+      <c r="G2872" t="inlineStr"/>
+      <c r="H2872" t="inlineStr"/>
+      <c r="I2872" t="inlineStr"/>
+    </row>
+    <row r="2873">
+      <c r="A2873" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2873" t="inlineStr">
+        <is>
+          <t>Monstera Deliciosa Variegata</t>
+        </is>
+      </c>
+      <c r="C2873" t="inlineStr"/>
+      <c r="D2873" t="inlineStr"/>
+      <c r="E2873" t="inlineStr"/>
+      <c r="F2873" t="inlineStr"/>
+      <c r="G2873" t="inlineStr"/>
+      <c r="H2873" t="inlineStr"/>
+      <c r="I2873" t="inlineStr"/>
+    </row>
+    <row r="2874">
+      <c r="A2874" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2874" t="inlineStr">
+        <is>
+          <t>Pachira Aquatica</t>
+        </is>
+      </c>
+      <c r="C2874" t="inlineStr"/>
+      <c r="D2874" t="inlineStr"/>
+      <c r="E2874" t="inlineStr"/>
+      <c r="F2874" t="inlineStr"/>
+      <c r="G2874" t="inlineStr"/>
+      <c r="H2874" t="inlineStr"/>
+      <c r="I2874" t="inlineStr"/>
+    </row>
+    <row r="2875">
+      <c r="A2875" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2875" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monstera Deliciosa </t>
+        </is>
+      </c>
+      <c r="C2875" t="inlineStr"/>
+      <c r="D2875" t="inlineStr"/>
+      <c r="E2875" t="inlineStr"/>
+      <c r="F2875" t="inlineStr"/>
+      <c r="G2875" t="inlineStr"/>
+      <c r="H2875" t="inlineStr"/>
+      <c r="I2875" t="inlineStr"/>
+    </row>
+    <row r="2876">
+      <c r="A2876" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B2876" t="inlineStr">
+        <is>
+          <t>Philodendron Imperial Red</t>
+        </is>
+      </c>
+      <c r="C2876" t="inlineStr"/>
+      <c r="D2876" t="inlineStr"/>
+      <c r="E2876" t="inlineStr"/>
+      <c r="F2876" t="inlineStr"/>
+      <c r="G2876" t="inlineStr"/>
+      <c r="H2876" t="inlineStr"/>
+      <c r="I2876" t="inlineStr"/>
+    </row>
+    <row r="2877"/>
+    <row r="2878">
+      <c r="A2878" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2878" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+      <c r="C2878" t="inlineStr"/>
+      <c r="D2878" t="inlineStr"/>
+      <c r="E2878" t="inlineStr"/>
+      <c r="F2878" t="inlineStr"/>
+      <c r="G2878" t="inlineStr"/>
+      <c r="H2878" t="inlineStr"/>
+      <c r="I2878" t="inlineStr"/>
+    </row>
+    <row r="2879">
+      <c r="A2879" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2879" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+      <c r="C2879" t="inlineStr"/>
+      <c r="D2879" t="inlineStr"/>
+      <c r="E2879" t="inlineStr"/>
+      <c r="F2879" t="inlineStr"/>
+      <c r="G2879" t="inlineStr"/>
+      <c r="H2879" t="inlineStr"/>
+      <c r="I2879" t="inlineStr"/>
+    </row>
+    <row r="2880">
+      <c r="A2880" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2880" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+      <c r="C2880" t="inlineStr"/>
+      <c r="D2880" t="inlineStr"/>
+      <c r="E2880" t="inlineStr"/>
+      <c r="F2880" t="inlineStr"/>
+      <c r="G2880" t="inlineStr"/>
+      <c r="H2880" t="inlineStr"/>
+      <c r="I2880" t="inlineStr"/>
+    </row>
+    <row r="2881">
+      <c r="A2881" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2881" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+      <c r="C2881" t="inlineStr"/>
+      <c r="D2881" t="inlineStr"/>
+      <c r="E2881" t="inlineStr"/>
+      <c r="F2881" t="inlineStr"/>
+      <c r="G2881" t="inlineStr"/>
+      <c r="H2881" t="inlineStr"/>
+      <c r="I2881" t="inlineStr"/>
+    </row>
+    <row r="2882">
+      <c r="A2882" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2882" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+      <c r="C2882" t="inlineStr"/>
+      <c r="D2882" t="inlineStr"/>
+      <c r="E2882" t="inlineStr"/>
+      <c r="F2882" t="inlineStr"/>
+      <c r="G2882" t="inlineStr"/>
+      <c r="H2882" t="inlineStr"/>
+      <c r="I2882" t="inlineStr"/>
+    </row>
+    <row r="2883">
+      <c r="A2883" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2883" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+      <c r="C2883" t="inlineStr"/>
+      <c r="D2883" t="inlineStr"/>
+      <c r="E2883" t="inlineStr"/>
+      <c r="F2883" t="inlineStr"/>
+      <c r="G2883" t="inlineStr"/>
+      <c r="H2883" t="inlineStr"/>
+      <c r="I2883" t="inlineStr"/>
+    </row>
+    <row r="2884">
+      <c r="A2884" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2884" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+      <c r="C2884" t="inlineStr"/>
+      <c r="D2884" t="inlineStr"/>
+      <c r="E2884" t="inlineStr"/>
+      <c r="F2884" t="inlineStr"/>
+      <c r="G2884" t="inlineStr"/>
+      <c r="H2884" t="inlineStr"/>
+      <c r="I2884" t="inlineStr"/>
+    </row>
+    <row r="2885">
+      <c r="A2885" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2885" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+      <c r="C2885" t="inlineStr"/>
+      <c r="D2885" t="inlineStr"/>
+      <c r="E2885" t="inlineStr"/>
+      <c r="F2885" t="inlineStr"/>
+      <c r="G2885" t="inlineStr"/>
+      <c r="H2885" t="inlineStr"/>
+      <c r="I2885" t="inlineStr"/>
+    </row>
+    <row r="2886">
+      <c r="A2886" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2886" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+      <c r="C2886" t="inlineStr"/>
+      <c r="D2886" t="inlineStr"/>
+      <c r="E2886" t="inlineStr"/>
+      <c r="F2886" t="inlineStr"/>
+      <c r="G2886" t="inlineStr"/>
+      <c r="H2886" t="inlineStr"/>
+      <c r="I2886" t="inlineStr"/>
+    </row>
+    <row r="2887">
+      <c r="A2887" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2887" t="inlineStr">
+        <is>
+          <t>Epipremnum Pinnatum Blue</t>
+        </is>
+      </c>
+      <c r="C2887" t="inlineStr"/>
+      <c r="D2887" t="inlineStr"/>
+      <c r="E2887" t="inlineStr"/>
+      <c r="F2887" t="inlineStr"/>
+      <c r="G2887" t="inlineStr"/>
+      <c r="H2887" t="inlineStr"/>
+      <c r="I2887" t="inlineStr"/>
+    </row>
+    <row r="2888">
+      <c r="A2888" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2888" t="inlineStr">
+        <is>
+          <t>Sansevieria Laurentii</t>
+        </is>
+      </c>
+      <c r="C2888" t="inlineStr"/>
+      <c r="D2888" t="inlineStr"/>
+      <c r="E2888" t="inlineStr"/>
+      <c r="F2888" t="inlineStr"/>
+      <c r="G2888" t="inlineStr"/>
+      <c r="H2888" t="inlineStr"/>
+      <c r="I2888" t="inlineStr"/>
+    </row>
+    <row r="2889">
+      <c r="A2889" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2889" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum Saal</t>
+        </is>
+      </c>
+      <c r="C2889" t="inlineStr"/>
+      <c r="D2889" t="inlineStr"/>
+      <c r="E2889" t="inlineStr"/>
+      <c r="F2889" t="inlineStr"/>
+      <c r="G2889" t="inlineStr"/>
+      <c r="H2889" t="inlineStr"/>
+      <c r="I2889" t="inlineStr"/>
+    </row>
+    <row r="2890">
+      <c r="A2890" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2890" t="inlineStr">
+        <is>
+          <t>Monstera Deliciosa Variegata</t>
+        </is>
+      </c>
+      <c r="C2890" t="inlineStr"/>
+      <c r="D2890" t="inlineStr"/>
+      <c r="E2890" t="inlineStr"/>
+      <c r="F2890" t="inlineStr"/>
+      <c r="G2890" t="inlineStr"/>
+      <c r="H2890" t="inlineStr"/>
+      <c r="I2890" t="inlineStr"/>
+    </row>
+    <row r="2891">
+      <c r="A2891" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2891" t="inlineStr">
+        <is>
+          <t>Pachira Aquatica</t>
+        </is>
+      </c>
+      <c r="C2891" t="inlineStr"/>
+      <c r="D2891" t="inlineStr"/>
+      <c r="E2891" t="inlineStr"/>
+      <c r="F2891" t="inlineStr"/>
+      <c r="G2891" t="inlineStr"/>
+      <c r="H2891" t="inlineStr"/>
+      <c r="I2891" t="inlineStr"/>
+    </row>
+    <row r="2892">
+      <c r="A2892" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2892" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monstera Deliciosa </t>
+        </is>
+      </c>
+      <c r="C2892" t="inlineStr"/>
+      <c r="D2892" t="inlineStr"/>
+      <c r="E2892" t="inlineStr"/>
+      <c r="F2892" t="inlineStr"/>
+      <c r="G2892" t="inlineStr"/>
+      <c r="H2892" t="inlineStr"/>
+      <c r="I2892" t="inlineStr"/>
+    </row>
+    <row r="2893">
+      <c r="A2893" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B2893" t="inlineStr">
+        <is>
+          <t>Philodendron Imperial Red</t>
+        </is>
+      </c>
+      <c r="C2893" t="inlineStr"/>
+      <c r="D2893" t="inlineStr"/>
+      <c r="E2893" t="inlineStr"/>
+      <c r="F2893" t="inlineStr"/>
+      <c r="G2893" t="inlineStr"/>
+      <c r="H2893" t="inlineStr"/>
+      <c r="I2893" t="inlineStr"/>
+    </row>
+    <row r="2894"/>
+    <row r="2895">
+      <c r="A2895" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2895" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+      <c r="C2895" t="inlineStr"/>
+      <c r="D2895" t="inlineStr"/>
+      <c r="E2895" t="inlineStr"/>
+      <c r="F2895" t="inlineStr"/>
+      <c r="G2895" t="inlineStr"/>
+      <c r="H2895" t="inlineStr"/>
+      <c r="I2895" t="inlineStr"/>
+    </row>
+    <row r="2896">
+      <c r="A2896" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2896" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+      <c r="C2896" t="inlineStr"/>
+      <c r="D2896" t="inlineStr"/>
+      <c r="E2896" t="inlineStr"/>
+      <c r="F2896" t="inlineStr"/>
+      <c r="G2896" t="inlineStr"/>
+      <c r="H2896" t="inlineStr"/>
+      <c r="I2896" t="inlineStr"/>
+    </row>
+    <row r="2897">
+      <c r="A2897" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2897" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+      <c r="C2897" t="inlineStr"/>
+      <c r="D2897" t="inlineStr"/>
+      <c r="E2897" t="inlineStr"/>
+      <c r="F2897" t="inlineStr"/>
+      <c r="G2897" t="inlineStr"/>
+      <c r="H2897" t="inlineStr"/>
+      <c r="I2897" t="inlineStr"/>
+    </row>
+    <row r="2898">
+      <c r="A2898" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2898" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+      <c r="C2898" t="inlineStr"/>
+      <c r="D2898" t="inlineStr"/>
+      <c r="E2898" t="inlineStr"/>
+      <c r="F2898" t="inlineStr"/>
+      <c r="G2898" t="inlineStr"/>
+      <c r="H2898" t="inlineStr"/>
+      <c r="I2898" t="inlineStr"/>
+    </row>
+    <row r="2899">
+      <c r="A2899" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2899" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+      <c r="C2899" t="inlineStr"/>
+      <c r="D2899" t="inlineStr"/>
+      <c r="E2899" t="inlineStr"/>
+      <c r="F2899" t="inlineStr"/>
+      <c r="G2899" t="inlineStr"/>
+      <c r="H2899" t="inlineStr"/>
+      <c r="I2899" t="inlineStr"/>
+    </row>
+    <row r="2900">
+      <c r="A2900" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2900" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+      <c r="C2900" t="inlineStr"/>
+      <c r="D2900" t="inlineStr"/>
+      <c r="E2900" t="inlineStr"/>
+      <c r="F2900" t="inlineStr"/>
+      <c r="G2900" t="inlineStr"/>
+      <c r="H2900" t="inlineStr"/>
+      <c r="I2900" t="inlineStr"/>
+    </row>
+    <row r="2901">
+      <c r="A2901" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2901" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+      <c r="C2901" t="inlineStr"/>
+      <c r="D2901" t="inlineStr"/>
+      <c r="E2901" t="inlineStr"/>
+      <c r="F2901" t="inlineStr"/>
+      <c r="G2901" t="inlineStr"/>
+      <c r="H2901" t="inlineStr"/>
+      <c r="I2901" t="inlineStr"/>
+    </row>
+    <row r="2902">
+      <c r="A2902" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2902" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+      <c r="C2902" t="inlineStr"/>
+      <c r="D2902" t="inlineStr"/>
+      <c r="E2902" t="inlineStr"/>
+      <c r="F2902" t="inlineStr"/>
+      <c r="G2902" t="inlineStr"/>
+      <c r="H2902" t="inlineStr"/>
+      <c r="I2902" t="inlineStr"/>
+    </row>
+    <row r="2903">
+      <c r="A2903" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2903" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+      <c r="C2903" t="inlineStr"/>
+      <c r="D2903" t="inlineStr"/>
+      <c r="E2903" t="inlineStr"/>
+      <c r="F2903" t="inlineStr"/>
+      <c r="G2903" t="inlineStr"/>
+      <c r="H2903" t="inlineStr"/>
+      <c r="I2903" t="inlineStr"/>
+    </row>
+    <row r="2904">
+      <c r="A2904" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2904" t="inlineStr">
+        <is>
+          <t>Epipremnum Pinnatum Blue</t>
+        </is>
+      </c>
+      <c r="C2904" t="inlineStr"/>
+      <c r="D2904" t="inlineStr"/>
+      <c r="E2904" t="inlineStr"/>
+      <c r="F2904" t="inlineStr"/>
+      <c r="G2904" t="inlineStr"/>
+      <c r="H2904" t="inlineStr"/>
+      <c r="I2904" t="inlineStr"/>
+    </row>
+    <row r="2905">
+      <c r="A2905" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2905" t="inlineStr">
+        <is>
+          <t>Sansevieria Laurentii</t>
+        </is>
+      </c>
+      <c r="C2905" t="inlineStr"/>
+      <c r="D2905" t="inlineStr"/>
+      <c r="E2905" t="inlineStr"/>
+      <c r="F2905" t="inlineStr"/>
+      <c r="G2905" t="inlineStr"/>
+      <c r="H2905" t="inlineStr"/>
+      <c r="I2905" t="inlineStr"/>
+    </row>
+    <row r="2906">
+      <c r="A2906" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2906" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum Saal</t>
+        </is>
+      </c>
+      <c r="C2906" t="inlineStr"/>
+      <c r="D2906" t="inlineStr"/>
+      <c r="E2906" t="inlineStr"/>
+      <c r="F2906" t="inlineStr"/>
+      <c r="G2906" t="inlineStr"/>
+      <c r="H2906" t="inlineStr"/>
+      <c r="I2906" t="inlineStr"/>
+    </row>
+    <row r="2907">
+      <c r="A2907" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2907" t="inlineStr">
+        <is>
+          <t>Monstera Deliciosa Variegata</t>
+        </is>
+      </c>
+      <c r="C2907" t="inlineStr"/>
+      <c r="D2907" t="inlineStr"/>
+      <c r="E2907" t="inlineStr"/>
+      <c r="F2907" t="inlineStr"/>
+      <c r="G2907" t="inlineStr"/>
+      <c r="H2907" t="inlineStr"/>
+      <c r="I2907" t="inlineStr"/>
+    </row>
+    <row r="2908">
+      <c r="A2908" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2908" t="inlineStr">
+        <is>
+          <t>Pachira Aquatica</t>
+        </is>
+      </c>
+      <c r="C2908" t="inlineStr"/>
+      <c r="D2908" t="inlineStr"/>
+      <c r="E2908" t="inlineStr"/>
+      <c r="F2908" t="inlineStr"/>
+      <c r="G2908" t="inlineStr"/>
+      <c r="H2908" t="inlineStr"/>
+      <c r="I2908" t="inlineStr"/>
+    </row>
+    <row r="2909">
+      <c r="A2909" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2909" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monstera Deliciosa </t>
+        </is>
+      </c>
+      <c r="C2909" t="inlineStr"/>
+      <c r="D2909" t="inlineStr"/>
+      <c r="E2909" t="inlineStr"/>
+      <c r="F2909" t="inlineStr"/>
+      <c r="G2909" t="inlineStr"/>
+      <c r="H2909" t="inlineStr"/>
+      <c r="I2909" t="inlineStr"/>
+    </row>
+    <row r="2910">
+      <c r="A2910" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B2910" t="inlineStr">
+        <is>
+          <t>Philodendron Imperial Red</t>
+        </is>
+      </c>
+      <c r="C2910" t="inlineStr"/>
+      <c r="D2910" t="inlineStr"/>
+      <c r="E2910" t="inlineStr"/>
+      <c r="F2910" t="inlineStr"/>
+      <c r="G2910" t="inlineStr"/>
+      <c r="H2910" t="inlineStr"/>
+      <c r="I2910" t="inlineStr"/>
+    </row>
+    <row r="2911"/>
+    <row r="2912">
+      <c r="A2912" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2912" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+      <c r="C2912" t="inlineStr"/>
+      <c r="D2912" t="inlineStr"/>
+      <c r="E2912" t="inlineStr"/>
+      <c r="F2912" t="inlineStr"/>
+      <c r="G2912" t="inlineStr"/>
+      <c r="H2912" t="inlineStr"/>
+      <c r="I2912" t="inlineStr"/>
+    </row>
+    <row r="2913">
+      <c r="A2913" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2913" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+      <c r="C2913" t="inlineStr"/>
+      <c r="D2913" t="inlineStr"/>
+      <c r="E2913" t="inlineStr"/>
+      <c r="F2913" t="inlineStr"/>
+      <c r="G2913" t="inlineStr"/>
+      <c r="H2913" t="inlineStr"/>
+      <c r="I2913" t="inlineStr"/>
+    </row>
+    <row r="2914">
+      <c r="A2914" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2914" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+      <c r="C2914" t="inlineStr"/>
+      <c r="D2914" t="inlineStr"/>
+      <c r="E2914" t="inlineStr"/>
+      <c r="F2914" t="inlineStr"/>
+      <c r="G2914" t="inlineStr"/>
+      <c r="H2914" t="inlineStr"/>
+      <c r="I2914" t="inlineStr"/>
+    </row>
+    <row r="2915">
+      <c r="A2915" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2915" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+      <c r="C2915" t="inlineStr"/>
+      <c r="D2915" t="inlineStr"/>
+      <c r="E2915" t="inlineStr"/>
+      <c r="F2915" t="inlineStr"/>
+      <c r="G2915" t="inlineStr"/>
+      <c r="H2915" t="inlineStr"/>
+      <c r="I2915" t="inlineStr"/>
+    </row>
+    <row r="2916">
+      <c r="A2916" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2916" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+      <c r="C2916" t="inlineStr"/>
+      <c r="D2916" t="inlineStr"/>
+      <c r="E2916" t="inlineStr"/>
+      <c r="F2916" t="inlineStr"/>
+      <c r="G2916" t="inlineStr"/>
+      <c r="H2916" t="inlineStr"/>
+      <c r="I2916" t="inlineStr"/>
+    </row>
+    <row r="2917">
+      <c r="A2917" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2917" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+      <c r="C2917" t="inlineStr"/>
+      <c r="D2917" t="inlineStr"/>
+      <c r="E2917" t="inlineStr"/>
+      <c r="F2917" t="inlineStr"/>
+      <c r="G2917" t="inlineStr"/>
+      <c r="H2917" t="inlineStr"/>
+      <c r="I2917" t="inlineStr"/>
+    </row>
+    <row r="2918">
+      <c r="A2918" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2918" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+      <c r="C2918" t="inlineStr"/>
+      <c r="D2918" t="inlineStr"/>
+      <c r="E2918" t="inlineStr"/>
+      <c r="F2918" t="inlineStr"/>
+      <c r="G2918" t="inlineStr"/>
+      <c r="H2918" t="inlineStr"/>
+      <c r="I2918" t="inlineStr"/>
+    </row>
+    <row r="2919">
+      <c r="A2919" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2919" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+      <c r="C2919" t="inlineStr"/>
+      <c r="D2919" t="inlineStr"/>
+      <c r="E2919" t="inlineStr"/>
+      <c r="F2919" t="inlineStr"/>
+      <c r="G2919" t="inlineStr"/>
+      <c r="H2919" t="inlineStr"/>
+      <c r="I2919" t="inlineStr"/>
+    </row>
+    <row r="2920">
+      <c r="A2920" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2920" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+      <c r="C2920" t="inlineStr"/>
+      <c r="D2920" t="inlineStr"/>
+      <c r="E2920" t="inlineStr"/>
+      <c r="F2920" t="inlineStr"/>
+      <c r="G2920" t="inlineStr"/>
+      <c r="H2920" t="inlineStr"/>
+      <c r="I2920" t="inlineStr"/>
+    </row>
+    <row r="2921">
+      <c r="A2921" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2921" t="inlineStr">
+        <is>
+          <t>Epipremnum Pinnatum Blue</t>
+        </is>
+      </c>
+      <c r="C2921" t="inlineStr"/>
+      <c r="D2921" t="inlineStr"/>
+      <c r="E2921" t="inlineStr"/>
+      <c r="F2921" t="inlineStr"/>
+      <c r="G2921" t="inlineStr"/>
+      <c r="H2921" t="inlineStr"/>
+      <c r="I2921" t="inlineStr"/>
+    </row>
+    <row r="2922">
+      <c r="A2922" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2922" t="inlineStr">
+        <is>
+          <t>Sansevieria Laurentii</t>
+        </is>
+      </c>
+      <c r="C2922" t="inlineStr"/>
+      <c r="D2922" t="inlineStr"/>
+      <c r="E2922" t="inlineStr"/>
+      <c r="F2922" t="inlineStr"/>
+      <c r="G2922" t="inlineStr"/>
+      <c r="H2922" t="inlineStr"/>
+      <c r="I2922" t="inlineStr"/>
+    </row>
+    <row r="2923">
+      <c r="A2923" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2923" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum Saal</t>
+        </is>
+      </c>
+      <c r="C2923" t="inlineStr"/>
+      <c r="D2923" t="inlineStr"/>
+      <c r="E2923" t="inlineStr"/>
+      <c r="F2923" t="inlineStr"/>
+      <c r="G2923" t="inlineStr"/>
+      <c r="H2923" t="inlineStr"/>
+      <c r="I2923" t="inlineStr"/>
+    </row>
+    <row r="2924">
+      <c r="A2924" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2924" t="inlineStr">
+        <is>
+          <t>Monstera Deliciosa Variegata</t>
+        </is>
+      </c>
+      <c r="C2924" t="inlineStr"/>
+      <c r="D2924" t="inlineStr"/>
+      <c r="E2924" t="inlineStr"/>
+      <c r="F2924" t="inlineStr"/>
+      <c r="G2924" t="inlineStr"/>
+      <c r="H2924" t="inlineStr"/>
+      <c r="I2924" t="inlineStr"/>
+    </row>
+    <row r="2925">
+      <c r="A2925" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2925" t="inlineStr">
+        <is>
+          <t>Pachira Aquatica</t>
+        </is>
+      </c>
+      <c r="C2925" t="inlineStr"/>
+      <c r="D2925" t="inlineStr"/>
+      <c r="E2925" t="inlineStr"/>
+      <c r="F2925" t="inlineStr"/>
+      <c r="G2925" t="inlineStr"/>
+      <c r="H2925" t="inlineStr"/>
+      <c r="I2925" t="inlineStr"/>
+    </row>
+    <row r="2926">
+      <c r="A2926" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2926" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monstera Deliciosa </t>
+        </is>
+      </c>
+      <c r="C2926" t="inlineStr"/>
+      <c r="D2926" t="inlineStr"/>
+      <c r="E2926" t="inlineStr"/>
+      <c r="F2926" t="inlineStr"/>
+      <c r="G2926" t="inlineStr"/>
+      <c r="H2926" t="inlineStr"/>
+      <c r="I2926" t="inlineStr"/>
+    </row>
+    <row r="2927">
+      <c r="A2927" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B2927" t="inlineStr">
+        <is>
+          <t>Philodendron Imperial Red</t>
+        </is>
+      </c>
+      <c r="C2927" t="inlineStr"/>
+      <c r="D2927" t="inlineStr"/>
+      <c r="E2927" t="inlineStr"/>
+      <c r="F2927" t="inlineStr"/>
+      <c r="G2927" t="inlineStr"/>
+      <c r="H2927" t="inlineStr"/>
+      <c r="I2927" t="inlineStr"/>
+    </row>
+    <row r="2928"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Preserve local changes to blumen_data.xlsx
</commit_message>
<xml_diff>
--- a/data/blumen_data.xlsx
+++ b/data/blumen_data.xlsx
@@ -490,7 +490,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD1313"/>
+  <dimension ref="A1:AD1398"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1068" activePane="bottomLeft" state="frozen"/>
@@ -15101,13 +15101,6 @@
           <t>Calathea Medalion</t>
         </is>
       </c>
-      <c r="C1212" t="inlineStr"/>
-      <c r="D1212" t="inlineStr"/>
-      <c r="E1212" t="inlineStr"/>
-      <c r="F1212" t="inlineStr"/>
-      <c r="G1212" t="inlineStr"/>
-      <c r="H1212" t="inlineStr"/>
-      <c r="I1212" t="inlineStr"/>
     </row>
     <row r="1213">
       <c r="A1213" t="inlineStr">
@@ -15120,13 +15113,6 @@
           <t>Epipremnum Aureum</t>
         </is>
       </c>
-      <c r="C1213" t="inlineStr"/>
-      <c r="D1213" t="inlineStr"/>
-      <c r="E1213" t="inlineStr"/>
-      <c r="F1213" t="inlineStr"/>
-      <c r="G1213" t="inlineStr"/>
-      <c r="H1213" t="inlineStr"/>
-      <c r="I1213" t="inlineStr"/>
     </row>
     <row r="1214">
       <c r="A1214" t="inlineStr">
@@ -15139,13 +15125,6 @@
           <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
-      <c r="C1214" t="inlineStr"/>
-      <c r="D1214" t="inlineStr"/>
-      <c r="E1214" t="inlineStr"/>
-      <c r="F1214" t="inlineStr"/>
-      <c r="G1214" t="inlineStr"/>
-      <c r="H1214" t="inlineStr"/>
-      <c r="I1214" t="inlineStr"/>
     </row>
     <row r="1215">
       <c r="A1215" t="inlineStr">
@@ -15158,13 +15137,6 @@
           <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
-      <c r="C1215" t="inlineStr"/>
-      <c r="D1215" t="inlineStr"/>
-      <c r="E1215" t="inlineStr"/>
-      <c r="F1215" t="inlineStr"/>
-      <c r="G1215" t="inlineStr"/>
-      <c r="H1215" t="inlineStr"/>
-      <c r="I1215" t="inlineStr"/>
     </row>
     <row r="1216">
       <c r="A1216" t="inlineStr">
@@ -15177,13 +15149,6 @@
           <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
-      <c r="C1216" t="inlineStr"/>
-      <c r="D1216" t="inlineStr"/>
-      <c r="E1216" t="inlineStr"/>
-      <c r="F1216" t="inlineStr"/>
-      <c r="G1216" t="inlineStr"/>
-      <c r="H1216" t="inlineStr"/>
-      <c r="I1216" t="inlineStr"/>
     </row>
     <row r="1217">
       <c r="A1217" t="inlineStr">
@@ -15196,13 +15161,6 @@
           <t>Monstera Adenossii</t>
         </is>
       </c>
-      <c r="C1217" t="inlineStr"/>
-      <c r="D1217" t="inlineStr"/>
-      <c r="E1217" t="inlineStr"/>
-      <c r="F1217" t="inlineStr"/>
-      <c r="G1217" t="inlineStr"/>
-      <c r="H1217" t="inlineStr"/>
-      <c r="I1217" t="inlineStr"/>
     </row>
     <row r="1218">
       <c r="A1218" t="inlineStr">
@@ -15215,13 +15173,6 @@
           <t>Ficus Elastica Abidjan</t>
         </is>
       </c>
-      <c r="C1218" t="inlineStr"/>
-      <c r="D1218" t="inlineStr"/>
-      <c r="E1218" t="inlineStr"/>
-      <c r="F1218" t="inlineStr"/>
-      <c r="G1218" t="inlineStr"/>
-      <c r="H1218" t="inlineStr"/>
-      <c r="I1218" t="inlineStr"/>
     </row>
     <row r="1219">
       <c r="A1219" t="inlineStr">
@@ -15234,13 +15185,6 @@
           <t>Peperomia Hope</t>
         </is>
       </c>
-      <c r="C1219" t="inlineStr"/>
-      <c r="D1219" t="inlineStr"/>
-      <c r="E1219" t="inlineStr"/>
-      <c r="F1219" t="inlineStr"/>
-      <c r="G1219" t="inlineStr"/>
-      <c r="H1219" t="inlineStr"/>
-      <c r="I1219" t="inlineStr"/>
     </row>
     <row r="1220">
       <c r="A1220" t="inlineStr">
@@ -15253,13 +15197,6 @@
           <t>Hoya Mathilde</t>
         </is>
       </c>
-      <c r="C1220" t="inlineStr"/>
-      <c r="D1220" t="inlineStr"/>
-      <c r="E1220" t="inlineStr"/>
-      <c r="F1220" t="inlineStr"/>
-      <c r="G1220" t="inlineStr"/>
-      <c r="H1220" t="inlineStr"/>
-      <c r="I1220" t="inlineStr"/>
     </row>
     <row r="1221">
       <c r="A1221" t="inlineStr">
@@ -15272,13 +15209,6 @@
           <t>Epipremnum Pinnatum Blue</t>
         </is>
       </c>
-      <c r="C1221" t="inlineStr"/>
-      <c r="D1221" t="inlineStr"/>
-      <c r="E1221" t="inlineStr"/>
-      <c r="F1221" t="inlineStr"/>
-      <c r="G1221" t="inlineStr"/>
-      <c r="H1221" t="inlineStr"/>
-      <c r="I1221" t="inlineStr"/>
     </row>
     <row r="1222">
       <c r="A1222" t="inlineStr">
@@ -15291,13 +15221,6 @@
           <t>Sansevieria Laurentii</t>
         </is>
       </c>
-      <c r="C1222" t="inlineStr"/>
-      <c r="D1222" t="inlineStr"/>
-      <c r="E1222" t="inlineStr"/>
-      <c r="F1222" t="inlineStr"/>
-      <c r="G1222" t="inlineStr"/>
-      <c r="H1222" t="inlineStr"/>
-      <c r="I1222" t="inlineStr"/>
     </row>
     <row r="1223">
       <c r="A1223" t="inlineStr">
@@ -15310,13 +15233,6 @@
           <t>Epipremnum Aureum Saal</t>
         </is>
       </c>
-      <c r="C1223" t="inlineStr"/>
-      <c r="D1223" t="inlineStr"/>
-      <c r="E1223" t="inlineStr"/>
-      <c r="F1223" t="inlineStr"/>
-      <c r="G1223" t="inlineStr"/>
-      <c r="H1223" t="inlineStr"/>
-      <c r="I1223" t="inlineStr"/>
     </row>
     <row r="1224">
       <c r="A1224" t="inlineStr">
@@ -15329,13 +15245,6 @@
           <t>Monstera Deliciosa Variegata</t>
         </is>
       </c>
-      <c r="C1224" t="inlineStr"/>
-      <c r="D1224" t="inlineStr"/>
-      <c r="E1224" t="inlineStr"/>
-      <c r="F1224" t="inlineStr"/>
-      <c r="G1224" t="inlineStr"/>
-      <c r="H1224" t="inlineStr"/>
-      <c r="I1224" t="inlineStr"/>
     </row>
     <row r="1225">
       <c r="A1225" t="inlineStr">
@@ -15348,13 +15257,6 @@
           <t>Pachira Aquatica</t>
         </is>
       </c>
-      <c r="C1225" t="inlineStr"/>
-      <c r="D1225" t="inlineStr"/>
-      <c r="E1225" t="inlineStr"/>
-      <c r="F1225" t="inlineStr"/>
-      <c r="G1225" t="inlineStr"/>
-      <c r="H1225" t="inlineStr"/>
-      <c r="I1225" t="inlineStr"/>
     </row>
     <row r="1226">
       <c r="A1226" t="inlineStr">
@@ -15367,13 +15269,6 @@
           <t xml:space="preserve">Monstera Deliciosa </t>
         </is>
       </c>
-      <c r="C1226" t="inlineStr"/>
-      <c r="D1226" t="inlineStr"/>
-      <c r="E1226" t="inlineStr"/>
-      <c r="F1226" t="inlineStr"/>
-      <c r="G1226" t="inlineStr"/>
-      <c r="H1226" t="inlineStr"/>
-      <c r="I1226" t="inlineStr"/>
     </row>
     <row r="1227">
       <c r="A1227" t="inlineStr">
@@ -15386,13 +15281,6 @@
           <t>Philodendron Imperial Red</t>
         </is>
       </c>
-      <c r="C1227" t="inlineStr"/>
-      <c r="D1227" t="inlineStr"/>
-      <c r="E1227" t="inlineStr"/>
-      <c r="F1227" t="inlineStr"/>
-      <c r="G1227" t="inlineStr"/>
-      <c r="H1227" t="inlineStr"/>
-      <c r="I1227" t="inlineStr"/>
     </row>
     <row r="1228"/>
     <row r="1229">
@@ -15406,13 +15294,6 @@
           <t>Calathea Medalion</t>
         </is>
       </c>
-      <c r="C1229" t="inlineStr"/>
-      <c r="D1229" t="inlineStr"/>
-      <c r="E1229" t="inlineStr"/>
-      <c r="F1229" t="inlineStr"/>
-      <c r="G1229" t="inlineStr"/>
-      <c r="H1229" t="inlineStr"/>
-      <c r="I1229" t="inlineStr"/>
     </row>
     <row r="1230">
       <c r="A1230" t="inlineStr">
@@ -15425,13 +15306,6 @@
           <t>Epipremnum Aureum</t>
         </is>
       </c>
-      <c r="C1230" t="inlineStr"/>
-      <c r="D1230" t="inlineStr"/>
-      <c r="E1230" t="inlineStr"/>
-      <c r="F1230" t="inlineStr"/>
-      <c r="G1230" t="inlineStr"/>
-      <c r="H1230" t="inlineStr"/>
-      <c r="I1230" t="inlineStr"/>
     </row>
     <row r="1231">
       <c r="A1231" t="inlineStr">
@@ -15444,13 +15318,6 @@
           <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
-      <c r="C1231" t="inlineStr"/>
-      <c r="D1231" t="inlineStr"/>
-      <c r="E1231" t="inlineStr"/>
-      <c r="F1231" t="inlineStr"/>
-      <c r="G1231" t="inlineStr"/>
-      <c r="H1231" t="inlineStr"/>
-      <c r="I1231" t="inlineStr"/>
     </row>
     <row r="1232">
       <c r="A1232" t="inlineStr">
@@ -15463,13 +15330,6 @@
           <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
-      <c r="C1232" t="inlineStr"/>
-      <c r="D1232" t="inlineStr"/>
-      <c r="E1232" t="inlineStr"/>
-      <c r="F1232" t="inlineStr"/>
-      <c r="G1232" t="inlineStr"/>
-      <c r="H1232" t="inlineStr"/>
-      <c r="I1232" t="inlineStr"/>
     </row>
     <row r="1233">
       <c r="A1233" t="inlineStr">
@@ -15482,13 +15342,6 @@
           <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
-      <c r="C1233" t="inlineStr"/>
-      <c r="D1233" t="inlineStr"/>
-      <c r="E1233" t="inlineStr"/>
-      <c r="F1233" t="inlineStr"/>
-      <c r="G1233" t="inlineStr"/>
-      <c r="H1233" t="inlineStr"/>
-      <c r="I1233" t="inlineStr"/>
     </row>
     <row r="1234">
       <c r="A1234" t="inlineStr">
@@ -15501,13 +15354,6 @@
           <t>Monstera Adenossii</t>
         </is>
       </c>
-      <c r="C1234" t="inlineStr"/>
-      <c r="D1234" t="inlineStr"/>
-      <c r="E1234" t="inlineStr"/>
-      <c r="F1234" t="inlineStr"/>
-      <c r="G1234" t="inlineStr"/>
-      <c r="H1234" t="inlineStr"/>
-      <c r="I1234" t="inlineStr"/>
     </row>
     <row r="1235">
       <c r="A1235" t="inlineStr">
@@ -15520,13 +15366,6 @@
           <t>Ficus Elastica Abidjan</t>
         </is>
       </c>
-      <c r="C1235" t="inlineStr"/>
-      <c r="D1235" t="inlineStr"/>
-      <c r="E1235" t="inlineStr"/>
-      <c r="F1235" t="inlineStr"/>
-      <c r="G1235" t="inlineStr"/>
-      <c r="H1235" t="inlineStr"/>
-      <c r="I1235" t="inlineStr"/>
     </row>
     <row r="1236">
       <c r="A1236" t="inlineStr">
@@ -15539,13 +15378,6 @@
           <t>Peperomia Hope</t>
         </is>
       </c>
-      <c r="C1236" t="inlineStr"/>
-      <c r="D1236" t="inlineStr"/>
-      <c r="E1236" t="inlineStr"/>
-      <c r="F1236" t="inlineStr"/>
-      <c r="G1236" t="inlineStr"/>
-      <c r="H1236" t="inlineStr"/>
-      <c r="I1236" t="inlineStr"/>
     </row>
     <row r="1237">
       <c r="A1237" t="inlineStr">
@@ -15558,13 +15390,6 @@
           <t>Hoya Mathilde</t>
         </is>
       </c>
-      <c r="C1237" t="inlineStr"/>
-      <c r="D1237" t="inlineStr"/>
-      <c r="E1237" t="inlineStr"/>
-      <c r="F1237" t="inlineStr"/>
-      <c r="G1237" t="inlineStr"/>
-      <c r="H1237" t="inlineStr"/>
-      <c r="I1237" t="inlineStr"/>
     </row>
     <row r="1238">
       <c r="A1238" t="inlineStr">
@@ -15577,13 +15402,6 @@
           <t>Epipremnum Pinnatum Blue</t>
         </is>
       </c>
-      <c r="C1238" t="inlineStr"/>
-      <c r="D1238" t="inlineStr"/>
-      <c r="E1238" t="inlineStr"/>
-      <c r="F1238" t="inlineStr"/>
-      <c r="G1238" t="inlineStr"/>
-      <c r="H1238" t="inlineStr"/>
-      <c r="I1238" t="inlineStr"/>
     </row>
     <row r="1239">
       <c r="A1239" t="inlineStr">
@@ -15596,13 +15414,6 @@
           <t>Sansevieria Laurentii</t>
         </is>
       </c>
-      <c r="C1239" t="inlineStr"/>
-      <c r="D1239" t="inlineStr"/>
-      <c r="E1239" t="inlineStr"/>
-      <c r="F1239" t="inlineStr"/>
-      <c r="G1239" t="inlineStr"/>
-      <c r="H1239" t="inlineStr"/>
-      <c r="I1239" t="inlineStr"/>
     </row>
     <row r="1240">
       <c r="A1240" t="inlineStr">
@@ -15615,13 +15426,6 @@
           <t>Epipremnum Aureum Saal</t>
         </is>
       </c>
-      <c r="C1240" t="inlineStr"/>
-      <c r="D1240" t="inlineStr"/>
-      <c r="E1240" t="inlineStr"/>
-      <c r="F1240" t="inlineStr"/>
-      <c r="G1240" t="inlineStr"/>
-      <c r="H1240" t="inlineStr"/>
-      <c r="I1240" t="inlineStr"/>
     </row>
     <row r="1241">
       <c r="A1241" t="inlineStr">
@@ -15634,13 +15438,6 @@
           <t>Monstera Deliciosa Variegata</t>
         </is>
       </c>
-      <c r="C1241" t="inlineStr"/>
-      <c r="D1241" t="inlineStr"/>
-      <c r="E1241" t="inlineStr"/>
-      <c r="F1241" t="inlineStr"/>
-      <c r="G1241" t="inlineStr"/>
-      <c r="H1241" t="inlineStr"/>
-      <c r="I1241" t="inlineStr"/>
     </row>
     <row r="1242">
       <c r="A1242" t="inlineStr">
@@ -15653,13 +15450,6 @@
           <t>Pachira Aquatica</t>
         </is>
       </c>
-      <c r="C1242" t="inlineStr"/>
-      <c r="D1242" t="inlineStr"/>
-      <c r="E1242" t="inlineStr"/>
-      <c r="F1242" t="inlineStr"/>
-      <c r="G1242" t="inlineStr"/>
-      <c r="H1242" t="inlineStr"/>
-      <c r="I1242" t="inlineStr"/>
     </row>
     <row r="1243">
       <c r="A1243" t="inlineStr">
@@ -15672,13 +15462,6 @@
           <t xml:space="preserve">Monstera Deliciosa </t>
         </is>
       </c>
-      <c r="C1243" t="inlineStr"/>
-      <c r="D1243" t="inlineStr"/>
-      <c r="E1243" t="inlineStr"/>
-      <c r="F1243" t="inlineStr"/>
-      <c r="G1243" t="inlineStr"/>
-      <c r="H1243" t="inlineStr"/>
-      <c r="I1243" t="inlineStr"/>
     </row>
     <row r="1244">
       <c r="A1244" t="inlineStr">
@@ -15691,13 +15474,6 @@
           <t>Philodendron Imperial Red</t>
         </is>
       </c>
-      <c r="C1244" t="inlineStr"/>
-      <c r="D1244" t="inlineStr"/>
-      <c r="E1244" t="inlineStr"/>
-      <c r="F1244" t="inlineStr"/>
-      <c r="G1244" t="inlineStr"/>
-      <c r="H1244" t="inlineStr"/>
-      <c r="I1244" t="inlineStr"/>
     </row>
     <row r="1245"/>
     <row r="1246">
@@ -15711,13 +15487,6 @@
           <t>Calathea Medalion</t>
         </is>
       </c>
-      <c r="C1246" t="inlineStr"/>
-      <c r="D1246" t="inlineStr"/>
-      <c r="E1246" t="inlineStr"/>
-      <c r="F1246" t="inlineStr"/>
-      <c r="G1246" t="inlineStr"/>
-      <c r="H1246" t="inlineStr"/>
-      <c r="I1246" t="inlineStr"/>
     </row>
     <row r="1247">
       <c r="A1247" t="inlineStr">
@@ -15730,13 +15499,6 @@
           <t>Epipremnum Aureum</t>
         </is>
       </c>
-      <c r="C1247" t="inlineStr"/>
-      <c r="D1247" t="inlineStr"/>
-      <c r="E1247" t="inlineStr"/>
-      <c r="F1247" t="inlineStr"/>
-      <c r="G1247" t="inlineStr"/>
-      <c r="H1247" t="inlineStr"/>
-      <c r="I1247" t="inlineStr"/>
     </row>
     <row r="1248">
       <c r="A1248" t="inlineStr">
@@ -15749,13 +15511,6 @@
           <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
-      <c r="C1248" t="inlineStr"/>
-      <c r="D1248" t="inlineStr"/>
-      <c r="E1248" t="inlineStr"/>
-      <c r="F1248" t="inlineStr"/>
-      <c r="G1248" t="inlineStr"/>
-      <c r="H1248" t="inlineStr"/>
-      <c r="I1248" t="inlineStr"/>
     </row>
     <row r="1249">
       <c r="A1249" t="inlineStr">
@@ -15768,13 +15523,6 @@
           <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
-      <c r="C1249" t="inlineStr"/>
-      <c r="D1249" t="inlineStr"/>
-      <c r="E1249" t="inlineStr"/>
-      <c r="F1249" t="inlineStr"/>
-      <c r="G1249" t="inlineStr"/>
-      <c r="H1249" t="inlineStr"/>
-      <c r="I1249" t="inlineStr"/>
     </row>
     <row r="1250">
       <c r="A1250" t="inlineStr">
@@ -15787,13 +15535,6 @@
           <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
-      <c r="C1250" t="inlineStr"/>
-      <c r="D1250" t="inlineStr"/>
-      <c r="E1250" t="inlineStr"/>
-      <c r="F1250" t="inlineStr"/>
-      <c r="G1250" t="inlineStr"/>
-      <c r="H1250" t="inlineStr"/>
-      <c r="I1250" t="inlineStr"/>
     </row>
     <row r="1251">
       <c r="A1251" t="inlineStr">
@@ -15806,13 +15547,6 @@
           <t>Monstera Adenossii</t>
         </is>
       </c>
-      <c r="C1251" t="inlineStr"/>
-      <c r="D1251" t="inlineStr"/>
-      <c r="E1251" t="inlineStr"/>
-      <c r="F1251" t="inlineStr"/>
-      <c r="G1251" t="inlineStr"/>
-      <c r="H1251" t="inlineStr"/>
-      <c r="I1251" t="inlineStr"/>
     </row>
     <row r="1252">
       <c r="A1252" t="inlineStr">
@@ -15825,13 +15559,6 @@
           <t>Ficus Elastica Abidjan</t>
         </is>
       </c>
-      <c r="C1252" t="inlineStr"/>
-      <c r="D1252" t="inlineStr"/>
-      <c r="E1252" t="inlineStr"/>
-      <c r="F1252" t="inlineStr"/>
-      <c r="G1252" t="inlineStr"/>
-      <c r="H1252" t="inlineStr"/>
-      <c r="I1252" t="inlineStr"/>
     </row>
     <row r="1253">
       <c r="A1253" t="inlineStr">
@@ -15844,13 +15571,6 @@
           <t>Peperomia Hope</t>
         </is>
       </c>
-      <c r="C1253" t="inlineStr"/>
-      <c r="D1253" t="inlineStr"/>
-      <c r="E1253" t="inlineStr"/>
-      <c r="F1253" t="inlineStr"/>
-      <c r="G1253" t="inlineStr"/>
-      <c r="H1253" t="inlineStr"/>
-      <c r="I1253" t="inlineStr"/>
     </row>
     <row r="1254">
       <c r="A1254" t="inlineStr">
@@ -15863,13 +15583,6 @@
           <t>Hoya Mathilde</t>
         </is>
       </c>
-      <c r="C1254" t="inlineStr"/>
-      <c r="D1254" t="inlineStr"/>
-      <c r="E1254" t="inlineStr"/>
-      <c r="F1254" t="inlineStr"/>
-      <c r="G1254" t="inlineStr"/>
-      <c r="H1254" t="inlineStr"/>
-      <c r="I1254" t="inlineStr"/>
     </row>
     <row r="1255">
       <c r="A1255" t="inlineStr">
@@ -15882,13 +15595,6 @@
           <t>Epipremnum Pinnatum Blue</t>
         </is>
       </c>
-      <c r="C1255" t="inlineStr"/>
-      <c r="D1255" t="inlineStr"/>
-      <c r="E1255" t="inlineStr"/>
-      <c r="F1255" t="inlineStr"/>
-      <c r="G1255" t="inlineStr"/>
-      <c r="H1255" t="inlineStr"/>
-      <c r="I1255" t="inlineStr"/>
     </row>
     <row r="1256">
       <c r="A1256" t="inlineStr">
@@ -15901,13 +15607,6 @@
           <t>Sansevieria Laurentii</t>
         </is>
       </c>
-      <c r="C1256" t="inlineStr"/>
-      <c r="D1256" t="inlineStr"/>
-      <c r="E1256" t="inlineStr"/>
-      <c r="F1256" t="inlineStr"/>
-      <c r="G1256" t="inlineStr"/>
-      <c r="H1256" t="inlineStr"/>
-      <c r="I1256" t="inlineStr"/>
     </row>
     <row r="1257">
       <c r="A1257" t="inlineStr">
@@ -15920,13 +15619,6 @@
           <t>Epipremnum Aureum Saal</t>
         </is>
       </c>
-      <c r="C1257" t="inlineStr"/>
-      <c r="D1257" t="inlineStr"/>
-      <c r="E1257" t="inlineStr"/>
-      <c r="F1257" t="inlineStr"/>
-      <c r="G1257" t="inlineStr"/>
-      <c r="H1257" t="inlineStr"/>
-      <c r="I1257" t="inlineStr"/>
     </row>
     <row r="1258">
       <c r="A1258" t="inlineStr">
@@ -15939,13 +15631,6 @@
           <t>Monstera Deliciosa Variegata</t>
         </is>
       </c>
-      <c r="C1258" t="inlineStr"/>
-      <c r="D1258" t="inlineStr"/>
-      <c r="E1258" t="inlineStr"/>
-      <c r="F1258" t="inlineStr"/>
-      <c r="G1258" t="inlineStr"/>
-      <c r="H1258" t="inlineStr"/>
-      <c r="I1258" t="inlineStr"/>
     </row>
     <row r="1259">
       <c r="A1259" t="inlineStr">
@@ -15958,13 +15643,6 @@
           <t>Pachira Aquatica</t>
         </is>
       </c>
-      <c r="C1259" t="inlineStr"/>
-      <c r="D1259" t="inlineStr"/>
-      <c r="E1259" t="inlineStr"/>
-      <c r="F1259" t="inlineStr"/>
-      <c r="G1259" t="inlineStr"/>
-      <c r="H1259" t="inlineStr"/>
-      <c r="I1259" t="inlineStr"/>
     </row>
     <row r="1260">
       <c r="A1260" t="inlineStr">
@@ -15977,13 +15655,6 @@
           <t xml:space="preserve">Monstera Deliciosa </t>
         </is>
       </c>
-      <c r="C1260" t="inlineStr"/>
-      <c r="D1260" t="inlineStr"/>
-      <c r="E1260" t="inlineStr"/>
-      <c r="F1260" t="inlineStr"/>
-      <c r="G1260" t="inlineStr"/>
-      <c r="H1260" t="inlineStr"/>
-      <c r="I1260" t="inlineStr"/>
     </row>
     <row r="1261">
       <c r="A1261" t="inlineStr">
@@ -15996,13 +15667,6 @@
           <t>Philodendron Imperial Red</t>
         </is>
       </c>
-      <c r="C1261" t="inlineStr"/>
-      <c r="D1261" t="inlineStr"/>
-      <c r="E1261" t="inlineStr"/>
-      <c r="F1261" t="inlineStr"/>
-      <c r="G1261" t="inlineStr"/>
-      <c r="H1261" t="inlineStr"/>
-      <c r="I1261" t="inlineStr"/>
     </row>
     <row r="1262"/>
     <row r="1263">
@@ -16016,13 +15680,6 @@
           <t>Calathea Medalion</t>
         </is>
       </c>
-      <c r="C1263" t="inlineStr"/>
-      <c r="D1263" t="inlineStr"/>
-      <c r="E1263" t="inlineStr"/>
-      <c r="F1263" t="inlineStr"/>
-      <c r="G1263" t="inlineStr"/>
-      <c r="H1263" t="inlineStr"/>
-      <c r="I1263" t="inlineStr"/>
     </row>
     <row r="1264">
       <c r="A1264" t="inlineStr">
@@ -16035,13 +15692,6 @@
           <t>Epipremnum Aureum</t>
         </is>
       </c>
-      <c r="C1264" t="inlineStr"/>
-      <c r="D1264" t="inlineStr"/>
-      <c r="E1264" t="inlineStr"/>
-      <c r="F1264" t="inlineStr"/>
-      <c r="G1264" t="inlineStr"/>
-      <c r="H1264" t="inlineStr"/>
-      <c r="I1264" t="inlineStr"/>
     </row>
     <row r="1265">
       <c r="A1265" t="inlineStr">
@@ -16054,13 +15704,6 @@
           <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
-      <c r="C1265" t="inlineStr"/>
-      <c r="D1265" t="inlineStr"/>
-      <c r="E1265" t="inlineStr"/>
-      <c r="F1265" t="inlineStr"/>
-      <c r="G1265" t="inlineStr"/>
-      <c r="H1265" t="inlineStr"/>
-      <c r="I1265" t="inlineStr"/>
     </row>
     <row r="1266">
       <c r="A1266" t="inlineStr">
@@ -16073,13 +15716,6 @@
           <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
-      <c r="C1266" t="inlineStr"/>
-      <c r="D1266" t="inlineStr"/>
-      <c r="E1266" t="inlineStr"/>
-      <c r="F1266" t="inlineStr"/>
-      <c r="G1266" t="inlineStr"/>
-      <c r="H1266" t="inlineStr"/>
-      <c r="I1266" t="inlineStr"/>
     </row>
     <row r="1267">
       <c r="A1267" t="inlineStr">
@@ -16092,13 +15728,6 @@
           <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
-      <c r="C1267" t="inlineStr"/>
-      <c r="D1267" t="inlineStr"/>
-      <c r="E1267" t="inlineStr"/>
-      <c r="F1267" t="inlineStr"/>
-      <c r="G1267" t="inlineStr"/>
-      <c r="H1267" t="inlineStr"/>
-      <c r="I1267" t="inlineStr"/>
     </row>
     <row r="1268">
       <c r="A1268" t="inlineStr">
@@ -16111,13 +15740,6 @@
           <t>Monstera Adenossii</t>
         </is>
       </c>
-      <c r="C1268" t="inlineStr"/>
-      <c r="D1268" t="inlineStr"/>
-      <c r="E1268" t="inlineStr"/>
-      <c r="F1268" t="inlineStr"/>
-      <c r="G1268" t="inlineStr"/>
-      <c r="H1268" t="inlineStr"/>
-      <c r="I1268" t="inlineStr"/>
     </row>
     <row r="1269">
       <c r="A1269" t="inlineStr">
@@ -16130,13 +15752,6 @@
           <t>Ficus Elastica Abidjan</t>
         </is>
       </c>
-      <c r="C1269" t="inlineStr"/>
-      <c r="D1269" t="inlineStr"/>
-      <c r="E1269" t="inlineStr"/>
-      <c r="F1269" t="inlineStr"/>
-      <c r="G1269" t="inlineStr"/>
-      <c r="H1269" t="inlineStr"/>
-      <c r="I1269" t="inlineStr"/>
     </row>
     <row r="1270">
       <c r="A1270" t="inlineStr">
@@ -16149,13 +15764,6 @@
           <t>Peperomia Hope</t>
         </is>
       </c>
-      <c r="C1270" t="inlineStr"/>
-      <c r="D1270" t="inlineStr"/>
-      <c r="E1270" t="inlineStr"/>
-      <c r="F1270" t="inlineStr"/>
-      <c r="G1270" t="inlineStr"/>
-      <c r="H1270" t="inlineStr"/>
-      <c r="I1270" t="inlineStr"/>
     </row>
     <row r="1271">
       <c r="A1271" t="inlineStr">
@@ -16168,13 +15776,6 @@
           <t>Hoya Mathilde</t>
         </is>
       </c>
-      <c r="C1271" t="inlineStr"/>
-      <c r="D1271" t="inlineStr"/>
-      <c r="E1271" t="inlineStr"/>
-      <c r="F1271" t="inlineStr"/>
-      <c r="G1271" t="inlineStr"/>
-      <c r="H1271" t="inlineStr"/>
-      <c r="I1271" t="inlineStr"/>
     </row>
     <row r="1272">
       <c r="A1272" t="inlineStr">
@@ -16187,13 +15788,6 @@
           <t>Epipremnum Pinnatum Blue</t>
         </is>
       </c>
-      <c r="C1272" t="inlineStr"/>
-      <c r="D1272" t="inlineStr"/>
-      <c r="E1272" t="inlineStr"/>
-      <c r="F1272" t="inlineStr"/>
-      <c r="G1272" t="inlineStr"/>
-      <c r="H1272" t="inlineStr"/>
-      <c r="I1272" t="inlineStr"/>
     </row>
     <row r="1273">
       <c r="A1273" t="inlineStr">
@@ -16206,13 +15800,6 @@
           <t>Sansevieria Laurentii</t>
         </is>
       </c>
-      <c r="C1273" t="inlineStr"/>
-      <c r="D1273" t="inlineStr"/>
-      <c r="E1273" t="inlineStr"/>
-      <c r="F1273" t="inlineStr"/>
-      <c r="G1273" t="inlineStr"/>
-      <c r="H1273" t="inlineStr"/>
-      <c r="I1273" t="inlineStr"/>
     </row>
     <row r="1274">
       <c r="A1274" t="inlineStr">
@@ -16225,13 +15812,6 @@
           <t>Epipremnum Aureum Saal</t>
         </is>
       </c>
-      <c r="C1274" t="inlineStr"/>
-      <c r="D1274" t="inlineStr"/>
-      <c r="E1274" t="inlineStr"/>
-      <c r="F1274" t="inlineStr"/>
-      <c r="G1274" t="inlineStr"/>
-      <c r="H1274" t="inlineStr"/>
-      <c r="I1274" t="inlineStr"/>
     </row>
     <row r="1275">
       <c r="A1275" t="inlineStr">
@@ -16244,13 +15824,6 @@
           <t>Monstera Deliciosa Variegata</t>
         </is>
       </c>
-      <c r="C1275" t="inlineStr"/>
-      <c r="D1275" t="inlineStr"/>
-      <c r="E1275" t="inlineStr"/>
-      <c r="F1275" t="inlineStr"/>
-      <c r="G1275" t="inlineStr"/>
-      <c r="H1275" t="inlineStr"/>
-      <c r="I1275" t="inlineStr"/>
     </row>
     <row r="1276">
       <c r="A1276" t="inlineStr">
@@ -16263,13 +15836,6 @@
           <t>Pachira Aquatica</t>
         </is>
       </c>
-      <c r="C1276" t="inlineStr"/>
-      <c r="D1276" t="inlineStr"/>
-      <c r="E1276" t="inlineStr"/>
-      <c r="F1276" t="inlineStr"/>
-      <c r="G1276" t="inlineStr"/>
-      <c r="H1276" t="inlineStr"/>
-      <c r="I1276" t="inlineStr"/>
     </row>
     <row r="1277">
       <c r="A1277" t="inlineStr">
@@ -16282,13 +15848,6 @@
           <t xml:space="preserve">Monstera Deliciosa </t>
         </is>
       </c>
-      <c r="C1277" t="inlineStr"/>
-      <c r="D1277" t="inlineStr"/>
-      <c r="E1277" t="inlineStr"/>
-      <c r="F1277" t="inlineStr"/>
-      <c r="G1277" t="inlineStr"/>
-      <c r="H1277" t="inlineStr"/>
-      <c r="I1277" t="inlineStr"/>
     </row>
     <row r="1278">
       <c r="A1278" t="inlineStr">
@@ -16301,13 +15860,6 @@
           <t>Philodendron Imperial Red</t>
         </is>
       </c>
-      <c r="C1278" t="inlineStr"/>
-      <c r="D1278" t="inlineStr"/>
-      <c r="E1278" t="inlineStr"/>
-      <c r="F1278" t="inlineStr"/>
-      <c r="G1278" t="inlineStr"/>
-      <c r="H1278" t="inlineStr"/>
-      <c r="I1278" t="inlineStr"/>
     </row>
     <row r="1279"/>
     <row r="1280">
@@ -16321,13 +15873,6 @@
           <t>Calathea Medalion</t>
         </is>
       </c>
-      <c r="C1280" t="inlineStr"/>
-      <c r="D1280" t="inlineStr"/>
-      <c r="E1280" t="inlineStr"/>
-      <c r="F1280" t="inlineStr"/>
-      <c r="G1280" t="inlineStr"/>
-      <c r="H1280" t="inlineStr"/>
-      <c r="I1280" t="inlineStr"/>
     </row>
     <row r="1281">
       <c r="A1281" t="inlineStr">
@@ -16340,13 +15885,6 @@
           <t>Epipremnum Aureum</t>
         </is>
       </c>
-      <c r="C1281" t="inlineStr"/>
-      <c r="D1281" t="inlineStr"/>
-      <c r="E1281" t="inlineStr"/>
-      <c r="F1281" t="inlineStr"/>
-      <c r="G1281" t="inlineStr"/>
-      <c r="H1281" t="inlineStr"/>
-      <c r="I1281" t="inlineStr"/>
     </row>
     <row r="1282">
       <c r="A1282" t="inlineStr">
@@ -16359,13 +15897,6 @@
           <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
-      <c r="C1282" t="inlineStr"/>
-      <c r="D1282" t="inlineStr"/>
-      <c r="E1282" t="inlineStr"/>
-      <c r="F1282" t="inlineStr"/>
-      <c r="G1282" t="inlineStr"/>
-      <c r="H1282" t="inlineStr"/>
-      <c r="I1282" t="inlineStr"/>
     </row>
     <row r="1283">
       <c r="A1283" t="inlineStr">
@@ -16378,13 +15909,6 @@
           <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
-      <c r="C1283" t="inlineStr"/>
-      <c r="D1283" t="inlineStr"/>
-      <c r="E1283" t="inlineStr"/>
-      <c r="F1283" t="inlineStr"/>
-      <c r="G1283" t="inlineStr"/>
-      <c r="H1283" t="inlineStr"/>
-      <c r="I1283" t="inlineStr"/>
     </row>
     <row r="1284">
       <c r="A1284" t="inlineStr">
@@ -16397,13 +15921,6 @@
           <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
-      <c r="C1284" t="inlineStr"/>
-      <c r="D1284" t="inlineStr"/>
-      <c r="E1284" t="inlineStr"/>
-      <c r="F1284" t="inlineStr"/>
-      <c r="G1284" t="inlineStr"/>
-      <c r="H1284" t="inlineStr"/>
-      <c r="I1284" t="inlineStr"/>
     </row>
     <row r="1285">
       <c r="A1285" t="inlineStr">
@@ -16416,13 +15933,6 @@
           <t>Monstera Adenossii</t>
         </is>
       </c>
-      <c r="C1285" t="inlineStr"/>
-      <c r="D1285" t="inlineStr"/>
-      <c r="E1285" t="inlineStr"/>
-      <c r="F1285" t="inlineStr"/>
-      <c r="G1285" t="inlineStr"/>
-      <c r="H1285" t="inlineStr"/>
-      <c r="I1285" t="inlineStr"/>
     </row>
     <row r="1286">
       <c r="A1286" t="inlineStr">
@@ -16435,13 +15945,6 @@
           <t>Ficus Elastica Abidjan</t>
         </is>
       </c>
-      <c r="C1286" t="inlineStr"/>
-      <c r="D1286" t="inlineStr"/>
-      <c r="E1286" t="inlineStr"/>
-      <c r="F1286" t="inlineStr"/>
-      <c r="G1286" t="inlineStr"/>
-      <c r="H1286" t="inlineStr"/>
-      <c r="I1286" t="inlineStr"/>
     </row>
     <row r="1287">
       <c r="A1287" t="inlineStr">
@@ -16454,13 +15957,6 @@
           <t>Peperomia Hope</t>
         </is>
       </c>
-      <c r="C1287" t="inlineStr"/>
-      <c r="D1287" t="inlineStr"/>
-      <c r="E1287" t="inlineStr"/>
-      <c r="F1287" t="inlineStr"/>
-      <c r="G1287" t="inlineStr"/>
-      <c r="H1287" t="inlineStr"/>
-      <c r="I1287" t="inlineStr"/>
     </row>
     <row r="1288">
       <c r="A1288" t="inlineStr">
@@ -16473,13 +15969,6 @@
           <t>Hoya Mathilde</t>
         </is>
       </c>
-      <c r="C1288" t="inlineStr"/>
-      <c r="D1288" t="inlineStr"/>
-      <c r="E1288" t="inlineStr"/>
-      <c r="F1288" t="inlineStr"/>
-      <c r="G1288" t="inlineStr"/>
-      <c r="H1288" t="inlineStr"/>
-      <c r="I1288" t="inlineStr"/>
     </row>
     <row r="1289">
       <c r="A1289" t="inlineStr">
@@ -16492,13 +15981,6 @@
           <t>Epipremnum Pinnatum Blue</t>
         </is>
       </c>
-      <c r="C1289" t="inlineStr"/>
-      <c r="D1289" t="inlineStr"/>
-      <c r="E1289" t="inlineStr"/>
-      <c r="F1289" t="inlineStr"/>
-      <c r="G1289" t="inlineStr"/>
-      <c r="H1289" t="inlineStr"/>
-      <c r="I1289" t="inlineStr"/>
     </row>
     <row r="1290">
       <c r="A1290" t="inlineStr">
@@ -16511,13 +15993,6 @@
           <t>Sansevieria Laurentii</t>
         </is>
       </c>
-      <c r="C1290" t="inlineStr"/>
-      <c r="D1290" t="inlineStr"/>
-      <c r="E1290" t="inlineStr"/>
-      <c r="F1290" t="inlineStr"/>
-      <c r="G1290" t="inlineStr"/>
-      <c r="H1290" t="inlineStr"/>
-      <c r="I1290" t="inlineStr"/>
     </row>
     <row r="1291">
       <c r="A1291" t="inlineStr">
@@ -16530,13 +16005,6 @@
           <t>Epipremnum Aureum Saal</t>
         </is>
       </c>
-      <c r="C1291" t="inlineStr"/>
-      <c r="D1291" t="inlineStr"/>
-      <c r="E1291" t="inlineStr"/>
-      <c r="F1291" t="inlineStr"/>
-      <c r="G1291" t="inlineStr"/>
-      <c r="H1291" t="inlineStr"/>
-      <c r="I1291" t="inlineStr"/>
     </row>
     <row r="1292">
       <c r="A1292" t="inlineStr">
@@ -16549,13 +16017,6 @@
           <t>Monstera Deliciosa Variegata</t>
         </is>
       </c>
-      <c r="C1292" t="inlineStr"/>
-      <c r="D1292" t="inlineStr"/>
-      <c r="E1292" t="inlineStr"/>
-      <c r="F1292" t="inlineStr"/>
-      <c r="G1292" t="inlineStr"/>
-      <c r="H1292" t="inlineStr"/>
-      <c r="I1292" t="inlineStr"/>
     </row>
     <row r="1293">
       <c r="A1293" t="inlineStr">
@@ -16568,13 +16029,6 @@
           <t>Pachira Aquatica</t>
         </is>
       </c>
-      <c r="C1293" t="inlineStr"/>
-      <c r="D1293" t="inlineStr"/>
-      <c r="E1293" t="inlineStr"/>
-      <c r="F1293" t="inlineStr"/>
-      <c r="G1293" t="inlineStr"/>
-      <c r="H1293" t="inlineStr"/>
-      <c r="I1293" t="inlineStr"/>
     </row>
     <row r="1294">
       <c r="A1294" t="inlineStr">
@@ -16587,13 +16041,6 @@
           <t xml:space="preserve">Monstera Deliciosa </t>
         </is>
       </c>
-      <c r="C1294" t="inlineStr"/>
-      <c r="D1294" t="inlineStr"/>
-      <c r="E1294" t="inlineStr"/>
-      <c r="F1294" t="inlineStr"/>
-      <c r="G1294" t="inlineStr"/>
-      <c r="H1294" t="inlineStr"/>
-      <c r="I1294" t="inlineStr"/>
     </row>
     <row r="1295">
       <c r="A1295" t="inlineStr">
@@ -16606,13 +16053,6 @@
           <t>Philodendron Imperial Red</t>
         </is>
       </c>
-      <c r="C1295" t="inlineStr"/>
-      <c r="D1295" t="inlineStr"/>
-      <c r="E1295" t="inlineStr"/>
-      <c r="F1295" t="inlineStr"/>
-      <c r="G1295" t="inlineStr"/>
-      <c r="H1295" t="inlineStr"/>
-      <c r="I1295" t="inlineStr"/>
     </row>
     <row r="1296"/>
     <row r="1297">
@@ -16626,13 +16066,6 @@
           <t>Calathea Medalion</t>
         </is>
       </c>
-      <c r="C1297" t="inlineStr"/>
-      <c r="D1297" t="inlineStr"/>
-      <c r="E1297" t="inlineStr"/>
-      <c r="F1297" t="inlineStr"/>
-      <c r="G1297" t="inlineStr"/>
-      <c r="H1297" t="inlineStr"/>
-      <c r="I1297" t="inlineStr"/>
     </row>
     <row r="1298">
       <c r="A1298" t="inlineStr">
@@ -16645,13 +16078,6 @@
           <t>Epipremnum Aureum</t>
         </is>
       </c>
-      <c r="C1298" t="inlineStr"/>
-      <c r="D1298" t="inlineStr"/>
-      <c r="E1298" t="inlineStr"/>
-      <c r="F1298" t="inlineStr"/>
-      <c r="G1298" t="inlineStr"/>
-      <c r="H1298" t="inlineStr"/>
-      <c r="I1298" t="inlineStr"/>
     </row>
     <row r="1299">
       <c r="A1299" t="inlineStr">
@@ -16664,13 +16090,6 @@
           <t xml:space="preserve">Philodendron Scandens Micans </t>
         </is>
       </c>
-      <c r="C1299" t="inlineStr"/>
-      <c r="D1299" t="inlineStr"/>
-      <c r="E1299" t="inlineStr"/>
-      <c r="F1299" t="inlineStr"/>
-      <c r="G1299" t="inlineStr"/>
-      <c r="H1299" t="inlineStr"/>
-      <c r="I1299" t="inlineStr"/>
     </row>
     <row r="1300">
       <c r="A1300" t="inlineStr">
@@ -16683,13 +16102,6 @@
           <t>Scindapsus Treubii Moonlight</t>
         </is>
       </c>
-      <c r="C1300" t="inlineStr"/>
-      <c r="D1300" t="inlineStr"/>
-      <c r="E1300" t="inlineStr"/>
-      <c r="F1300" t="inlineStr"/>
-      <c r="G1300" t="inlineStr"/>
-      <c r="H1300" t="inlineStr"/>
-      <c r="I1300" t="inlineStr"/>
     </row>
     <row r="1301">
       <c r="A1301" t="inlineStr">
@@ -16702,13 +16114,6 @@
           <t>Philodendron Hedaracium Brasil</t>
         </is>
       </c>
-      <c r="C1301" t="inlineStr"/>
-      <c r="D1301" t="inlineStr"/>
-      <c r="E1301" t="inlineStr"/>
-      <c r="F1301" t="inlineStr"/>
-      <c r="G1301" t="inlineStr"/>
-      <c r="H1301" t="inlineStr"/>
-      <c r="I1301" t="inlineStr"/>
     </row>
     <row r="1302">
       <c r="A1302" t="inlineStr">
@@ -16721,13 +16126,6 @@
           <t>Monstera Adenossii</t>
         </is>
       </c>
-      <c r="C1302" t="inlineStr"/>
-      <c r="D1302" t="inlineStr"/>
-      <c r="E1302" t="inlineStr"/>
-      <c r="F1302" t="inlineStr"/>
-      <c r="G1302" t="inlineStr"/>
-      <c r="H1302" t="inlineStr"/>
-      <c r="I1302" t="inlineStr"/>
     </row>
     <row r="1303">
       <c r="A1303" t="inlineStr">
@@ -16740,13 +16138,6 @@
           <t>Ficus Elastica Abidjan</t>
         </is>
       </c>
-      <c r="C1303" t="inlineStr"/>
-      <c r="D1303" t="inlineStr"/>
-      <c r="E1303" t="inlineStr"/>
-      <c r="F1303" t="inlineStr"/>
-      <c r="G1303" t="inlineStr"/>
-      <c r="H1303" t="inlineStr"/>
-      <c r="I1303" t="inlineStr"/>
     </row>
     <row r="1304">
       <c r="A1304" t="inlineStr">
@@ -16759,13 +16150,6 @@
           <t>Peperomia Hope</t>
         </is>
       </c>
-      <c r="C1304" t="inlineStr"/>
-      <c r="D1304" t="inlineStr"/>
-      <c r="E1304" t="inlineStr"/>
-      <c r="F1304" t="inlineStr"/>
-      <c r="G1304" t="inlineStr"/>
-      <c r="H1304" t="inlineStr"/>
-      <c r="I1304" t="inlineStr"/>
     </row>
     <row r="1305">
       <c r="A1305" t="inlineStr">
@@ -16778,13 +16162,6 @@
           <t>Hoya Mathilde</t>
         </is>
       </c>
-      <c r="C1305" t="inlineStr"/>
-      <c r="D1305" t="inlineStr"/>
-      <c r="E1305" t="inlineStr"/>
-      <c r="F1305" t="inlineStr"/>
-      <c r="G1305" t="inlineStr"/>
-      <c r="H1305" t="inlineStr"/>
-      <c r="I1305" t="inlineStr"/>
     </row>
     <row r="1306">
       <c r="A1306" t="inlineStr">
@@ -16797,13 +16174,6 @@
           <t>Epipremnum Pinnatum Blue</t>
         </is>
       </c>
-      <c r="C1306" t="inlineStr"/>
-      <c r="D1306" t="inlineStr"/>
-      <c r="E1306" t="inlineStr"/>
-      <c r="F1306" t="inlineStr"/>
-      <c r="G1306" t="inlineStr"/>
-      <c r="H1306" t="inlineStr"/>
-      <c r="I1306" t="inlineStr"/>
     </row>
     <row r="1307">
       <c r="A1307" t="inlineStr">
@@ -16816,13 +16186,6 @@
           <t>Sansevieria Laurentii</t>
         </is>
       </c>
-      <c r="C1307" t="inlineStr"/>
-      <c r="D1307" t="inlineStr"/>
-      <c r="E1307" t="inlineStr"/>
-      <c r="F1307" t="inlineStr"/>
-      <c r="G1307" t="inlineStr"/>
-      <c r="H1307" t="inlineStr"/>
-      <c r="I1307" t="inlineStr"/>
     </row>
     <row r="1308">
       <c r="A1308" t="inlineStr">
@@ -16835,13 +16198,6 @@
           <t>Epipremnum Aureum Saal</t>
         </is>
       </c>
-      <c r="C1308" t="inlineStr"/>
-      <c r="D1308" t="inlineStr"/>
-      <c r="E1308" t="inlineStr"/>
-      <c r="F1308" t="inlineStr"/>
-      <c r="G1308" t="inlineStr"/>
-      <c r="H1308" t="inlineStr"/>
-      <c r="I1308" t="inlineStr"/>
     </row>
     <row r="1309">
       <c r="A1309" t="inlineStr">
@@ -16854,13 +16210,6 @@
           <t>Monstera Deliciosa Variegata</t>
         </is>
       </c>
-      <c r="C1309" t="inlineStr"/>
-      <c r="D1309" t="inlineStr"/>
-      <c r="E1309" t="inlineStr"/>
-      <c r="F1309" t="inlineStr"/>
-      <c r="G1309" t="inlineStr"/>
-      <c r="H1309" t="inlineStr"/>
-      <c r="I1309" t="inlineStr"/>
     </row>
     <row r="1310">
       <c r="A1310" t="inlineStr">
@@ -16873,13 +16222,6 @@
           <t>Pachira Aquatica</t>
         </is>
       </c>
-      <c r="C1310" t="inlineStr"/>
-      <c r="D1310" t="inlineStr"/>
-      <c r="E1310" t="inlineStr"/>
-      <c r="F1310" t="inlineStr"/>
-      <c r="G1310" t="inlineStr"/>
-      <c r="H1310" t="inlineStr"/>
-      <c r="I1310" t="inlineStr"/>
     </row>
     <row r="1311">
       <c r="A1311" t="inlineStr">
@@ -16892,13 +16234,6 @@
           <t xml:space="preserve">Monstera Deliciosa </t>
         </is>
       </c>
-      <c r="C1311" t="inlineStr"/>
-      <c r="D1311" t="inlineStr"/>
-      <c r="E1311" t="inlineStr"/>
-      <c r="F1311" t="inlineStr"/>
-      <c r="G1311" t="inlineStr"/>
-      <c r="H1311" t="inlineStr"/>
-      <c r="I1311" t="inlineStr"/>
     </row>
     <row r="1312">
       <c r="A1312" t="inlineStr">
@@ -16911,15 +16246,1533 @@
           <t>Philodendron Imperial Red</t>
         </is>
       </c>
-      <c r="C1312" t="inlineStr"/>
-      <c r="D1312" t="inlineStr"/>
-      <c r="E1312" t="inlineStr"/>
-      <c r="F1312" t="inlineStr"/>
-      <c r="G1312" t="inlineStr"/>
-      <c r="H1312" t="inlineStr"/>
-      <c r="I1312" t="inlineStr"/>
     </row>
     <row r="1313"/>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr"/>
+      <c r="D1314" t="inlineStr"/>
+      <c r="E1314" t="inlineStr"/>
+      <c r="F1314" t="inlineStr"/>
+      <c r="G1314" t="inlineStr"/>
+      <c r="H1314" t="inlineStr"/>
+      <c r="I1314" t="inlineStr"/>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr"/>
+      <c r="D1315" t="inlineStr"/>
+      <c r="E1315" t="inlineStr"/>
+      <c r="F1315" t="inlineStr"/>
+      <c r="G1315" t="inlineStr"/>
+      <c r="H1315" t="inlineStr"/>
+      <c r="I1315" t="inlineStr"/>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr"/>
+      <c r="D1316" t="inlineStr"/>
+      <c r="E1316" t="inlineStr"/>
+      <c r="F1316" t="inlineStr"/>
+      <c r="G1316" t="inlineStr"/>
+      <c r="H1316" t="inlineStr"/>
+      <c r="I1316" t="inlineStr"/>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr"/>
+      <c r="D1317" t="inlineStr"/>
+      <c r="E1317" t="inlineStr"/>
+      <c r="F1317" t="inlineStr"/>
+      <c r="G1317" t="inlineStr"/>
+      <c r="H1317" t="inlineStr"/>
+      <c r="I1317" t="inlineStr"/>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr"/>
+      <c r="D1318" t="inlineStr"/>
+      <c r="E1318" t="inlineStr"/>
+      <c r="F1318" t="inlineStr"/>
+      <c r="G1318" t="inlineStr"/>
+      <c r="H1318" t="inlineStr"/>
+      <c r="I1318" t="inlineStr"/>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr"/>
+      <c r="D1319" t="inlineStr"/>
+      <c r="E1319" t="inlineStr"/>
+      <c r="F1319" t="inlineStr"/>
+      <c r="G1319" t="inlineStr"/>
+      <c r="H1319" t="inlineStr"/>
+      <c r="I1319" t="inlineStr"/>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr"/>
+      <c r="D1320" t="inlineStr"/>
+      <c r="E1320" t="inlineStr"/>
+      <c r="F1320" t="inlineStr"/>
+      <c r="G1320" t="inlineStr"/>
+      <c r="H1320" t="inlineStr"/>
+      <c r="I1320" t="inlineStr"/>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr"/>
+      <c r="D1321" t="inlineStr"/>
+      <c r="E1321" t="inlineStr"/>
+      <c r="F1321" t="inlineStr"/>
+      <c r="G1321" t="inlineStr"/>
+      <c r="H1321" t="inlineStr"/>
+      <c r="I1321" t="inlineStr"/>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr"/>
+      <c r="D1322" t="inlineStr"/>
+      <c r="E1322" t="inlineStr"/>
+      <c r="F1322" t="inlineStr"/>
+      <c r="G1322" t="inlineStr"/>
+      <c r="H1322" t="inlineStr"/>
+      <c r="I1322" t="inlineStr"/>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Epipremnum Pinnatum Blue</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr"/>
+      <c r="D1323" t="inlineStr"/>
+      <c r="E1323" t="inlineStr"/>
+      <c r="F1323" t="inlineStr"/>
+      <c r="G1323" t="inlineStr"/>
+      <c r="H1323" t="inlineStr"/>
+      <c r="I1323" t="inlineStr"/>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Sansevieria Laurentii</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr"/>
+      <c r="D1324" t="inlineStr"/>
+      <c r="E1324" t="inlineStr"/>
+      <c r="F1324" t="inlineStr"/>
+      <c r="G1324" t="inlineStr"/>
+      <c r="H1324" t="inlineStr"/>
+      <c r="I1324" t="inlineStr"/>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum Saal</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr"/>
+      <c r="D1325" t="inlineStr"/>
+      <c r="E1325" t="inlineStr"/>
+      <c r="F1325" t="inlineStr"/>
+      <c r="G1325" t="inlineStr"/>
+      <c r="H1325" t="inlineStr"/>
+      <c r="I1325" t="inlineStr"/>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Monstera Deliciosa Variegata</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr"/>
+      <c r="D1326" t="inlineStr"/>
+      <c r="E1326" t="inlineStr"/>
+      <c r="F1326" t="inlineStr"/>
+      <c r="G1326" t="inlineStr"/>
+      <c r="H1326" t="inlineStr"/>
+      <c r="I1326" t="inlineStr"/>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Pachira Aquatica</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr"/>
+      <c r="D1327" t="inlineStr"/>
+      <c r="E1327" t="inlineStr"/>
+      <c r="F1327" t="inlineStr"/>
+      <c r="G1327" t="inlineStr"/>
+      <c r="H1327" t="inlineStr"/>
+      <c r="I1327" t="inlineStr"/>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monstera Deliciosa </t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr"/>
+      <c r="D1328" t="inlineStr"/>
+      <c r="E1328" t="inlineStr"/>
+      <c r="F1328" t="inlineStr"/>
+      <c r="G1328" t="inlineStr"/>
+      <c r="H1328" t="inlineStr"/>
+      <c r="I1328" t="inlineStr"/>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>05.08.2025</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Philodendron Imperial Red</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr"/>
+      <c r="D1329" t="inlineStr"/>
+      <c r="E1329" t="inlineStr"/>
+      <c r="F1329" t="inlineStr"/>
+      <c r="G1329" t="inlineStr"/>
+      <c r="H1329" t="inlineStr"/>
+      <c r="I1329" t="inlineStr"/>
+    </row>
+    <row r="1330"/>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr"/>
+      <c r="D1331" t="inlineStr"/>
+      <c r="E1331" t="inlineStr"/>
+      <c r="F1331" t="inlineStr"/>
+      <c r="G1331" t="inlineStr"/>
+      <c r="H1331" t="inlineStr"/>
+      <c r="I1331" t="inlineStr"/>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr"/>
+      <c r="D1332" t="inlineStr"/>
+      <c r="E1332" t="inlineStr"/>
+      <c r="F1332" t="inlineStr"/>
+      <c r="G1332" t="inlineStr"/>
+      <c r="H1332" t="inlineStr"/>
+      <c r="I1332" t="inlineStr"/>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr"/>
+      <c r="D1333" t="inlineStr"/>
+      <c r="E1333" t="inlineStr"/>
+      <c r="F1333" t="inlineStr"/>
+      <c r="G1333" t="inlineStr"/>
+      <c r="H1333" t="inlineStr"/>
+      <c r="I1333" t="inlineStr"/>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr"/>
+      <c r="D1334" t="inlineStr"/>
+      <c r="E1334" t="inlineStr"/>
+      <c r="F1334" t="inlineStr"/>
+      <c r="G1334" t="inlineStr"/>
+      <c r="H1334" t="inlineStr"/>
+      <c r="I1334" t="inlineStr"/>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr"/>
+      <c r="D1335" t="inlineStr"/>
+      <c r="E1335" t="inlineStr"/>
+      <c r="F1335" t="inlineStr"/>
+      <c r="G1335" t="inlineStr"/>
+      <c r="H1335" t="inlineStr"/>
+      <c r="I1335" t="inlineStr"/>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr"/>
+      <c r="D1336" t="inlineStr"/>
+      <c r="E1336" t="inlineStr"/>
+      <c r="F1336" t="inlineStr"/>
+      <c r="G1336" t="inlineStr"/>
+      <c r="H1336" t="inlineStr"/>
+      <c r="I1336" t="inlineStr"/>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr"/>
+      <c r="D1337" t="inlineStr"/>
+      <c r="E1337" t="inlineStr"/>
+      <c r="F1337" t="inlineStr"/>
+      <c r="G1337" t="inlineStr"/>
+      <c r="H1337" t="inlineStr"/>
+      <c r="I1337" t="inlineStr"/>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr"/>
+      <c r="D1338" t="inlineStr"/>
+      <c r="E1338" t="inlineStr"/>
+      <c r="F1338" t="inlineStr"/>
+      <c r="G1338" t="inlineStr"/>
+      <c r="H1338" t="inlineStr"/>
+      <c r="I1338" t="inlineStr"/>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr"/>
+      <c r="D1339" t="inlineStr"/>
+      <c r="E1339" t="inlineStr"/>
+      <c r="F1339" t="inlineStr"/>
+      <c r="G1339" t="inlineStr"/>
+      <c r="H1339" t="inlineStr"/>
+      <c r="I1339" t="inlineStr"/>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Epipremnum Pinnatum Blue</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr"/>
+      <c r="D1340" t="inlineStr"/>
+      <c r="E1340" t="inlineStr"/>
+      <c r="F1340" t="inlineStr"/>
+      <c r="G1340" t="inlineStr"/>
+      <c r="H1340" t="inlineStr"/>
+      <c r="I1340" t="inlineStr"/>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Sansevieria Laurentii</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr"/>
+      <c r="D1341" t="inlineStr"/>
+      <c r="E1341" t="inlineStr"/>
+      <c r="F1341" t="inlineStr"/>
+      <c r="G1341" t="inlineStr"/>
+      <c r="H1341" t="inlineStr"/>
+      <c r="I1341" t="inlineStr"/>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum Saal</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr"/>
+      <c r="D1342" t="inlineStr"/>
+      <c r="E1342" t="inlineStr"/>
+      <c r="F1342" t="inlineStr"/>
+      <c r="G1342" t="inlineStr"/>
+      <c r="H1342" t="inlineStr"/>
+      <c r="I1342" t="inlineStr"/>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Monstera Deliciosa Variegata</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr"/>
+      <c r="D1343" t="inlineStr"/>
+      <c r="E1343" t="inlineStr"/>
+      <c r="F1343" t="inlineStr"/>
+      <c r="G1343" t="inlineStr"/>
+      <c r="H1343" t="inlineStr"/>
+      <c r="I1343" t="inlineStr"/>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Pachira Aquatica</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr"/>
+      <c r="D1344" t="inlineStr"/>
+      <c r="E1344" t="inlineStr"/>
+      <c r="F1344" t="inlineStr"/>
+      <c r="G1344" t="inlineStr"/>
+      <c r="H1344" t="inlineStr"/>
+      <c r="I1344" t="inlineStr"/>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monstera Deliciosa </t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr"/>
+      <c r="D1345" t="inlineStr"/>
+      <c r="E1345" t="inlineStr"/>
+      <c r="F1345" t="inlineStr"/>
+      <c r="G1345" t="inlineStr"/>
+      <c r="H1345" t="inlineStr"/>
+      <c r="I1345" t="inlineStr"/>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>09.08.2025</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Philodendron Imperial Red</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr"/>
+      <c r="D1346" t="inlineStr"/>
+      <c r="E1346" t="inlineStr"/>
+      <c r="F1346" t="inlineStr"/>
+      <c r="G1346" t="inlineStr"/>
+      <c r="H1346" t="inlineStr"/>
+      <c r="I1346" t="inlineStr"/>
+    </row>
+    <row r="1347"/>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr"/>
+      <c r="D1348" t="inlineStr"/>
+      <c r="E1348" t="inlineStr"/>
+      <c r="F1348" t="inlineStr"/>
+      <c r="G1348" t="inlineStr"/>
+      <c r="H1348" t="inlineStr"/>
+      <c r="I1348" t="inlineStr"/>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr"/>
+      <c r="D1349" t="inlineStr"/>
+      <c r="E1349" t="inlineStr"/>
+      <c r="F1349" t="inlineStr"/>
+      <c r="G1349" t="inlineStr"/>
+      <c r="H1349" t="inlineStr"/>
+      <c r="I1349" t="inlineStr"/>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr"/>
+      <c r="D1350" t="inlineStr"/>
+      <c r="E1350" t="inlineStr"/>
+      <c r="F1350" t="inlineStr"/>
+      <c r="G1350" t="inlineStr"/>
+      <c r="H1350" t="inlineStr"/>
+      <c r="I1350" t="inlineStr"/>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr"/>
+      <c r="D1351" t="inlineStr"/>
+      <c r="E1351" t="inlineStr"/>
+      <c r="F1351" t="inlineStr"/>
+      <c r="G1351" t="inlineStr"/>
+      <c r="H1351" t="inlineStr"/>
+      <c r="I1351" t="inlineStr"/>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr"/>
+      <c r="D1352" t="inlineStr"/>
+      <c r="E1352" t="inlineStr"/>
+      <c r="F1352" t="inlineStr"/>
+      <c r="G1352" t="inlineStr"/>
+      <c r="H1352" t="inlineStr"/>
+      <c r="I1352" t="inlineStr"/>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr"/>
+      <c r="D1353" t="inlineStr"/>
+      <c r="E1353" t="inlineStr"/>
+      <c r="F1353" t="inlineStr"/>
+      <c r="G1353" t="inlineStr"/>
+      <c r="H1353" t="inlineStr"/>
+      <c r="I1353" t="inlineStr"/>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr"/>
+      <c r="D1354" t="inlineStr"/>
+      <c r="E1354" t="inlineStr"/>
+      <c r="F1354" t="inlineStr"/>
+      <c r="G1354" t="inlineStr"/>
+      <c r="H1354" t="inlineStr"/>
+      <c r="I1354" t="inlineStr"/>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr"/>
+      <c r="D1355" t="inlineStr"/>
+      <c r="E1355" t="inlineStr"/>
+      <c r="F1355" t="inlineStr"/>
+      <c r="G1355" t="inlineStr"/>
+      <c r="H1355" t="inlineStr"/>
+      <c r="I1355" t="inlineStr"/>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr"/>
+      <c r="D1356" t="inlineStr"/>
+      <c r="E1356" t="inlineStr"/>
+      <c r="F1356" t="inlineStr"/>
+      <c r="G1356" t="inlineStr"/>
+      <c r="H1356" t="inlineStr"/>
+      <c r="I1356" t="inlineStr"/>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Epipremnum Pinnatum Blue</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr"/>
+      <c r="D1357" t="inlineStr"/>
+      <c r="E1357" t="inlineStr"/>
+      <c r="F1357" t="inlineStr"/>
+      <c r="G1357" t="inlineStr"/>
+      <c r="H1357" t="inlineStr"/>
+      <c r="I1357" t="inlineStr"/>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Sansevieria Laurentii</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr"/>
+      <c r="D1358" t="inlineStr"/>
+      <c r="E1358" t="inlineStr"/>
+      <c r="F1358" t="inlineStr"/>
+      <c r="G1358" t="inlineStr"/>
+      <c r="H1358" t="inlineStr"/>
+      <c r="I1358" t="inlineStr"/>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum Saal</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr"/>
+      <c r="D1359" t="inlineStr"/>
+      <c r="E1359" t="inlineStr"/>
+      <c r="F1359" t="inlineStr"/>
+      <c r="G1359" t="inlineStr"/>
+      <c r="H1359" t="inlineStr"/>
+      <c r="I1359" t="inlineStr"/>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Monstera Deliciosa Variegata</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr"/>
+      <c r="D1360" t="inlineStr"/>
+      <c r="E1360" t="inlineStr"/>
+      <c r="F1360" t="inlineStr"/>
+      <c r="G1360" t="inlineStr"/>
+      <c r="H1360" t="inlineStr"/>
+      <c r="I1360" t="inlineStr"/>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Pachira Aquatica</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr"/>
+      <c r="D1361" t="inlineStr"/>
+      <c r="E1361" t="inlineStr"/>
+      <c r="F1361" t="inlineStr"/>
+      <c r="G1361" t="inlineStr"/>
+      <c r="H1361" t="inlineStr"/>
+      <c r="I1361" t="inlineStr"/>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monstera Deliciosa </t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr"/>
+      <c r="D1362" t="inlineStr"/>
+      <c r="E1362" t="inlineStr"/>
+      <c r="F1362" t="inlineStr"/>
+      <c r="G1362" t="inlineStr"/>
+      <c r="H1362" t="inlineStr"/>
+      <c r="I1362" t="inlineStr"/>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>10.08.2025</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Philodendron Imperial Red</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr"/>
+      <c r="D1363" t="inlineStr"/>
+      <c r="E1363" t="inlineStr"/>
+      <c r="F1363" t="inlineStr"/>
+      <c r="G1363" t="inlineStr"/>
+      <c r="H1363" t="inlineStr"/>
+      <c r="I1363" t="inlineStr"/>
+    </row>
+    <row r="1364"/>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr"/>
+      <c r="D1365" t="inlineStr"/>
+      <c r="E1365" t="inlineStr"/>
+      <c r="F1365" t="inlineStr"/>
+      <c r="G1365" t="inlineStr"/>
+      <c r="H1365" t="inlineStr"/>
+      <c r="I1365" t="inlineStr"/>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr"/>
+      <c r="D1366" t="inlineStr"/>
+      <c r="E1366" t="inlineStr"/>
+      <c r="F1366" t="inlineStr"/>
+      <c r="G1366" t="inlineStr"/>
+      <c r="H1366" t="inlineStr"/>
+      <c r="I1366" t="inlineStr"/>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr"/>
+      <c r="D1367" t="inlineStr"/>
+      <c r="E1367" t="inlineStr"/>
+      <c r="F1367" t="inlineStr"/>
+      <c r="G1367" t="inlineStr"/>
+      <c r="H1367" t="inlineStr"/>
+      <c r="I1367" t="inlineStr"/>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr"/>
+      <c r="D1368" t="inlineStr"/>
+      <c r="E1368" t="inlineStr"/>
+      <c r="F1368" t="inlineStr"/>
+      <c r="G1368" t="inlineStr"/>
+      <c r="H1368" t="inlineStr"/>
+      <c r="I1368" t="inlineStr"/>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr"/>
+      <c r="D1369" t="inlineStr"/>
+      <c r="E1369" t="inlineStr"/>
+      <c r="F1369" t="inlineStr"/>
+      <c r="G1369" t="inlineStr"/>
+      <c r="H1369" t="inlineStr"/>
+      <c r="I1369" t="inlineStr"/>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr"/>
+      <c r="D1370" t="inlineStr"/>
+      <c r="E1370" t="inlineStr"/>
+      <c r="F1370" t="inlineStr"/>
+      <c r="G1370" t="inlineStr"/>
+      <c r="H1370" t="inlineStr"/>
+      <c r="I1370" t="inlineStr"/>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr"/>
+      <c r="D1371" t="inlineStr"/>
+      <c r="E1371" t="inlineStr"/>
+      <c r="F1371" t="inlineStr"/>
+      <c r="G1371" t="inlineStr"/>
+      <c r="H1371" t="inlineStr"/>
+      <c r="I1371" t="inlineStr"/>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr"/>
+      <c r="D1372" t="inlineStr"/>
+      <c r="E1372" t="inlineStr"/>
+      <c r="F1372" t="inlineStr"/>
+      <c r="G1372" t="inlineStr"/>
+      <c r="H1372" t="inlineStr"/>
+      <c r="I1372" t="inlineStr"/>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr"/>
+      <c r="D1373" t="inlineStr"/>
+      <c r="E1373" t="inlineStr"/>
+      <c r="F1373" t="inlineStr"/>
+      <c r="G1373" t="inlineStr"/>
+      <c r="H1373" t="inlineStr"/>
+      <c r="I1373" t="inlineStr"/>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Epipremnum Pinnatum Blue</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr"/>
+      <c r="D1374" t="inlineStr"/>
+      <c r="E1374" t="inlineStr"/>
+      <c r="F1374" t="inlineStr"/>
+      <c r="G1374" t="inlineStr"/>
+      <c r="H1374" t="inlineStr"/>
+      <c r="I1374" t="inlineStr"/>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Sansevieria Laurentii</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr"/>
+      <c r="D1375" t="inlineStr"/>
+      <c r="E1375" t="inlineStr"/>
+      <c r="F1375" t="inlineStr"/>
+      <c r="G1375" t="inlineStr"/>
+      <c r="H1375" t="inlineStr"/>
+      <c r="I1375" t="inlineStr"/>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum Saal</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr"/>
+      <c r="D1376" t="inlineStr"/>
+      <c r="E1376" t="inlineStr"/>
+      <c r="F1376" t="inlineStr"/>
+      <c r="G1376" t="inlineStr"/>
+      <c r="H1376" t="inlineStr"/>
+      <c r="I1376" t="inlineStr"/>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Monstera Deliciosa Variegata</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr"/>
+      <c r="D1377" t="inlineStr"/>
+      <c r="E1377" t="inlineStr"/>
+      <c r="F1377" t="inlineStr"/>
+      <c r="G1377" t="inlineStr"/>
+      <c r="H1377" t="inlineStr"/>
+      <c r="I1377" t="inlineStr"/>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Pachira Aquatica</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr"/>
+      <c r="D1378" t="inlineStr"/>
+      <c r="E1378" t="inlineStr"/>
+      <c r="F1378" t="inlineStr"/>
+      <c r="G1378" t="inlineStr"/>
+      <c r="H1378" t="inlineStr"/>
+      <c r="I1378" t="inlineStr"/>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monstera Deliciosa </t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr"/>
+      <c r="D1379" t="inlineStr"/>
+      <c r="E1379" t="inlineStr"/>
+      <c r="F1379" t="inlineStr"/>
+      <c r="G1379" t="inlineStr"/>
+      <c r="H1379" t="inlineStr"/>
+      <c r="I1379" t="inlineStr"/>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>11.08.2025</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Philodendron Imperial Red</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr"/>
+      <c r="D1380" t="inlineStr"/>
+      <c r="E1380" t="inlineStr"/>
+      <c r="F1380" t="inlineStr"/>
+      <c r="G1380" t="inlineStr"/>
+      <c r="H1380" t="inlineStr"/>
+      <c r="I1380" t="inlineStr"/>
+    </row>
+    <row r="1381"/>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Calathea Medalion</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr"/>
+      <c r="D1382" t="inlineStr"/>
+      <c r="E1382" t="inlineStr"/>
+      <c r="F1382" t="inlineStr"/>
+      <c r="G1382" t="inlineStr"/>
+      <c r="H1382" t="inlineStr"/>
+      <c r="I1382" t="inlineStr"/>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr"/>
+      <c r="D1383" t="inlineStr"/>
+      <c r="E1383" t="inlineStr"/>
+      <c r="F1383" t="inlineStr"/>
+      <c r="G1383" t="inlineStr"/>
+      <c r="H1383" t="inlineStr"/>
+      <c r="I1383" t="inlineStr"/>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Philodendron Scandens Micans </t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr"/>
+      <c r="D1384" t="inlineStr"/>
+      <c r="E1384" t="inlineStr"/>
+      <c r="F1384" t="inlineStr"/>
+      <c r="G1384" t="inlineStr"/>
+      <c r="H1384" t="inlineStr"/>
+      <c r="I1384" t="inlineStr"/>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Scindapsus Treubii Moonlight</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr"/>
+      <c r="D1385" t="inlineStr"/>
+      <c r="E1385" t="inlineStr"/>
+      <c r="F1385" t="inlineStr"/>
+      <c r="G1385" t="inlineStr"/>
+      <c r="H1385" t="inlineStr"/>
+      <c r="I1385" t="inlineStr"/>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Philodendron Hedaracium Brasil</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr"/>
+      <c r="D1386" t="inlineStr"/>
+      <c r="E1386" t="inlineStr"/>
+      <c r="F1386" t="inlineStr"/>
+      <c r="G1386" t="inlineStr"/>
+      <c r="H1386" t="inlineStr"/>
+      <c r="I1386" t="inlineStr"/>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Monstera Adenossii</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr"/>
+      <c r="D1387" t="inlineStr"/>
+      <c r="E1387" t="inlineStr"/>
+      <c r="F1387" t="inlineStr"/>
+      <c r="G1387" t="inlineStr"/>
+      <c r="H1387" t="inlineStr"/>
+      <c r="I1387" t="inlineStr"/>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Ficus Elastica Abidjan</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr"/>
+      <c r="D1388" t="inlineStr"/>
+      <c r="E1388" t="inlineStr"/>
+      <c r="F1388" t="inlineStr"/>
+      <c r="G1388" t="inlineStr"/>
+      <c r="H1388" t="inlineStr"/>
+      <c r="I1388" t="inlineStr"/>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Peperomia Hope</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr"/>
+      <c r="D1389" t="inlineStr"/>
+      <c r="E1389" t="inlineStr"/>
+      <c r="F1389" t="inlineStr"/>
+      <c r="G1389" t="inlineStr"/>
+      <c r="H1389" t="inlineStr"/>
+      <c r="I1389" t="inlineStr"/>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Hoya Mathilde</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr"/>
+      <c r="D1390" t="inlineStr"/>
+      <c r="E1390" t="inlineStr"/>
+      <c r="F1390" t="inlineStr"/>
+      <c r="G1390" t="inlineStr"/>
+      <c r="H1390" t="inlineStr"/>
+      <c r="I1390" t="inlineStr"/>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Epipremnum Pinnatum Blue</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr"/>
+      <c r="D1391" t="inlineStr"/>
+      <c r="E1391" t="inlineStr"/>
+      <c r="F1391" t="inlineStr"/>
+      <c r="G1391" t="inlineStr"/>
+      <c r="H1391" t="inlineStr"/>
+      <c r="I1391" t="inlineStr"/>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Sansevieria Laurentii</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr"/>
+      <c r="D1392" t="inlineStr"/>
+      <c r="E1392" t="inlineStr"/>
+      <c r="F1392" t="inlineStr"/>
+      <c r="G1392" t="inlineStr"/>
+      <c r="H1392" t="inlineStr"/>
+      <c r="I1392" t="inlineStr"/>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Epipremnum Aureum Saal</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr"/>
+      <c r="D1393" t="inlineStr"/>
+      <c r="E1393" t="inlineStr"/>
+      <c r="F1393" t="inlineStr"/>
+      <c r="G1393" t="inlineStr"/>
+      <c r="H1393" t="inlineStr"/>
+      <c r="I1393" t="inlineStr"/>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Monstera Deliciosa Variegata</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr"/>
+      <c r="D1394" t="inlineStr"/>
+      <c r="E1394" t="inlineStr"/>
+      <c r="F1394" t="inlineStr"/>
+      <c r="G1394" t="inlineStr"/>
+      <c r="H1394" t="inlineStr"/>
+      <c r="I1394" t="inlineStr"/>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Pachira Aquatica</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr"/>
+      <c r="D1395" t="inlineStr"/>
+      <c r="E1395" t="inlineStr"/>
+      <c r="F1395" t="inlineStr"/>
+      <c r="G1395" t="inlineStr"/>
+      <c r="H1395" t="inlineStr"/>
+      <c r="I1395" t="inlineStr"/>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monstera Deliciosa </t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr"/>
+      <c r="D1396" t="inlineStr"/>
+      <c r="E1396" t="inlineStr"/>
+      <c r="F1396" t="inlineStr"/>
+      <c r="G1396" t="inlineStr"/>
+      <c r="H1396" t="inlineStr"/>
+      <c r="I1396" t="inlineStr"/>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>12.08.2025</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Philodendron Imperial Red</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr"/>
+      <c r="D1397" t="inlineStr"/>
+      <c r="E1397" t="inlineStr"/>
+      <c r="F1397" t="inlineStr"/>
+      <c r="G1397" t="inlineStr"/>
+      <c r="H1397" t="inlineStr"/>
+      <c r="I1397" t="inlineStr"/>
+    </row>
+    <row r="1398"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>